<commit_message>
fixing capacity constraint rule, pipeline capex rule, and strategic test
</commit_message>
<xml_diff>
--- a/pareto/case_studies/input_data_generic_strategic_case_study_LAYFLAT_FULL.xlsx
+++ b/pareto/case_studies/input_data_generic_strategic_case_study_LAYFLAT_FULL.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://d.docs.live.net/54325818ffabb65a/Documents/KeyLogic/PARETO/project-pareto/pareto/case_studies/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="150" documentId="13_ncr:1_{10D5EE35-54BB-4542-BD99-B88C1035F5E1}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{78A6A069-9FC1-4912-B11D-598E787244A3}"/>
+  <xr:revisionPtr revIDLastSave="152" documentId="13_ncr:1_{10D5EE35-54BB-4542-BD99-B88C1035F5E1}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{7986D10D-DF25-4645-93C9-59388EA3F1E2}"/>
   <bookViews>
-    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" tabRatio="834" firstSheet="54" activeTab="60" xr2:uid="{FB8C51AB-905F-4544-9E4B-1F4384FA855C}"/>
+    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" tabRatio="834" firstSheet="27" activeTab="29" xr2:uid="{FB8C51AB-905F-4544-9E4B-1F4384FA855C}"/>
   </bookViews>
   <sheets>
     <sheet name="Overview" sheetId="33" r:id="rId1"/>
@@ -7377,8 +7377,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{44AE275C-BC38-44C0-8EFB-EA0A3ABCF1EE}">
   <dimension ref="A1:F17"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="A2" sqref="A2"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="I14" sqref="I14"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9.33203125" defaultRowHeight="15.6" x14ac:dyDescent="0.3"/>
@@ -15392,7 +15392,7 @@
   <dimension ref="A1:F20"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="M24" sqref="M24"/>
+      <selection activeCell="A3" sqref="A3:F5"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9.33203125" defaultRowHeight="15.6" x14ac:dyDescent="0.3"/>
@@ -24984,7 +24984,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{92EDDE38-2D71-4494-ABC1-8D5269A138D9}">
   <dimension ref="A1:B4"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="D10" sqref="D10"/>
     </sheetView>
   </sheetViews>

</xml_diff>

<commit_message>
Update to case studies to accomodate for water quality calculations.
</commit_message>
<xml_diff>
--- a/pareto/case_studies/input_data_generic_strategic_case_study_LAYFLAT_FULL.xlsx
+++ b/pareto/case_studies/input_data_generic_strategic_case_study_LAYFLAT_FULL.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="24527"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="24701"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\GitHub\PARETO - dev\project-pareto\pareto\case_studies\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{C7BA1116-7D67-4951-AAC0-08F92A26DE3F}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{B208342E-2DC7-47CB-B788-4D2AD2C9401C}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="17640" tabRatio="834" firstSheet="53" activeTab="61" xr2:uid="{FB8C51AB-905F-4544-9E4B-1F4384FA855C}"/>
+    <workbookView xWindow="28680" yWindow="-120" windowWidth="29040" windowHeight="17640" tabRatio="834" firstSheet="55" activeTab="63" xr2:uid="{FB8C51AB-905F-4544-9E4B-1F4384FA855C}"/>
   </bookViews>
   <sheets>
     <sheet name="Overview" sheetId="33" r:id="rId1"/>
@@ -75,6 +75,8 @@
     <sheet name="PipelineExpansionDistance" sheetId="94" r:id="rId60"/>
     <sheet name="Hydraulics" sheetId="93" r:id="rId61"/>
     <sheet name="Economics" sheetId="95" r:id="rId62"/>
+    <sheet name="PadWaterQuality" sheetId="96" r:id="rId63"/>
+    <sheet name="StorageInitialWaterQuality" sheetId="97" r:id="rId64"/>
   </sheets>
   <definedNames>
     <definedName name="_xlnm._FilterDatabase" localSheetId="59" hidden="1">#REF!</definedName>
@@ -99,7 +101,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1110" uniqueCount="273">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1136" uniqueCount="277">
   <si>
     <t>List of all Production Pad Identifiers [-]</t>
   </si>
@@ -918,16 +920,29 @@
   </si>
   <si>
     <t>CAPEX_lifetime</t>
+  </si>
+  <si>
+    <t>Water Quality at Production Pads (mg/L)</t>
+  </si>
+  <si>
+    <t>Pads</t>
+  </si>
+  <si>
+    <t>TDS</t>
+  </si>
+  <si>
+    <t>Initial Water Quality at Storage (mg/L)</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <numFmts count="1">
+  <numFmts count="2">
+    <numFmt numFmtId="43" formatCode="_(* #,##0.00_);_(* \(#,##0.00\);_(* &quot;-&quot;??_);_(@_)"/>
     <numFmt numFmtId="164" formatCode="#,##0.0"/>
   </numFmts>
-  <fonts count="8" x14ac:knownFonts="1">
+  <fonts count="9" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -986,6 +1001,13 @@
       <family val="2"/>
       <scheme val="minor"/>
     </font>
+    <font>
+      <sz val="11"/>
+      <color theme="1"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
   </fonts>
   <fills count="4">
     <fill>
@@ -1007,7 +1029,7 @@
       </patternFill>
     </fill>
   </fills>
-  <borders count="16">
+  <borders count="22">
     <border>
       <left/>
       <right/>
@@ -1184,12 +1206,95 @@
       </bottom>
       <diagonal/>
     </border>
+    <border>
+      <left style="thin">
+        <color indexed="64"/>
+      </left>
+      <right style="medium">
+        <color indexed="64"/>
+      </right>
+      <top style="medium">
+        <color indexed="64"/>
+      </top>
+      <bottom style="thin">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="medium">
+        <color indexed="64"/>
+      </left>
+      <right style="thin">
+        <color indexed="64"/>
+      </right>
+      <top style="thin">
+        <color indexed="64"/>
+      </top>
+      <bottom/>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color indexed="64"/>
+      </left>
+      <right style="medium">
+        <color indexed="64"/>
+      </right>
+      <top/>
+      <bottom/>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color indexed="64"/>
+      </left>
+      <right style="medium">
+        <color indexed="64"/>
+      </right>
+      <top/>
+      <bottom style="medium">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="medium">
+        <color indexed="64"/>
+      </left>
+      <right style="thin">
+        <color indexed="64"/>
+      </right>
+      <top style="thin">
+        <color indexed="64"/>
+      </top>
+      <bottom style="medium">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color indexed="64"/>
+      </left>
+      <right style="medium">
+        <color indexed="64"/>
+      </right>
+      <top style="thin">
+        <color indexed="64"/>
+      </top>
+      <bottom style="medium">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
   </borders>
-  <cellStyleXfs count="2">
+  <cellStyleXfs count="3">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="6" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="43" fontId="8" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="56">
+  <cellXfs count="63">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1"/>
@@ -1308,8 +1413,30 @@
     <xf numFmtId="4" fontId="1" fillId="3" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
+    <xf numFmtId="0" fontId="3" fillId="3" borderId="16" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="3" borderId="17" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="43" fontId="1" fillId="3" borderId="14" xfId="2" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="43" fontId="1" fillId="3" borderId="18" xfId="2" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="43" fontId="1" fillId="3" borderId="19" xfId="2" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="3" borderId="20" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="43" fontId="1" fillId="3" borderId="21" xfId="2" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
   </cellXfs>
-  <cellStyles count="2">
+  <cellStyles count="3">
+    <cellStyle name="Comma" xfId="2" builtinId="3"/>
     <cellStyle name="Hyperlink" xfId="1" builtinId="8"/>
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
@@ -25044,7 +25171,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{ED2F8796-71C2-44EA-9373-5A0165D7B559}">
   <dimension ref="A1:B4"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="F10" sqref="F10"/>
     </sheetView>
   </sheetViews>
@@ -25080,6 +25207,229 @@
       </c>
       <c r="B4" s="40">
         <v>20</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet63.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{B32CB9AD-BE1A-4B42-ACBF-244C18AEB0E2}">
+  <dimension ref="A1:B21"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="E23" sqref="E23"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <cols>
+    <col min="2" max="2" width="12.7109375" bestFit="1" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:2" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A1" t="s">
+        <v>273</v>
+      </c>
+    </row>
+    <row r="2" spans="1:2" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="A2" s="7" t="s">
+        <v>274</v>
+      </c>
+      <c r="B2" s="56" t="s">
+        <v>275</v>
+      </c>
+    </row>
+    <row r="3" spans="1:2" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="A3" s="57" t="s">
+        <v>130</v>
+      </c>
+      <c r="B3" s="58">
+        <v>142277</v>
+      </c>
+    </row>
+    <row r="4" spans="1:2" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="A4" s="29" t="s">
+        <v>3</v>
+      </c>
+      <c r="B4" s="59">
+        <v>140998</v>
+      </c>
+    </row>
+    <row r="5" spans="1:2" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="A5" s="29" t="s">
+        <v>4</v>
+      </c>
+      <c r="B5" s="59">
+        <v>172490.2</v>
+      </c>
+    </row>
+    <row r="6" spans="1:2" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="A6" s="29" t="s">
+        <v>122</v>
+      </c>
+      <c r="B6" s="59">
+        <v>257547</v>
+      </c>
+    </row>
+    <row r="7" spans="1:2" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="A7" s="29" t="s">
+        <v>123</v>
+      </c>
+      <c r="B7" s="59">
+        <v>241833.8</v>
+      </c>
+    </row>
+    <row r="8" spans="1:2" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="A8" s="29" t="s">
+        <v>124</v>
+      </c>
+      <c r="B8" s="59">
+        <v>188503.7</v>
+      </c>
+    </row>
+    <row r="9" spans="1:2" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="A9" s="29" t="s">
+        <v>125</v>
+      </c>
+      <c r="B9" s="59">
+        <v>146716</v>
+      </c>
+    </row>
+    <row r="10" spans="1:2" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="A10" s="29" t="s">
+        <v>126</v>
+      </c>
+      <c r="B10" s="59">
+        <v>216563</v>
+      </c>
+    </row>
+    <row r="11" spans="1:2" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="A11" s="29" t="s">
+        <v>127</v>
+      </c>
+      <c r="B11" s="59">
+        <v>150626</v>
+      </c>
+    </row>
+    <row r="12" spans="1:2" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="A12" s="29" t="s">
+        <v>128</v>
+      </c>
+      <c r="B12" s="59">
+        <v>247061</v>
+      </c>
+    </row>
+    <row r="13" spans="1:2" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="A13" s="29" t="s">
+        <v>129</v>
+      </c>
+      <c r="B13" s="59">
+        <v>180968</v>
+      </c>
+    </row>
+    <row r="14" spans="1:2" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="A14" s="29" t="s">
+        <v>131</v>
+      </c>
+      <c r="B14" s="59">
+        <v>195584</v>
+      </c>
+    </row>
+    <row r="15" spans="1:2" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="A15" s="29" t="s">
+        <v>132</v>
+      </c>
+      <c r="B15" s="59">
+        <v>148655</v>
+      </c>
+    </row>
+    <row r="16" spans="1:2" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="A16" s="29" t="s">
+        <v>133</v>
+      </c>
+      <c r="B16" s="59">
+        <v>185369</v>
+      </c>
+    </row>
+    <row r="17" spans="1:2" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="A17" s="29" t="s">
+        <v>134</v>
+      </c>
+      <c r="B17" s="59">
+        <v>222724</v>
+      </c>
+    </row>
+    <row r="18" spans="1:2" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="A18" s="29" t="s">
+        <v>5</v>
+      </c>
+      <c r="B18" s="59">
+        <v>165376</v>
+      </c>
+    </row>
+    <row r="19" spans="1:2" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="A19" s="29" t="s">
+        <v>135</v>
+      </c>
+      <c r="B19" s="59">
+        <v>240977</v>
+      </c>
+    </row>
+    <row r="20" spans="1:2" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="A20" s="29" t="s">
+        <v>136</v>
+      </c>
+      <c r="B20" s="59">
+        <v>192794</v>
+      </c>
+    </row>
+    <row r="21" spans="1:2" ht="16.5" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A21" s="30" t="s">
+        <v>137</v>
+      </c>
+      <c r="B21" s="60">
+        <v>216769</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup orientation="portrait" r:id="rId1"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet64.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{105E52B2-E3FA-4F38-8D25-CE95F27EC564}">
+  <dimension ref="A1:B3"/>
+  <sheetViews>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="D13" activeCellId="1" sqref="J12 D13"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <cols>
+    <col min="2" max="2" width="12.7109375" bestFit="1" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:2" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A1" t="s">
+        <v>276</v>
+      </c>
+    </row>
+    <row r="2" spans="1:2" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="A2" s="7" t="s">
+        <v>274</v>
+      </c>
+      <c r="B2" s="56" t="s">
+        <v>275</v>
+      </c>
+    </row>
+    <row r="3" spans="1:2" ht="16.5" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A3" s="61" t="s">
+        <v>81</v>
+      </c>
+      <c r="B3" s="62">
+        <v>150000</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Update treatment efficiency to be per water quality component
</commit_message>
<xml_diff>
--- a/pareto/case_studies/input_data_generic_strategic_case_study_LAYFLAT_FULL.xlsx
+++ b/pareto/case_studies/input_data_generic_strategic_case_study_LAYFLAT_FULL.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\GitHub\PARETO - dev\project-pareto\pareto\case_studies\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{B208342E-2DC7-47CB-B788-4D2AD2C9401C}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{1B77B60F-605C-46C1-AC2F-C7986D780800}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="28680" yWindow="-120" windowWidth="29040" windowHeight="17640" tabRatio="834" firstSheet="55" activeTab="63" xr2:uid="{FB8C51AB-905F-4544-9E4B-1F4384FA855C}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="17640" tabRatio="834" firstSheet="55" activeTab="62" xr2:uid="{FB8C51AB-905F-4544-9E4B-1F4384FA855C}"/>
   </bookViews>
   <sheets>
     <sheet name="Overview" sheetId="33" r:id="rId1"/>
@@ -101,7 +101,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1136" uniqueCount="277">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1136" uniqueCount="278">
   <si>
     <t>List of all Production Pad Identifiers [-]</t>
   </si>
@@ -932,6 +932,9 @@
   </si>
   <si>
     <t>Initial Water Quality at Storage (mg/L)</t>
+  </si>
+  <si>
+    <t>PADS</t>
   </si>
 </sst>
 </file>
@@ -16833,7 +16836,7 @@
   <dimension ref="A1:B4"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="A2" sqref="A2"/>
+      <selection activeCell="B3" sqref="B3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9.28515625" defaultRowHeight="15.75" x14ac:dyDescent="0.25"/>
@@ -16851,7 +16854,7 @@
         <v>255</v>
       </c>
       <c r="B2" s="28" t="s">
-        <v>250</v>
+        <v>275</v>
       </c>
     </row>
     <row r="3" spans="1:2" s="9" customFormat="1" x14ac:dyDescent="0.25">
@@ -25218,8 +25221,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{B32CB9AD-BE1A-4B42-ACBF-244C18AEB0E2}">
   <dimension ref="A1:B21"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="E23" sqref="E23"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="C2" sqref="C2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -25234,7 +25237,7 @@
     </row>
     <row r="2" spans="1:2" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A2" s="7" t="s">
-        <v>274</v>
+        <v>277</v>
       </c>
       <c r="B2" s="56" t="s">
         <v>275</v>
@@ -25402,7 +25405,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{105E52B2-E3FA-4F38-8D25-CE95F27EC564}">
   <dimension ref="A1:B3"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="D13" activeCellId="1" sqref="J12 D13"/>
     </sheetView>
   </sheetViews>

</xml_diff>

<commit_message>
adjust input distances with karen's feedback
</commit_message>
<xml_diff>
--- a/pareto/case_studies/input_data_generic_strategic_case_study_LAYFLAT_FULL.xlsx
+++ b/pareto/case_studies/input_data_generic_strategic_case_study_LAYFLAT_FULL.xlsx
@@ -1,14 +1,14 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="24729"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="24827"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\melodys\Documents\1. Projects\PARETO - Department of Energy\Code Updates\GIT Tracked Folder\project-pareto\pareto\case_studies\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{6900FB7E-A4FB-4990-8DB6-20A229D53679}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{B757F140-DC91-4A67-9410-6B01CD0E1014}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="16680" yWindow="-16320" windowWidth="29040" windowHeight="15840" tabRatio="834" firstSheet="56" activeTab="59" xr2:uid="{FB8C51AB-905F-4544-9E4B-1F4384FA855C}"/>
   </bookViews>
@@ -17386,8 +17386,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{9547EF3E-C271-4F2C-A3E7-66F3B3003AB1}">
   <dimension ref="A1:AP61"/>
   <sheetViews>
-    <sheetView showZeros="0" tabSelected="1" zoomScale="55" zoomScaleNormal="55" workbookViewId="0">
-      <selection activeCell="P20" sqref="P20"/>
+    <sheetView showZeros="0" tabSelected="1" topLeftCell="A13" zoomScale="55" zoomScaleNormal="55" workbookViewId="0">
+      <selection activeCell="F52" sqref="F52"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -17532,7 +17532,7 @@
         <v>130</v>
       </c>
       <c r="B3" s="46">
-        <v>5.7039999999999997</v>
+        <v>1.0969230769230769</v>
       </c>
       <c r="C3" s="46">
         <v>0</v>
@@ -17672,7 +17672,7 @@
         <v>0</v>
       </c>
       <c r="F4" s="46">
-        <v>6.7388000000000003</v>
+        <v>1.295923076923077</v>
       </c>
       <c r="G4" s="46">
         <v>0</v>
@@ -17803,7 +17803,7 @@
         <v>0</v>
       </c>
       <c r="G5" s="46">
-        <v>5.0251999999999999</v>
+        <v>0.9663846153846154</v>
       </c>
       <c r="H5" s="46">
         <v>0</v>
@@ -17946,7 +17946,7 @@
         <v>0</v>
       </c>
       <c r="L6" s="46">
-        <v>10.0296</v>
+        <v>1.9287692307692308</v>
       </c>
       <c r="M6" s="46">
         <v>0</v>
@@ -18071,13 +18071,13 @@
         <v>0</v>
       </c>
       <c r="K7" s="46">
-        <v>23.6739469471283</v>
+        <v>4.5526821052169808</v>
       </c>
       <c r="L7" s="46">
         <v>0</v>
       </c>
       <c r="M7" s="46">
-        <v>5.9484000000000004</v>
+        <v>1.143923076923077</v>
       </c>
       <c r="N7" s="46">
         <v>0</v>
@@ -18217,7 +18217,7 @@
         <v>0</v>
       </c>
       <c r="Q8" s="46">
-        <v>9.9032</v>
+        <v>1.9044615384615386</v>
       </c>
       <c r="R8" s="46">
         <v>0</v>
@@ -18342,7 +18342,7 @@
         <v>0</v>
       </c>
       <c r="P9" s="46">
-        <v>12.288903996290491</v>
+        <v>2.3632507685174025</v>
       </c>
       <c r="Q9" s="46">
         <v>0</v>
@@ -18479,7 +18479,7 @@
         <v>0</v>
       </c>
       <c r="S10" s="46">
-        <v>3.9807999999999999</v>
+        <v>0.7655384615384615</v>
       </c>
       <c r="T10" s="46">
         <v>0</v>
@@ -18616,7 +18616,7 @@
         <v>0</v>
       </c>
       <c r="V11" s="46">
-        <v>9.6988000000000003</v>
+        <v>1.8651538461538462</v>
       </c>
       <c r="W11" s="46">
         <v>0</v>
@@ -18738,7 +18738,7 @@
         <v>0</v>
       </c>
       <c r="T12" s="46">
-        <v>9.6148000000000007</v>
+        <v>1.849</v>
       </c>
       <c r="U12" s="46">
         <v>0</v>
@@ -18884,7 +18884,7 @@
         <v>0</v>
       </c>
       <c r="Z13" s="46">
-        <v>15.318800000000001</v>
+        <v>2.9459230769230773</v>
       </c>
       <c r="AA13" s="46">
         <v>0</v>
@@ -19018,7 +19018,7 @@
         <v>0</v>
       </c>
       <c r="AB14" s="46">
-        <v>3.4019999999999997</v>
+        <v>0.65423076923076917</v>
       </c>
       <c r="AC14" s="46">
         <v>0</v>
@@ -19146,7 +19146,7 @@
         <v>0</v>
       </c>
       <c r="AB15" s="46">
-        <v>3.5811999999999999</v>
+        <v>0.68869230769230771</v>
       </c>
       <c r="AC15" s="46">
         <v>0</v>
@@ -19274,7 +19274,7 @@
         <v>0</v>
       </c>
       <c r="AB16" s="46">
-        <v>4.97</v>
+        <v>0.95576923076923082</v>
       </c>
       <c r="AC16" s="46">
         <v>0</v>
@@ -19393,7 +19393,7 @@
         <v>0</v>
       </c>
       <c r="Y17" s="11">
-        <v>9.6996000000000002</v>
+        <v>1.8653076923076923</v>
       </c>
       <c r="Z17" s="11">
         <v>0</v>
@@ -19458,7 +19458,7 @@
         <v>0</v>
       </c>
       <c r="D18" s="46">
-        <v>4.484</v>
+        <v>0.86230769230769222</v>
       </c>
       <c r="E18" s="46">
         <v>0</v>
@@ -19554,7 +19554,7 @@
         <v>0</v>
       </c>
       <c r="AJ18" s="46">
-        <v>28.063880000000005</v>
+        <v>5.3969000000000005</v>
       </c>
       <c r="AK18" s="32">
         <v>0</v>
@@ -19607,7 +19607,7 @@
         <v>0</v>
       </c>
       <c r="K19" s="46">
-        <v>8.5172000000000008</v>
+        <v>1.637923076923077</v>
       </c>
       <c r="L19" s="46">
         <v>0</v>
@@ -19682,7 +19682,7 @@
         <v>0</v>
       </c>
       <c r="AJ19" s="46">
-        <v>24.708839999999999</v>
+        <v>4.7516999999999996</v>
       </c>
       <c r="AK19" s="32">
         <v>0</v>
@@ -19756,7 +19756,7 @@
         <v>0</v>
       </c>
       <c r="R20" s="46">
-        <v>8.2788000000000004</v>
+        <v>1.5920769230769232</v>
       </c>
       <c r="S20" s="46">
         <v>0</v>
@@ -19813,7 +19813,7 @@
         <v>0</v>
       </c>
       <c r="AK20" s="32">
-        <v>37.559080000000002</v>
+        <v>7.222900000000001</v>
       </c>
       <c r="AL20" s="35">
         <v>0</v>
@@ -19902,7 +19902,7 @@
         <v>0</v>
       </c>
       <c r="X21" s="11">
-        <v>8.8379999999999992</v>
+        <v>1.6996153846153845</v>
       </c>
       <c r="Y21" s="11">
         <v>0</v>
@@ -19941,7 +19941,7 @@
         <v>0</v>
       </c>
       <c r="AK21" s="12">
-        <v>37.183640000000004</v>
+        <v>7.1507000000000005</v>
       </c>
       <c r="AL21" s="36">
         <v>0</v>
@@ -19967,7 +19967,7 @@
         <v>0</v>
       </c>
       <c r="C22" s="55">
-        <v>16.300963910394145</v>
+        <v>3.1348007519988741</v>
       </c>
       <c r="D22" s="46">
         <v>0</v>
@@ -20051,7 +20051,7 @@
         <v>0</v>
       </c>
       <c r="AE22" s="55">
-        <v>16.686799999999998</v>
+        <v>3.2089999999999996</v>
       </c>
       <c r="AF22" s="46">
         <v>0</v>
@@ -20092,19 +20092,19 @@
         <v>83</v>
       </c>
       <c r="B23" s="55">
-        <v>16.300963910394145</v>
+        <v>3.1348007519988741</v>
       </c>
       <c r="C23" s="55">
         <v>0</v>
       </c>
       <c r="D23" s="46">
-        <v>3.3188</v>
+        <v>0.63823076923076927</v>
       </c>
       <c r="E23" s="46">
         <v>0</v>
       </c>
       <c r="F23" s="46">
-        <v>7.2567999999999993</v>
+        <v>1.3955384615384614</v>
       </c>
       <c r="G23" s="46">
         <v>0</v>
@@ -20223,13 +20223,13 @@
         <v>0</v>
       </c>
       <c r="C24" s="46">
-        <v>3.3188</v>
+        <v>0.63823076923076927</v>
       </c>
       <c r="D24" s="46">
         <v>0</v>
       </c>
       <c r="E24" s="46">
-        <v>3.3251999999999997</v>
+        <v>0.63946153846153841</v>
       </c>
       <c r="F24" s="46">
         <v>0</v>
@@ -20331,7 +20331,7 @@
         <v>0</v>
       </c>
       <c r="AM24" s="46">
-        <v>4.484</v>
+        <v>0.86230769230769222</v>
       </c>
       <c r="AN24" s="46">
         <v>0</v>
@@ -20354,7 +20354,7 @@
         <v>0</v>
       </c>
       <c r="D25" s="46">
-        <v>3.3251999999999997</v>
+        <v>0.63946153846153841</v>
       </c>
       <c r="E25" s="46">
         <v>0</v>
@@ -20363,7 +20363,7 @@
         <v>0</v>
       </c>
       <c r="G25" s="46">
-        <v>5.0132000000000003</v>
+        <v>0.96407692307692316</v>
       </c>
       <c r="H25" s="46">
         <v>0</v>
@@ -20438,7 +20438,7 @@
         <v>0</v>
       </c>
       <c r="AF25" s="46">
-        <v>5.2652000000000001</v>
+        <v>1.0125384615384616</v>
       </c>
       <c r="AG25" s="46">
         <v>0</v>
@@ -20479,7 +20479,7 @@
         <v>0</v>
       </c>
       <c r="C26" s="55">
-        <v>7.2567999999999993</v>
+        <v>1.3955384615384614</v>
       </c>
       <c r="D26" s="46">
         <v>0</v>
@@ -20497,7 +20497,7 @@
         <v>0</v>
       </c>
       <c r="I26" s="46">
-        <v>5.7724000000000002</v>
+        <v>1.1100769230769232</v>
       </c>
       <c r="J26" s="46">
         <v>0</v>
@@ -20613,7 +20613,7 @@
         <v>0</v>
       </c>
       <c r="E27" s="46">
-        <v>5.0132000000000003</v>
+        <v>0.96407692307692316</v>
       </c>
       <c r="F27" s="46">
         <v>0</v>
@@ -20622,7 +20622,7 @@
         <v>0</v>
       </c>
       <c r="H27" s="46">
-        <v>4.6120000000000001</v>
+        <v>0.88692307692307693</v>
       </c>
       <c r="I27" s="46">
         <v>0</v>
@@ -20747,16 +20747,16 @@
         <v>0</v>
       </c>
       <c r="G28" s="46">
-        <v>4.6120000000000001</v>
+        <v>0.88692307692307693</v>
       </c>
       <c r="H28" s="46">
         <v>0</v>
       </c>
       <c r="I28" s="46">
-        <v>2.4312</v>
+        <v>0.46753846153846157</v>
       </c>
       <c r="J28" s="46">
-        <v>9.7796000000000003</v>
+        <v>1.8806923076923077</v>
       </c>
       <c r="K28" s="46">
         <v>0</v>
@@ -20872,13 +20872,13 @@
         <v>0</v>
       </c>
       <c r="F29" s="46">
-        <v>5.7724000000000002</v>
+        <v>1.1100769230769232</v>
       </c>
       <c r="G29" s="46">
         <v>0</v>
       </c>
       <c r="H29" s="46">
-        <v>2.4312</v>
+        <v>0.46753846153846157</v>
       </c>
       <c r="I29" s="46">
         <v>0</v>
@@ -20962,7 +20962,7 @@
         <v>0</v>
       </c>
       <c r="AJ29" s="46">
-        <v>7.0396000000000001</v>
+        <v>1.3537692307692308</v>
       </c>
       <c r="AK29" s="32">
         <v>0</v>
@@ -21006,7 +21006,7 @@
         <v>0</v>
       </c>
       <c r="H30" s="46">
-        <v>9.7796000000000003</v>
+        <v>1.8806923076923077</v>
       </c>
       <c r="I30" s="46">
         <v>0</v>
@@ -21015,10 +21015,10 @@
         <v>0</v>
       </c>
       <c r="K30" s="46">
-        <v>3.9751999999999996</v>
+        <v>0.76446153846153841</v>
       </c>
       <c r="L30" s="46">
-        <v>15.5404</v>
+        <v>2.9885384615384614</v>
       </c>
       <c r="M30" s="46">
         <v>0</v>
@@ -21140,7 +21140,7 @@
         <v>0</v>
       </c>
       <c r="J31" s="46">
-        <v>3.9751999999999996</v>
+        <v>0.76446153846153841</v>
       </c>
       <c r="K31" s="46">
         <v>0</v>
@@ -21149,7 +21149,7 @@
         <v>0</v>
       </c>
       <c r="M31" s="46">
-        <v>29.622346947128303</v>
+        <v>5.6966051821400585</v>
       </c>
       <c r="N31" s="46">
         <v>0</v>
@@ -21230,7 +21230,7 @@
         <v>0</v>
       </c>
       <c r="AN31" s="46">
-        <v>8.5172000000000008</v>
+        <v>1.637923076923077</v>
       </c>
       <c r="AO31" s="46">
         <v>0</v>
@@ -21268,7 +21268,7 @@
         <v>0</v>
       </c>
       <c r="J32" s="46">
-        <v>15.5404</v>
+        <v>2.9885384615384614</v>
       </c>
       <c r="K32" s="46">
         <v>0</v>
@@ -21280,7 +21280,7 @@
         <v>0</v>
       </c>
       <c r="N32" s="46">
-        <v>10.572000000000001</v>
+        <v>2.0330769230769232</v>
       </c>
       <c r="O32" s="46">
         <v>0</v>
@@ -21399,7 +21399,7 @@
         <v>0</v>
       </c>
       <c r="K33" s="46">
-        <v>29.622346947128303</v>
+        <v>5.6966051821400585</v>
       </c>
       <c r="L33" s="46">
         <v>0</v>
@@ -21411,7 +21411,7 @@
         <v>0</v>
       </c>
       <c r="O33" s="46">
-        <v>19.539442440750435</v>
+        <v>3.757585084759699</v>
       </c>
       <c r="P33" s="46">
         <v>0</v>
@@ -21480,7 +21480,7 @@
         <v>0</v>
       </c>
       <c r="AL33" s="32">
-        <v>4.34</v>
+        <v>0.83461538461538465</v>
       </c>
       <c r="AM33" s="46">
         <v>0</v>
@@ -21530,7 +21530,7 @@
         <v>0</v>
       </c>
       <c r="L34" s="46">
-        <v>10.572000000000001</v>
+        <v>2.0330769230769232</v>
       </c>
       <c r="M34" s="46">
         <v>0</v>
@@ -21539,7 +21539,7 @@
         <v>0</v>
       </c>
       <c r="O34" s="46">
-        <v>12.435062680670844</v>
+        <v>2.391358207821316</v>
       </c>
       <c r="P34" s="46">
         <v>0</v>
@@ -21593,7 +21593,7 @@
         <v>0</v>
       </c>
       <c r="AG34" s="46">
-        <v>12.073599999999999</v>
+        <v>2.3218461538461534</v>
       </c>
       <c r="AH34" s="46">
         <v>0</v>
@@ -21661,10 +21661,10 @@
         <v>0</v>
       </c>
       <c r="M35" s="46">
-        <v>19.539442440750435</v>
+        <v>3.757585084759699</v>
       </c>
       <c r="N35" s="46">
-        <v>12.435062680670844</v>
+        <v>2.391358207821316</v>
       </c>
       <c r="O35" s="46">
         <v>0</v>
@@ -21712,7 +21712,7 @@
         <v>0</v>
       </c>
       <c r="AD35" s="32">
-        <v>5.5836000000000006</v>
+        <v>1.0737692307692308</v>
       </c>
       <c r="AE35" s="46">
         <v>0</v>
@@ -21801,7 +21801,7 @@
         <v>0</v>
       </c>
       <c r="Q36" s="46">
-        <v>5.4215999999999998</v>
+        <v>1.0426153846153845</v>
       </c>
       <c r="R36" s="46">
         <v>0</v>
@@ -21840,7 +21840,7 @@
         <v>0</v>
       </c>
       <c r="AD36" s="32">
-        <v>2.8575999999999997</v>
+        <v>0.54953846153846153</v>
       </c>
       <c r="AE36" s="46">
         <v>0</v>
@@ -21926,13 +21926,13 @@
         <v>0</v>
       </c>
       <c r="P37" s="46">
-        <v>5.4215999999999998</v>
+        <v>1.0426153846153845</v>
       </c>
       <c r="Q37" s="46">
         <v>0</v>
       </c>
       <c r="R37" s="46">
-        <v>12.8013468273532</v>
+        <v>2.4617974667986924</v>
       </c>
       <c r="S37" s="46">
         <v>0</v>
@@ -22057,7 +22057,7 @@
         <v>0</v>
       </c>
       <c r="Q38" s="46">
-        <v>12.8013468273532</v>
+        <v>2.4617974667986924</v>
       </c>
       <c r="R38" s="46">
         <v>0</v>
@@ -22108,7 +22108,7 @@
         <v>0</v>
       </c>
       <c r="AH38" s="46">
-        <v>25.943965577156415</v>
+        <v>4.9892241494531566</v>
       </c>
       <c r="AI38" s="32">
         <v>0</v>
@@ -22129,7 +22129,7 @@
         <v>0</v>
       </c>
       <c r="AO38" s="46">
-        <v>8.2788000000000004</v>
+        <v>1.5920769230769232</v>
       </c>
       <c r="AP38" s="32">
         <v>0</v>
@@ -22194,7 +22194,7 @@
         <v>0</v>
       </c>
       <c r="T39" s="46">
-        <v>3.6275999999999997</v>
+        <v>0.69761538461538464</v>
       </c>
       <c r="U39" s="46">
         <v>0</v>
@@ -22236,7 +22236,7 @@
         <v>0</v>
       </c>
       <c r="AH39" s="46">
-        <v>13.675999999999998</v>
+        <v>2.63</v>
       </c>
       <c r="AI39" s="32">
         <v>0</v>
@@ -22319,7 +22319,7 @@
         <v>0</v>
       </c>
       <c r="S40" s="46">
-        <v>3.6275999999999997</v>
+        <v>0.69761538461538464</v>
       </c>
       <c r="T40" s="46">
         <v>0</v>
@@ -22331,7 +22331,7 @@
         <v>0</v>
       </c>
       <c r="W40" s="46">
-        <v>21.991199999999999</v>
+        <v>4.2290769230769225</v>
       </c>
       <c r="X40" s="46">
         <v>0</v>
@@ -22456,7 +22456,7 @@
         <v>0</v>
       </c>
       <c r="V41" s="46">
-        <v>2.9739999999999998</v>
+        <v>0.57192307692307687</v>
       </c>
       <c r="W41" s="46">
         <v>0</v>
@@ -22480,7 +22480,7 @@
         <v>0</v>
       </c>
       <c r="AD41" s="32">
-        <v>3.8188</v>
+        <v>0.73438461538461541</v>
       </c>
       <c r="AE41" s="46">
         <v>0</v>
@@ -22501,7 +22501,7 @@
         <v>0</v>
       </c>
       <c r="AK41" s="32">
-        <v>9.0667999999999989</v>
+        <v>1.7436153846153843</v>
       </c>
       <c r="AL41" s="32">
         <v>0</v>
@@ -22581,13 +22581,13 @@
         <v>0</v>
       </c>
       <c r="U42" s="46">
-        <v>2.9739999999999998</v>
+        <v>0.57192307692307687</v>
       </c>
       <c r="V42" s="46">
         <v>0</v>
       </c>
       <c r="W42" s="46">
-        <v>2.9560000000000004</v>
+        <v>0.56846153846153846</v>
       </c>
       <c r="X42" s="46">
         <v>0</v>
@@ -22706,19 +22706,19 @@
         <v>0</v>
       </c>
       <c r="T43" s="46">
-        <v>21.991199999999999</v>
+        <v>4.2290769230769225</v>
       </c>
       <c r="U43" s="46">
         <v>0</v>
       </c>
       <c r="V43" s="46">
-        <v>2.9560000000000004</v>
+        <v>0.56846153846153846</v>
       </c>
       <c r="W43" s="46">
         <v>0</v>
       </c>
       <c r="X43" s="46">
-        <v>11.505599999999999</v>
+        <v>2.2126153846153844</v>
       </c>
       <c r="Y43" s="46">
         <v>0</v>
@@ -22745,7 +22745,7 @@
         <v>0</v>
       </c>
       <c r="AG43" s="46">
-        <v>15.523199999999999</v>
+        <v>2.9852307692307689</v>
       </c>
       <c r="AH43" s="46">
         <v>0</v>
@@ -22843,13 +22843,13 @@
         <v>0</v>
       </c>
       <c r="W44" s="46">
-        <v>11.505599999999999</v>
+        <v>2.2126153846153844</v>
       </c>
       <c r="X44" s="46">
         <v>0</v>
       </c>
       <c r="Y44" s="46">
-        <v>11.4428</v>
+        <v>2.2005384615384616</v>
       </c>
       <c r="Z44" s="46">
         <v>0</v>
@@ -22900,7 +22900,7 @@
         <v>0</v>
       </c>
       <c r="AP44" s="32">
-        <v>8.8379999999999992</v>
+        <v>1.6996153846153845</v>
       </c>
     </row>
     <row r="45" spans="1:42" ht="15.6" x14ac:dyDescent="0.3">
@@ -22974,13 +22974,13 @@
         <v>0</v>
       </c>
       <c r="X45" s="46">
-        <v>11.4428</v>
+        <v>2.2005384615384616</v>
       </c>
       <c r="Y45" s="46">
         <v>0</v>
       </c>
       <c r="Z45" s="46">
-        <v>5.0924000000000005</v>
+        <v>0.97930769230769243</v>
       </c>
       <c r="AA45" s="46">
         <v>0</v>
@@ -23105,13 +23105,13 @@
         <v>0</v>
       </c>
       <c r="Y46" s="46">
-        <v>5.0924000000000005</v>
+        <v>0.97930769230769243</v>
       </c>
       <c r="Z46" s="46">
         <v>0</v>
       </c>
       <c r="AA46" s="46">
-        <v>6.3364000000000003</v>
+        <v>1.2185384615384616</v>
       </c>
       <c r="AB46" s="46">
         <v>0</v>
@@ -23236,16 +23236,16 @@
         <v>0</v>
       </c>
       <c r="Z47" s="46">
-        <v>6.3364000000000003</v>
+        <v>1.2185384615384616</v>
       </c>
       <c r="AA47" s="46">
         <v>0</v>
       </c>
       <c r="AB47" s="46">
-        <v>6.6024000000000003</v>
+        <v>1.2696923076923077</v>
       </c>
       <c r="AC47" s="46">
-        <v>7.1392000000000007</v>
+        <v>1.3729230769230771</v>
       </c>
       <c r="AD47" s="32">
         <v>0</v>
@@ -23367,7 +23367,7 @@
         <v>0</v>
       </c>
       <c r="AA48" s="46">
-        <v>6.6024000000000003</v>
+        <v>1.2696923076923077</v>
       </c>
       <c r="AB48" s="46">
         <v>0</v>
@@ -23495,7 +23495,7 @@
         <v>0</v>
       </c>
       <c r="AA49" s="46">
-        <v>7.1392000000000007</v>
+        <v>1.3729230769230771</v>
       </c>
       <c r="AB49" s="46">
         <v>0</v>
@@ -23519,7 +23519,7 @@
         <v>0</v>
       </c>
       <c r="AI49" s="32">
-        <v>8.9832000000000001</v>
+        <v>1.7275384615384617</v>
       </c>
       <c r="AJ49" s="46">
         <v>0</v>
@@ -23587,10 +23587,10 @@
         <v>0</v>
       </c>
       <c r="O50" s="11">
-        <v>5.5836000000000006</v>
+        <v>1.0737692307692308</v>
       </c>
       <c r="P50" s="11">
-        <v>2.8575999999999997</v>
+        <v>0.54953846153846153</v>
       </c>
       <c r="Q50" s="11">
         <v>0</v>
@@ -23605,7 +23605,7 @@
         <v>0</v>
       </c>
       <c r="U50" s="11">
-        <v>3.8188</v>
+        <v>0.73438461538461541</v>
       </c>
       <c r="V50" s="11">
         <v>0</v>
@@ -23709,7 +23709,7 @@
         <v>0</v>
       </c>
       <c r="M51" s="11">
-        <v>4.34</v>
+        <v>0.83461538461538465</v>
       </c>
       <c r="N51" s="11">
         <v>0</v>
@@ -23915,7 +23915,7 @@
         <v>0</v>
       </c>
       <c r="AM52" s="46">
-        <v>10.4</v>
+        <v>2</v>
       </c>
       <c r="AN52" s="46">
         <v>0</v>
@@ -24043,7 +24043,7 @@
         <v>0</v>
       </c>
       <c r="AM53" s="46">
-        <v>10.8</v>
+        <v>2.0769230769230771</v>
       </c>
       <c r="AN53" s="46">
         <v>0</v>
@@ -24174,7 +24174,7 @@
         <v>0</v>
       </c>
       <c r="AN54" s="46">
-        <v>10.4</v>
+        <v>2</v>
       </c>
       <c r="AO54" s="46">
         <v>0</v>
@@ -24302,7 +24302,7 @@
         <v>0</v>
       </c>
       <c r="AN55" s="46">
-        <v>10.8</v>
+        <v>2.0769230769230771</v>
       </c>
       <c r="AO55" s="46">
         <v>0</v>
@@ -24433,7 +24433,7 @@
         <v>0</v>
       </c>
       <c r="AO56" s="46">
-        <v>12</v>
+        <v>2.3076923076923075</v>
       </c>
       <c r="AP56" s="32">
         <v>0</v>
@@ -24561,7 +24561,7 @@
         <v>0</v>
       </c>
       <c r="AO57" s="46">
-        <v>11.2</v>
+        <v>2.1538461538461537</v>
       </c>
       <c r="AP57" s="32">
         <v>0</v>
@@ -24692,7 +24692,7 @@
         <v>0</v>
       </c>
       <c r="AP58" s="32">
-        <v>8.8000000000000007</v>
+        <v>1.6923076923076925</v>
       </c>
     </row>
     <row r="59" spans="1:42" ht="16.2" thickBot="1" x14ac:dyDescent="0.35">
@@ -24820,7 +24820,7 @@
         <v>0</v>
       </c>
       <c r="AP59" s="12">
-        <v>8.4</v>
+        <v>1.6153846153846154</v>
       </c>
     </row>
     <row r="60" spans="1:42" ht="15.6" x14ac:dyDescent="0.3">
@@ -24849,7 +24849,7 @@
         <v>0</v>
       </c>
       <c r="I60" s="46">
-        <v>7.0396000000000001</v>
+        <v>1.3537692307692308</v>
       </c>
       <c r="J60" s="46">
         <v>0</v>
@@ -24939,10 +24939,10 @@
         <v>0</v>
       </c>
       <c r="AM60" s="46">
-        <v>28.063880000000005</v>
+        <v>5.3969000000000005</v>
       </c>
       <c r="AN60" s="46">
-        <v>24.708839999999999</v>
+        <v>4.7516999999999996</v>
       </c>
       <c r="AO60" s="46">
         <v>0</v>
@@ -25013,7 +25013,7 @@
         <v>0</v>
       </c>
       <c r="U61" s="11">
-        <v>9.0667999999999989</v>
+        <v>1.7436153846153843</v>
       </c>
       <c r="V61" s="11">
         <v>0</v>
@@ -25073,10 +25073,10 @@
         <v>0</v>
       </c>
       <c r="AO61" s="11">
-        <v>37.559080000000002</v>
+        <v>7.222900000000001</v>
       </c>
       <c r="AP61" s="12">
-        <v>37.183640000000004</v>
+        <v>7.1507000000000005</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Update input files with node capacity tab
</commit_message>
<xml_diff>
--- a/pareto/case_studies/input_data_generic_strategic_case_study_LAYFLAT_FULL.xlsx
+++ b/pareto/case_studies/input_data_generic_strategic_case_study_LAYFLAT_FULL.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="24527"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="24827"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\GitHub\PARETO - dev\project-pareto\pareto\case_studies\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{C7BA1116-7D67-4951-AAC0-08F92A26DE3F}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{CCAA3210-01C8-4401-93F4-5B83C618D471}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="17640" tabRatio="834" firstSheet="53" activeTab="61" xr2:uid="{FB8C51AB-905F-4544-9E4B-1F4384FA855C}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="17640" tabRatio="834" xr2:uid="{FB8C51AB-905F-4544-9E4B-1F4384FA855C}"/>
   </bookViews>
   <sheets>
     <sheet name="Overview" sheetId="33" r:id="rId1"/>
@@ -49,36 +49,37 @@
     <sheet name="CompletionsDemand" sheetId="8" r:id="rId34"/>
     <sheet name="PadRates" sheetId="65" r:id="rId35"/>
     <sheet name="FlowbackRates" sheetId="75" r:id="rId36"/>
-    <sheet name="InitialPipelineCapacity" sheetId="66" r:id="rId37"/>
-    <sheet name="InitialDisposalCapacity" sheetId="46" r:id="rId38"/>
-    <sheet name="InitialStorageCapacity" sheetId="80" r:id="rId39"/>
-    <sheet name="InitialTreatmentCapacity" sheetId="67" r:id="rId40"/>
-    <sheet name="FreshwaterSourcingAvailability" sheetId="47" r:id="rId41"/>
-    <sheet name="CompletionsPadStorage" sheetId="72" r:id="rId42"/>
-    <sheet name="PadOffloadingCapacity" sheetId="48" r:id="rId43"/>
-    <sheet name="TruckingTime" sheetId="7" r:id="rId44"/>
-    <sheet name="DisposalOperationalCost" sheetId="49" r:id="rId45"/>
-    <sheet name="TreatmentOperationalCost" sheetId="68" r:id="rId46"/>
-    <sheet name="ReuseOperationalCost" sheetId="50" r:id="rId47"/>
-    <sheet name="PipelineOperationalCost" sheetId="69" r:id="rId48"/>
-    <sheet name="FreshSourcingCost" sheetId="52" r:id="rId49"/>
-    <sheet name="TruckingHourlyCost" sheetId="71" r:id="rId50"/>
-    <sheet name="PipelineDiameterValues" sheetId="78" r:id="rId51"/>
-    <sheet name="DisposalCapacityIncrements" sheetId="79" r:id="rId52"/>
-    <sheet name="StorageCapacityIncrements" sheetId="81" r:id="rId53"/>
-    <sheet name="TreatmentCapacityIncrements" sheetId="87" r:id="rId54"/>
-    <sheet name="TreatmentEfficiency" sheetId="85" r:id="rId55"/>
-    <sheet name="DisposalExpansionCost" sheetId="90" r:id="rId56"/>
-    <sheet name="StorageExpansionCost" sheetId="91" r:id="rId57"/>
-    <sheet name="TreatmentExpansionCost" sheetId="92" r:id="rId58"/>
-    <sheet name="PipelineExpansionCost" sheetId="89" r:id="rId59"/>
-    <sheet name="PipelineExpansionDistance" sheetId="94" r:id="rId60"/>
-    <sheet name="Hydraulics" sheetId="93" r:id="rId61"/>
-    <sheet name="Economics" sheetId="95" r:id="rId62"/>
+    <sheet name="NodeCapacities" sheetId="96" r:id="rId37"/>
+    <sheet name="InitialPipelineCapacity" sheetId="66" r:id="rId38"/>
+    <sheet name="InitialDisposalCapacity" sheetId="46" r:id="rId39"/>
+    <sheet name="InitialStorageCapacity" sheetId="80" r:id="rId40"/>
+    <sheet name="InitialTreatmentCapacity" sheetId="67" r:id="rId41"/>
+    <sheet name="FreshwaterSourcingAvailability" sheetId="47" r:id="rId42"/>
+    <sheet name="CompletionsPadStorage" sheetId="72" r:id="rId43"/>
+    <sheet name="PadOffloadingCapacity" sheetId="48" r:id="rId44"/>
+    <sheet name="TruckingTime" sheetId="7" r:id="rId45"/>
+    <sheet name="DisposalOperationalCost" sheetId="49" r:id="rId46"/>
+    <sheet name="TreatmentOperationalCost" sheetId="68" r:id="rId47"/>
+    <sheet name="ReuseOperationalCost" sheetId="50" r:id="rId48"/>
+    <sheet name="PipelineOperationalCost" sheetId="69" r:id="rId49"/>
+    <sheet name="FreshSourcingCost" sheetId="52" r:id="rId50"/>
+    <sheet name="TruckingHourlyCost" sheetId="71" r:id="rId51"/>
+    <sheet name="PipelineDiameterValues" sheetId="78" r:id="rId52"/>
+    <sheet name="DisposalCapacityIncrements" sheetId="79" r:id="rId53"/>
+    <sheet name="StorageCapacityIncrements" sheetId="81" r:id="rId54"/>
+    <sheet name="TreatmentCapacityIncrements" sheetId="87" r:id="rId55"/>
+    <sheet name="TreatmentEfficiency" sheetId="85" r:id="rId56"/>
+    <sheet name="DisposalExpansionCost" sheetId="90" r:id="rId57"/>
+    <sheet name="StorageExpansionCost" sheetId="91" r:id="rId58"/>
+    <sheet name="TreatmentExpansionCost" sheetId="92" r:id="rId59"/>
+    <sheet name="PipelineExpansionCost" sheetId="89" r:id="rId60"/>
+    <sheet name="PipelineExpansionDistance" sheetId="94" r:id="rId61"/>
+    <sheet name="Hydraulics" sheetId="93" r:id="rId62"/>
+    <sheet name="Economics" sheetId="95" r:id="rId63"/>
   </sheets>
   <definedNames>
-    <definedName name="_xlnm._FilterDatabase" localSheetId="59" hidden="1">#REF!</definedName>
-    <definedName name="_xlnm.Extract" localSheetId="59">PipelineExpansionDistance!$O$3</definedName>
+    <definedName name="_xlnm._FilterDatabase" localSheetId="60" hidden="1">#REF!</definedName>
+    <definedName name="_xlnm.Extract" localSheetId="60">PipelineExpansionDistance!$O$3</definedName>
   </definedNames>
   <calcPr calcId="191029"/>
   <extLst>
@@ -99,7 +100,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1110" uniqueCount="273">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1142" uniqueCount="274">
   <si>
     <t>List of all Production Pad Identifiers [-]</t>
   </si>
@@ -918,6 +919,9 @@
   </si>
   <si>
     <t>CAPEX_lifetime</t>
+  </si>
+  <si>
+    <t>Table of Node Capacity Capacity  [bbl/week]</t>
   </si>
 </sst>
 </file>
@@ -1723,7 +1727,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{80E5E074-61D5-4D82-B0DB-255C2595EBED}">
   <dimension ref="B1:M37"/>
   <sheetViews>
-    <sheetView zoomScale="110" zoomScaleNormal="110" workbookViewId="0"/>
+    <sheetView tabSelected="1" zoomScale="110" zoomScaleNormal="110" workbookViewId="0"/>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
@@ -2459,7 +2463,7 @@
   <dimension ref="A1:T30"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="F3" sqref="F3"/>
+      <selection activeCell="I12" sqref="I12"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9.28515625" defaultRowHeight="15.75" x14ac:dyDescent="0.25"/>
@@ -12641,6 +12645,270 @@
 </file>
 
 <file path=xl/worksheets/sheet37.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{177368FE-B582-4A98-BA14-59D042664C2C}">
+  <dimension ref="A1:B31"/>
+  <sheetViews>
+    <sheetView workbookViewId="0"/>
+  </sheetViews>
+  <sheetFormatPr defaultColWidth="9.28515625" defaultRowHeight="15.75" x14ac:dyDescent="0.25"/>
+  <cols>
+    <col min="1" max="1" width="11" style="1" customWidth="1"/>
+    <col min="2" max="2" width="10.140625" style="1" bestFit="1" customWidth="1"/>
+    <col min="3" max="16384" width="9.28515625" style="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:2" ht="16.5" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A1" s="1" t="s">
+        <v>273</v>
+      </c>
+    </row>
+    <row r="2" spans="1:2" s="9" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A2" s="7" t="s">
+        <v>248</v>
+      </c>
+      <c r="B2" s="28" t="s">
+        <v>250</v>
+      </c>
+    </row>
+    <row r="3" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A3" s="29" t="s">
+        <v>150</v>
+      </c>
+      <c r="B3" s="38">
+        <v>1000000</v>
+      </c>
+    </row>
+    <row r="4" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A4" s="29" t="s">
+        <v>83</v>
+      </c>
+      <c r="B4" s="38">
+        <v>1000000</v>
+      </c>
+    </row>
+    <row r="5" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A5" s="29" t="s">
+        <v>84</v>
+      </c>
+      <c r="B5" s="38">
+        <v>1000000</v>
+      </c>
+    </row>
+    <row r="6" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A6" s="29" t="s">
+        <v>85</v>
+      </c>
+      <c r="B6" s="38">
+        <v>1000000</v>
+      </c>
+    </row>
+    <row r="7" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A7" s="29" t="s">
+        <v>86</v>
+      </c>
+      <c r="B7" s="38">
+        <v>1000000</v>
+      </c>
+    </row>
+    <row r="8" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A8" s="29" t="s">
+        <v>87</v>
+      </c>
+      <c r="B8" s="38">
+        <v>1000000</v>
+      </c>
+    </row>
+    <row r="9" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A9" s="29" t="s">
+        <v>88</v>
+      </c>
+      <c r="B9" s="38">
+        <v>1000000</v>
+      </c>
+    </row>
+    <row r="10" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A10" s="29" t="s">
+        <v>89</v>
+      </c>
+      <c r="B10" s="38">
+        <v>1000000</v>
+      </c>
+    </row>
+    <row r="11" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A11" s="29" t="s">
+        <v>151</v>
+      </c>
+      <c r="B11" s="38">
+        <v>1000000</v>
+      </c>
+    </row>
+    <row r="12" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A12" s="29" t="s">
+        <v>152</v>
+      </c>
+      <c r="B12" s="38">
+        <v>1000000</v>
+      </c>
+    </row>
+    <row r="13" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A13" s="29" t="s">
+        <v>153</v>
+      </c>
+      <c r="B13" s="38">
+        <v>1000000</v>
+      </c>
+    </row>
+    <row r="14" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A14" s="29" t="s">
+        <v>154</v>
+      </c>
+      <c r="B14" s="38">
+        <v>1000000</v>
+      </c>
+    </row>
+    <row r="15" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A15" s="29" t="s">
+        <v>155</v>
+      </c>
+      <c r="B15" s="38">
+        <v>1000000</v>
+      </c>
+    </row>
+    <row r="16" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A16" s="29" t="s">
+        <v>156</v>
+      </c>
+      <c r="B16" s="38">
+        <v>1000000</v>
+      </c>
+    </row>
+    <row r="17" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A17" s="29" t="s">
+        <v>157</v>
+      </c>
+      <c r="B17" s="38">
+        <v>1000000</v>
+      </c>
+    </row>
+    <row r="18" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A18" s="29" t="s">
+        <v>158</v>
+      </c>
+      <c r="B18" s="38">
+        <v>1000000</v>
+      </c>
+    </row>
+    <row r="19" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A19" s="29" t="s">
+        <v>159</v>
+      </c>
+      <c r="B19" s="38">
+        <v>1000000</v>
+      </c>
+    </row>
+    <row r="20" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A20" s="29" t="s">
+        <v>160</v>
+      </c>
+      <c r="B20" s="38">
+        <v>1000000</v>
+      </c>
+    </row>
+    <row r="21" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A21" s="29" t="s">
+        <v>161</v>
+      </c>
+      <c r="B21" s="38">
+        <v>1000000</v>
+      </c>
+    </row>
+    <row r="22" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A22" s="29" t="s">
+        <v>162</v>
+      </c>
+      <c r="B22" s="38">
+        <v>1000000</v>
+      </c>
+    </row>
+    <row r="23" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A23" s="29" t="s">
+        <v>163</v>
+      </c>
+      <c r="B23" s="38">
+        <v>1000000</v>
+      </c>
+    </row>
+    <row r="24" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A24" s="29" t="s">
+        <v>164</v>
+      </c>
+      <c r="B24" s="38">
+        <v>1000000</v>
+      </c>
+    </row>
+    <row r="25" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A25" s="29" t="s">
+        <v>165</v>
+      </c>
+      <c r="B25" s="38">
+        <v>1000000</v>
+      </c>
+    </row>
+    <row r="26" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A26" s="29" t="s">
+        <v>166</v>
+      </c>
+      <c r="B26" s="38">
+        <v>1000000</v>
+      </c>
+    </row>
+    <row r="27" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A27" s="29" t="s">
+        <v>167</v>
+      </c>
+      <c r="B27" s="38">
+        <v>1000000</v>
+      </c>
+    </row>
+    <row r="28" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A28" s="29" t="s">
+        <v>168</v>
+      </c>
+      <c r="B28" s="38">
+        <v>1000000</v>
+      </c>
+    </row>
+    <row r="29" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A29" s="29" t="s">
+        <v>169</v>
+      </c>
+      <c r="B29" s="38">
+        <v>1000000</v>
+      </c>
+    </row>
+    <row r="30" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A30" s="29" t="s">
+        <v>170</v>
+      </c>
+      <c r="B30" s="38">
+        <v>1000000</v>
+      </c>
+    </row>
+    <row r="31" spans="1:2" ht="16.5" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A31" s="30" t="s">
+        <v>171</v>
+      </c>
+      <c r="B31" s="40">
+        <v>1000000</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup orientation="portrait" r:id="rId1"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet38.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{9AE628BF-A05C-42C8-8EC7-63FF3B624ADC}">
   <dimension ref="A1:U26"/>
   <sheetViews>
@@ -13433,7 +13701,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet38.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet39.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{50D65BC4-7454-4A45-AA93-771B11A13108}">
   <dimension ref="A1:B7"/>
   <sheetViews>
@@ -13496,46 +13764,6 @@
         <v>140</v>
       </c>
       <c r="B7" s="40">
-        <v>0</v>
-      </c>
-    </row>
-  </sheetData>
-  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <pageSetup orientation="portrait" r:id="rId1"/>
-</worksheet>
-</file>
-
-<file path=xl/worksheets/sheet39.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{CEDF796A-A87C-4F37-A825-AF0AD18C802A}">
-  <dimension ref="A1:B3"/>
-  <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="A2" sqref="A2"/>
-    </sheetView>
-  </sheetViews>
-  <sheetFormatPr defaultColWidth="9.28515625" defaultRowHeight="15.75" x14ac:dyDescent="0.25"/>
-  <cols>
-    <col min="1" max="16384" width="9.28515625" style="1"/>
-  </cols>
-  <sheetData>
-    <row r="1" spans="1:2" ht="16.5" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A1" s="1" t="s">
-        <v>202</v>
-      </c>
-    </row>
-    <row r="2" spans="1:2" s="9" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A2" s="7" t="s">
-        <v>254</v>
-      </c>
-      <c r="B2" s="28" t="s">
-        <v>250</v>
-      </c>
-    </row>
-    <row r="3" spans="1:2" ht="16.5" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A3" s="30" t="s">
-        <v>81</v>
-      </c>
-      <c r="B3" s="40">
         <v>0</v>
       </c>
     </row>
@@ -13728,6 +13956,46 @@
 </file>
 
 <file path=xl/worksheets/sheet40.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{CEDF796A-A87C-4F37-A825-AF0AD18C802A}">
+  <dimension ref="A1:B3"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="A2" sqref="A2"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultColWidth="9.28515625" defaultRowHeight="15.75" x14ac:dyDescent="0.25"/>
+  <cols>
+    <col min="1" max="16384" width="9.28515625" style="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:2" ht="16.5" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A1" s="1" t="s">
+        <v>202</v>
+      </c>
+    </row>
+    <row r="2" spans="1:2" s="9" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A2" s="7" t="s">
+        <v>254</v>
+      </c>
+      <c r="B2" s="28" t="s">
+        <v>250</v>
+      </c>
+    </row>
+    <row r="3" spans="1:2" ht="16.5" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A3" s="30" t="s">
+        <v>81</v>
+      </c>
+      <c r="B3" s="40">
+        <v>0</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup orientation="portrait" r:id="rId1"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet41.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{09A13F53-E3AE-452E-A1A1-316A2C800322}">
   <dimension ref="A1:B4"/>
   <sheetViews>
@@ -13775,7 +14043,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet41.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet42.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{F4A2DBF7-A8C0-4CE1-BE66-F8E077B6F0F1}">
   <dimension ref="A1:BA21"/>
   <sheetViews>
@@ -15294,7 +15562,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet42.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet43.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{9DAB793D-71C1-4CA2-A5D0-D94D2FB81D42}">
   <dimension ref="A1:B6"/>
   <sheetViews>
@@ -15360,7 +15628,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet43.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet44.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{F216C6A0-7BAD-498F-AAE7-F43EE79415DD}">
   <dimension ref="A1:B3"/>
   <sheetViews>
@@ -15400,7 +15668,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet44.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet45.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{4D257926-ED56-4D32-9A5B-F7129B221F36}">
   <dimension ref="A1:F20"/>
   <sheetViews>
@@ -15614,7 +15882,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet45.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet46.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{CDED9A13-6613-4A4D-92BC-DD0B79B273AD}">
   <dimension ref="A1:B7"/>
   <sheetViews>
@@ -15687,7 +15955,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet46.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet47.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{E7050C77-5C7B-4C97-8F2B-C60EA6AF1AED}">
   <dimension ref="A1:B4"/>
   <sheetViews>
@@ -15735,7 +16003,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet47.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet48.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{0F35D225-B5AF-4E75-9547-7AC1A8034351}">
   <dimension ref="A1:B6"/>
   <sheetViews>
@@ -15799,7 +16067,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet48.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet49.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{5AE24AD9-42B2-417F-BF2D-D0F067DA599C}">
   <dimension ref="A1:G10"/>
   <sheetViews>
@@ -15940,102 +16208,6 @@
     </row>
   </sheetData>
   <phoneticPr fontId="2" type="noConversion"/>
-  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <pageSetup orientation="portrait" r:id="rId1"/>
-</worksheet>
-</file>
-
-<file path=xl/worksheets/sheet49.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{61B9AF2E-9304-4DC1-ABFA-7D5DAA6BA0BC}">
-  <dimension ref="A1:B10"/>
-  <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="A2" sqref="A2"/>
-    </sheetView>
-  </sheetViews>
-  <sheetFormatPr defaultColWidth="9.28515625" defaultRowHeight="15.75" x14ac:dyDescent="0.25"/>
-  <cols>
-    <col min="1" max="16384" width="9.28515625" style="1"/>
-  </cols>
-  <sheetData>
-    <row r="1" spans="1:2" ht="16.5" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A1" s="1" t="s">
-        <v>187</v>
-      </c>
-    </row>
-    <row r="2" spans="1:2" s="9" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A2" s="7" t="s">
-        <v>253</v>
-      </c>
-      <c r="B2" s="28" t="s">
-        <v>250</v>
-      </c>
-    </row>
-    <row r="3" spans="1:2" s="9" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A3" s="29" t="s">
-        <v>67</v>
-      </c>
-      <c r="B3" s="32">
-        <v>1.35</v>
-      </c>
-    </row>
-    <row r="4" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A4" s="29" t="s">
-        <v>68</v>
-      </c>
-      <c r="B4" s="32">
-        <v>1.25</v>
-      </c>
-    </row>
-    <row r="5" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A5" s="29" t="s">
-        <v>142</v>
-      </c>
-      <c r="B5" s="32">
-        <v>1.35</v>
-      </c>
-    </row>
-    <row r="6" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A6" s="29" t="s">
-        <v>143</v>
-      </c>
-      <c r="B6" s="32">
-        <v>1.25</v>
-      </c>
-    </row>
-    <row r="7" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A7" s="29" t="s">
-        <v>144</v>
-      </c>
-      <c r="B7" s="32">
-        <v>1.35</v>
-      </c>
-    </row>
-    <row r="8" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A8" s="29" t="s">
-        <v>145</v>
-      </c>
-      <c r="B8" s="32">
-        <v>1.1499999999999999</v>
-      </c>
-    </row>
-    <row r="9" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A9" s="29" t="s">
-        <v>146</v>
-      </c>
-      <c r="B9" s="32">
-        <v>1.35</v>
-      </c>
-    </row>
-    <row r="10" spans="1:2" ht="16.5" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A10" s="30" t="s">
-        <v>147</v>
-      </c>
-      <c r="B10" s="12">
-        <v>1.25</v>
-      </c>
-    </row>
-  </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" r:id="rId1"/>
 </worksheet>
@@ -16229,6 +16401,102 @@
 </file>
 
 <file path=xl/worksheets/sheet50.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{61B9AF2E-9304-4DC1-ABFA-7D5DAA6BA0BC}">
+  <dimension ref="A1:B10"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="A2" sqref="A2"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultColWidth="9.28515625" defaultRowHeight="15.75" x14ac:dyDescent="0.25"/>
+  <cols>
+    <col min="1" max="16384" width="9.28515625" style="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:2" ht="16.5" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A1" s="1" t="s">
+        <v>187</v>
+      </c>
+    </row>
+    <row r="2" spans="1:2" s="9" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A2" s="7" t="s">
+        <v>253</v>
+      </c>
+      <c r="B2" s="28" t="s">
+        <v>250</v>
+      </c>
+    </row>
+    <row r="3" spans="1:2" s="9" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A3" s="29" t="s">
+        <v>67</v>
+      </c>
+      <c r="B3" s="32">
+        <v>1.35</v>
+      </c>
+    </row>
+    <row r="4" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A4" s="29" t="s">
+        <v>68</v>
+      </c>
+      <c r="B4" s="32">
+        <v>1.25</v>
+      </c>
+    </row>
+    <row r="5" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A5" s="29" t="s">
+        <v>142</v>
+      </c>
+      <c r="B5" s="32">
+        <v>1.35</v>
+      </c>
+    </row>
+    <row r="6" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A6" s="29" t="s">
+        <v>143</v>
+      </c>
+      <c r="B6" s="32">
+        <v>1.25</v>
+      </c>
+    </row>
+    <row r="7" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A7" s="29" t="s">
+        <v>144</v>
+      </c>
+      <c r="B7" s="32">
+        <v>1.35</v>
+      </c>
+    </row>
+    <row r="8" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A8" s="29" t="s">
+        <v>145</v>
+      </c>
+      <c r="B8" s="32">
+        <v>1.1499999999999999</v>
+      </c>
+    </row>
+    <row r="9" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A9" s="29" t="s">
+        <v>146</v>
+      </c>
+      <c r="B9" s="32">
+        <v>1.35</v>
+      </c>
+    </row>
+    <row r="10" spans="1:2" ht="16.5" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A10" s="30" t="s">
+        <v>147</v>
+      </c>
+      <c r="B10" s="12">
+        <v>1.25</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup orientation="portrait" r:id="rId1"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet51.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{35585569-7889-4883-A327-3B12D4AB6358}">
   <dimension ref="A1:B23"/>
   <sheetViews>
@@ -16429,7 +16697,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet51.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet52.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{805632D3-BD42-4D5C-8C0F-68DF124ED3E8}">
   <dimension ref="A1:B8"/>
   <sheetViews>
@@ -16509,7 +16777,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet52.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet53.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{982C988E-F277-4EB8-BD08-045871CAA4ED}">
   <dimension ref="A1:B6"/>
   <sheetViews>
@@ -16573,7 +16841,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet53.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet54.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{52F26805-7F3D-4935-8D0C-80B2E9E9F409}">
   <dimension ref="A1:B6"/>
   <sheetViews>
@@ -16637,7 +16905,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet54.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet55.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{5F6DB070-53D7-4763-B1D6-04233A007F0E}">
   <dimension ref="A1:B6"/>
   <sheetViews>
@@ -16701,7 +16969,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet55.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet56.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{92B45C9D-7A15-425D-8487-B88B27280274}">
   <dimension ref="A1:B4"/>
   <sheetViews>
@@ -16749,7 +17017,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet56.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet57.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{B1E5CD4B-C8DB-4A49-956D-761D45563331}">
   <dimension ref="A1:E18"/>
   <sheetViews>
@@ -16912,7 +17180,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet57.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet58.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{344AC655-401B-435E-9F3E-B4AFCEDA07DB}">
   <dimension ref="A1:E14"/>
   <sheetViews>
@@ -17006,7 +17274,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet58.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet59.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{906D3944-A6F1-468B-A756-A99C077811C6}">
   <dimension ref="A1:E15"/>
   <sheetViews>
@@ -17114,46 +17382,6 @@
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" r:id="rId1"/>
-</worksheet>
-</file>
-
-<file path=xl/worksheets/sheet59.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{6C902C13-E391-4A34-8851-63FF84EE5034}">
-  <dimension ref="A1:B3"/>
-  <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="B5" sqref="B5"/>
-    </sheetView>
-  </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
-  <cols>
-    <col min="1" max="1" width="33.140625" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="9.28515625" customWidth="1"/>
-  </cols>
-  <sheetData>
-    <row r="1" spans="1:2" ht="16.5" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A1" s="31" t="s">
-        <v>267</v>
-      </c>
-    </row>
-    <row r="2" spans="1:2" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="A2" s="7" t="s">
-        <v>269</v>
-      </c>
-      <c r="B2" s="28" t="s">
-        <v>264</v>
-      </c>
-    </row>
-    <row r="3" spans="1:2" ht="16.5" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A3" s="30" t="s">
-        <v>268</v>
-      </c>
-      <c r="B3" s="40">
-        <v>120000</v>
-      </c>
-    </row>
-  </sheetData>
-  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
 </file>
 
@@ -17294,6 +17522,46 @@
 </file>
 
 <file path=xl/worksheets/sheet60.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{6C902C13-E391-4A34-8851-63FF84EE5034}">
+  <dimension ref="A1:B3"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="B5" sqref="B5"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <cols>
+    <col min="1" max="1" width="33.140625" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="9.28515625" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:2" ht="16.5" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A1" s="31" t="s">
+        <v>267</v>
+      </c>
+    </row>
+    <row r="2" spans="1:2" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="A2" s="7" t="s">
+        <v>269</v>
+      </c>
+      <c r="B2" s="28" t="s">
+        <v>264</v>
+      </c>
+    </row>
+    <row r="3" spans="1:2" ht="16.5" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A3" s="30" t="s">
+        <v>268</v>
+      </c>
+      <c r="B3" s="40">
+        <v>120000</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet61.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{9AE67BAE-6607-47A3-AB16-0544FAF51C24}">
   <dimension ref="A1:AP61"/>
   <sheetViews>
@@ -24993,7 +25261,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet61.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet62.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{92EDDE38-2D71-4494-ABC1-8D5269A138D9}">
   <dimension ref="A1:B4"/>
   <sheetViews>
@@ -25040,12 +25308,12 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet62.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet63.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{ED2F8796-71C2-44EA-9373-5A0165D7B559}">
   <dimension ref="A1:B4"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="F10" sqref="F10"/>
+    <sheetView topLeftCell="A4" workbookViewId="0">
+      <selection activeCell="A44" sqref="A44:A46"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>

</xml_diff>

<commit_message>
Update documentation, add config option for including pipeline capacity, only build constraint if a value is inputted for node.
</commit_message>
<xml_diff>
--- a/pareto/case_studies/input_data_generic_strategic_case_study_LAYFLAT_FULL.xlsx
+++ b/pareto/case_studies/input_data_generic_strategic_case_study_LAYFLAT_FULL.xlsx
@@ -5,12 +5,12 @@
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\NienkeW\Downloads\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\GitHub\PARETO - dev\project-pareto\pareto\case_studies\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{4E136156-4F56-49BB-BBB8-422B549DE4F8}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{81BFF46E-F655-4AC7-958E-AFD75318A040}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="28680" yWindow="-120" windowWidth="29040" windowHeight="17640" tabRatio="834" xr2:uid="{FB8C51AB-905F-4544-9E4B-1F4384FA855C}"/>
+    <workbookView xWindow="28680" yWindow="-120" windowWidth="29040" windowHeight="17640" tabRatio="834" firstSheet="14" activeTab="35" xr2:uid="{FB8C51AB-905F-4544-9E4B-1F4384FA855C}"/>
   </bookViews>
   <sheets>
     <sheet name="Overview" sheetId="33" r:id="rId1"/>
@@ -980,7 +980,7 @@
     <t>Initial Water Quality at Completiond Pad Storage (mg/L)</t>
   </si>
   <si>
-    <t>Table of Node Capacity Capacity  [bbl/week]</t>
+    <t>Table of Node Capacity Capacity  [bbl/week] * absence of node or empty cell signifies no max capacity</t>
   </si>
 </sst>
 </file>
@@ -1976,7 +1976,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{80E5E074-61D5-4D82-B0DB-255C2595EBED}">
   <dimension ref="B1:M37"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="110" zoomScaleNormal="110" workbookViewId="0"/>
+    <sheetView zoomScale="110" zoomScaleNormal="110" workbookViewId="0"/>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
@@ -12178,7 +12178,9 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{D27E83FA-0F3B-443C-8B3E-ADC37406AEAD}">
   <dimension ref="A1:B31"/>
   <sheetViews>
-    <sheetView workbookViewId="0"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="C4" sqref="C4"/>
+    </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9.28515625" defaultRowHeight="15.75" x14ac:dyDescent="0.25"/>
   <cols>
@@ -12204,233 +12206,175 @@
       <c r="A3" s="29" t="s">
         <v>150</v>
       </c>
-      <c r="B3" s="38">
-        <v>1000000</v>
-      </c>
+      <c r="B3" s="38"/>
     </row>
     <row r="4" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A4" s="29" t="s">
         <v>83</v>
       </c>
-      <c r="B4" s="38">
-        <v>1000000</v>
-      </c>
+      <c r="B4" s="38"/>
     </row>
     <row r="5" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A5" s="29" t="s">
         <v>84</v>
       </c>
-      <c r="B5" s="38">
-        <v>1000000</v>
-      </c>
+      <c r="B5" s="38"/>
     </row>
     <row r="6" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A6" s="29" t="s">
         <v>85</v>
       </c>
-      <c r="B6" s="38">
-        <v>1000000</v>
-      </c>
+      <c r="B6" s="38"/>
     </row>
     <row r="7" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A7" s="29" t="s">
         <v>86</v>
       </c>
-      <c r="B7" s="38">
-        <v>1000000</v>
-      </c>
+      <c r="B7" s="38"/>
     </row>
     <row r="8" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A8" s="29" t="s">
         <v>87</v>
       </c>
-      <c r="B8" s="38">
-        <v>1000000</v>
-      </c>
+      <c r="B8" s="38"/>
     </row>
     <row r="9" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A9" s="29" t="s">
         <v>88</v>
       </c>
-      <c r="B9" s="38">
-        <v>1000000</v>
-      </c>
+      <c r="B9" s="38"/>
     </row>
     <row r="10" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A10" s="29" t="s">
         <v>89</v>
       </c>
-      <c r="B10" s="38">
-        <v>1000000</v>
-      </c>
+      <c r="B10" s="38"/>
     </row>
     <row r="11" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A11" s="29" t="s">
         <v>151</v>
       </c>
-      <c r="B11" s="38">
-        <v>1000000</v>
-      </c>
+      <c r="B11" s="38"/>
     </row>
     <row r="12" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A12" s="29" t="s">
         <v>152</v>
       </c>
-      <c r="B12" s="38">
-        <v>1000000</v>
-      </c>
+      <c r="B12" s="38"/>
     </row>
     <row r="13" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A13" s="29" t="s">
         <v>153</v>
       </c>
-      <c r="B13" s="38">
-        <v>1000000</v>
-      </c>
+      <c r="B13" s="38"/>
     </row>
     <row r="14" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A14" s="29" t="s">
         <v>154</v>
       </c>
-      <c r="B14" s="38">
-        <v>1000000</v>
-      </c>
+      <c r="B14" s="38"/>
     </row>
     <row r="15" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A15" s="29" t="s">
         <v>155</v>
       </c>
-      <c r="B15" s="38">
-        <v>1000000</v>
-      </c>
+      <c r="B15" s="38"/>
     </row>
     <row r="16" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A16" s="29" t="s">
         <v>156</v>
       </c>
-      <c r="B16" s="38">
-        <v>1000000</v>
-      </c>
+      <c r="B16" s="38"/>
     </row>
     <row r="17" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A17" s="29" t="s">
         <v>157</v>
       </c>
-      <c r="B17" s="38">
-        <v>1000000</v>
-      </c>
+      <c r="B17" s="38"/>
     </row>
     <row r="18" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A18" s="29" t="s">
         <v>158</v>
       </c>
-      <c r="B18" s="38">
-        <v>1000000</v>
-      </c>
+      <c r="B18" s="38"/>
     </row>
     <row r="19" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A19" s="29" t="s">
         <v>159</v>
       </c>
-      <c r="B19" s="38">
-        <v>1000000</v>
-      </c>
+      <c r="B19" s="38"/>
     </row>
     <row r="20" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A20" s="29" t="s">
         <v>160</v>
       </c>
-      <c r="B20" s="38">
-        <v>1000000</v>
-      </c>
+      <c r="B20" s="38"/>
     </row>
     <row r="21" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A21" s="29" t="s">
         <v>161</v>
       </c>
-      <c r="B21" s="38">
-        <v>1000000</v>
-      </c>
+      <c r="B21" s="38"/>
     </row>
     <row r="22" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A22" s="29" t="s">
         <v>162</v>
       </c>
-      <c r="B22" s="38">
-        <v>1000000</v>
-      </c>
+      <c r="B22" s="38"/>
     </row>
     <row r="23" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A23" s="29" t="s">
         <v>163</v>
       </c>
-      <c r="B23" s="38">
-        <v>1000000</v>
-      </c>
+      <c r="B23" s="38"/>
     </row>
     <row r="24" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A24" s="29" t="s">
         <v>164</v>
       </c>
-      <c r="B24" s="38">
-        <v>1000000</v>
-      </c>
+      <c r="B24" s="38"/>
     </row>
     <row r="25" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A25" s="29" t="s">
         <v>165</v>
       </c>
-      <c r="B25" s="38">
-        <v>1000000</v>
-      </c>
+      <c r="B25" s="38"/>
     </row>
     <row r="26" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A26" s="29" t="s">
         <v>166</v>
       </c>
-      <c r="B26" s="38">
-        <v>1000000</v>
-      </c>
+      <c r="B26" s="38"/>
     </row>
     <row r="27" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A27" s="29" t="s">
         <v>167</v>
       </c>
-      <c r="B27" s="38">
-        <v>1000000</v>
-      </c>
+      <c r="B27" s="38"/>
     </row>
     <row r="28" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A28" s="29" t="s">
         <v>168</v>
       </c>
-      <c r="B28" s="38">
-        <v>1000000</v>
-      </c>
+      <c r="B28" s="38"/>
     </row>
     <row r="29" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A29" s="29" t="s">
         <v>169</v>
       </c>
-      <c r="B29" s="38">
-        <v>1000000</v>
-      </c>
+      <c r="B29" s="38"/>
     </row>
     <row r="30" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A30" s="29" t="s">
         <v>170</v>
       </c>
-      <c r="B30" s="38">
-        <v>1000000</v>
-      </c>
+      <c r="B30" s="38"/>
     </row>
     <row r="31" spans="1:2" ht="16.5" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A31" s="30" t="s">
         <v>171</v>
       </c>
-      <c r="B31" s="40">
-        <v>1000000</v>
-      </c>
+      <c r="B31" s="40"/>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>

</xml_diff>

<commit_message>
autopopulate units in input file, update generate_results to select output units, add test for unit consistency, update oil_bbl to display as bbl
</commit_message>
<xml_diff>
--- a/pareto/case_studies/input_data_generic_strategic_case_study_LAYFLAT_FULL.xlsx
+++ b/pareto/case_studies/input_data_generic_strategic_case_study_LAYFLAT_FULL.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\melodys\Documents\1. Projects\PARETO - Department of Energy\Code Updates\GIT Tracked Folder\project-pareto\pareto\case_studies\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{CEA0A007-68A5-4F73-B6AA-FE5367B0D2E4}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{07327253-9B73-474C-AA9A-D5C81C57AF57}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" tabRatio="834" activeTab="2" xr2:uid="{FB8C51AB-905F-4544-9E4B-1F4384FA855C}"/>
+    <workbookView xWindow="16680" yWindow="-16320" windowWidth="29040" windowHeight="15840" tabRatio="834" firstSheet="2" activeTab="2" xr2:uid="{FB8C51AB-905F-4544-9E4B-1F4384FA855C}"/>
   </bookViews>
   <sheets>
     <sheet name="Overview" sheetId="33" r:id="rId1"/>
@@ -48,9 +48,9 @@
     <sheet name="CCT" sheetId="74" r:id="rId33"/>
     <sheet name="CST" sheetId="64" r:id="rId34"/>
     <sheet name="CompletionsDemand" sheetId="8" r:id="rId35"/>
-    <sheet name="NodeCapacities" sheetId="102" r:id="rId36"/>
-    <sheet name="PadRates" sheetId="65" r:id="rId37"/>
-    <sheet name="FlowbackRates" sheetId="75" r:id="rId38"/>
+    <sheet name="PadRates" sheetId="65" r:id="rId36"/>
+    <sheet name="FlowbackRates" sheetId="75" r:id="rId37"/>
+    <sheet name="NodeCapacities" sheetId="102" r:id="rId38"/>
     <sheet name="InitialPipelineCapacity" sheetId="66" r:id="rId39"/>
     <sheet name="InitialDisposalCapacity" sheetId="46" r:id="rId40"/>
     <sheet name="InitialStorageCapacity" sheetId="80" r:id="rId41"/>
@@ -133,7 +133,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="3570" uniqueCount="317">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="3547" uniqueCount="293">
   <si>
     <t>List of all Production Pad Identifiers [-]</t>
   </si>
@@ -885,125 +885,9 @@
     <t>TDS</t>
   </si>
   <si>
-    <t>PADS</t>
-  </si>
-  <si>
     <t>Pads</t>
   </si>
   <si>
-    <t>Table of Trucking Hourly Cost  [currency/hour]</t>
-  </si>
-  <si>
-    <t>Table of Disposal Operational Cost  [currency/volume]</t>
-  </si>
-  <si>
-    <t>Table of Treatment Operational Cost  [currency/volume]</t>
-  </si>
-  <si>
-    <t>Table of Reuse Operational Cost  [currency/volume]</t>
-  </si>
-  <si>
-    <t>Table of Pipeline Operational Cost between Sites [currency/volume]</t>
-  </si>
-  <si>
-    <t>Table of Freshwater Sourcing Cost  [currency/volume]</t>
-  </si>
-  <si>
-    <t>Table of Storage Capacity Expansion Cost [currency/volume]</t>
-  </si>
-  <si>
-    <t>Table of Node Capacity Capacity  [volume/time] * absence of node or empty cell signifies no max capacity</t>
-  </si>
-  <si>
-    <t>Table of Completions Water Demand for Completions Sites over Weeks [volume/time]</t>
-  </si>
-  <si>
-    <t>Table of Production Rate Forecasts by Pads [volume/time]</t>
-  </si>
-  <si>
-    <t>Table of Flowback Rate Forecasts by Pads [volume/time]</t>
-  </si>
-  <si>
-    <t>Table of Initial Pipeline Capacity between Sites [volume/time]</t>
-  </si>
-  <si>
-    <t>Table of Initial Disposal Capacity  [volume/time]</t>
-  </si>
-  <si>
-    <t>Table of Initial Treatment Capacity  [volume/time]</t>
-  </si>
-  <si>
-    <t>Table of Freshwater Sourcing Availability [volume/time]</t>
-  </si>
-  <si>
-    <t>Table of Pad Offloading Capacity  [volume/time]</t>
-  </si>
-  <si>
-    <t>Table of Disposal Capacity Expansion Increments [volume/time]</t>
-  </si>
-  <si>
-    <t>Table of Treatment Capacity Expansion Increments [volume/time]</t>
-  </si>
-  <si>
-    <t>Table of Pipeline Capacity Expansion Increments [volume/time]</t>
-  </si>
-  <si>
-    <t>Table of Initial Storage Capacity  [volume]</t>
-  </si>
-  <si>
-    <t>Table of Completions Pad Storage Capacity [volume]</t>
-  </si>
-  <si>
-    <t>Table of Storage Capacity Expansion Increments [volume]</t>
-  </si>
-  <si>
-    <t>Table of Pipeline Diameters [diameter]</t>
-  </si>
-  <si>
-    <t>Table of Disposal Capacity Expansion Cost [currency/(volume/time)]</t>
-  </si>
-  <si>
-    <t>Table of Treatment Capacity Expansion Cost [currency/(volume/time)]</t>
-  </si>
-  <si>
-    <r>
-      <t>Pipeline Expansion Cost [currency/(diameter</t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="12"/>
-        <color theme="1"/>
-        <rFont val="Calibri"/>
-        <family val="2"/>
-      </rPr>
-      <t>·</t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="12"/>
-        <color theme="1"/>
-        <rFont val="Times New Roman"/>
-        <family val="1"/>
-      </rPr>
-      <t>distance)]</t>
-    </r>
-  </si>
-  <si>
-    <t>Table of Pipeline Expansion Distances [distance]</t>
-  </si>
-  <si>
-    <t>Table of Pipeline Capacity Expansion Costs [currency/(volume/time)]</t>
-  </si>
-  <si>
-    <t>Water Quality at Production Pads [concentration]</t>
-  </si>
-  <si>
-    <t>Initial Water Quality at Storage [concentration]</t>
-  </si>
-  <si>
-    <t>Initial Water Quality at Completiond Pad Storage [concentration]</t>
-  </si>
-  <si>
     <t>volume</t>
   </si>
   <si>
@@ -1052,12 +936,6 @@
     <t>cm</t>
   </si>
   <si>
-    <t>oil_bbl</t>
-  </si>
-  <si>
-    <t>koil_bbl</t>
-  </si>
-  <si>
     <t>foot</t>
   </si>
   <si>
@@ -1076,9 +954,6 @@
     <t>42 gallons</t>
   </si>
   <si>
-    <t>1000 oil_bbl</t>
-  </si>
-  <si>
     <t>1000 m</t>
   </si>
   <si>
@@ -1094,9 +969,6 @@
     <t>30.44 days</t>
   </si>
   <si>
-    <t>Notes on Units</t>
-  </si>
-  <si>
     <t>ppm</t>
   </si>
   <si>
@@ -1104,6 +976,42 @@
   </si>
   <si>
     <t>kg/liter</t>
+  </si>
+  <si>
+    <t>bbl</t>
+  </si>
+  <si>
+    <t>kbbl</t>
+  </si>
+  <si>
+    <t>1000 bbl</t>
+  </si>
+  <si>
+    <t>Unit Description</t>
+  </si>
+  <si>
+    <t>Unit Relationships</t>
+  </si>
+  <si>
+    <t>Distance units are used for defining lengths of pipelines and pipeline expansion costs</t>
+  </si>
+  <si>
+    <t>This unit applies to diameter of pipelines and pipeline expansion costs</t>
+  </si>
+  <si>
+    <t>Concentration unit defines water quality (e.g., TDS concentration)</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Volume units are used to represent water flows (e.g. bbl/day), flow capacities, storage capacity, costs etc. </t>
+  </si>
+  <si>
+    <t>Currency unit defines costs</t>
+  </si>
+  <si>
+    <t>Time units refers to input data relative to time (e.g., water flows in bbl/day)</t>
+  </si>
+  <si>
+    <t>The decision period is the amount of time in a single decision period or discretization (e.g., T01 is 1 week)</t>
   </si>
 </sst>
 </file>
@@ -1115,7 +1023,7 @@
     <numFmt numFmtId="164" formatCode="#,##0.0"/>
     <numFmt numFmtId="165" formatCode="0.0"/>
   </numFmts>
-  <fonts count="10" x14ac:knownFonts="1">
+  <fonts count="9" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -1180,12 +1088,6 @@
       <name val="Calibri"/>
       <family val="2"/>
       <scheme val="minor"/>
-    </font>
-    <font>
-      <sz val="12"/>
-      <color theme="1"/>
-      <name val="Calibri"/>
-      <family val="2"/>
     </font>
   </fonts>
   <fills count="5">
@@ -1839,7 +1741,6 @@
     <xf numFmtId="3" fontId="1" fillId="3" borderId="24" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="21" xfId="0" applyFont="1" applyBorder="1"/>
     <xf numFmtId="3" fontId="1" fillId="3" borderId="25" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
@@ -1923,7 +1824,10 @@
     <xf numFmtId="0" fontId="1" fillId="4" borderId="35" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="1" fillId="4" borderId="38" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="3" fillId="4" borderId="32" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="4" borderId="38" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
   </cellXfs>
@@ -4090,7 +3994,7 @@
   <dimension ref="A1:T8"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="A6" sqref="A6"/>
+      <selection activeCell="G13" sqref="G13"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9.33203125" defaultRowHeight="15.6" x14ac:dyDescent="0.3"/>
@@ -4257,13 +4161,12 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{5EADE56A-3552-4283-86E6-D2B76E77A8C0}">
   <dimension ref="A1:AD17"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="B3" sqref="B3"/>
-    </sheetView>
+    <sheetView workbookViewId="0"/>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9.33203125" defaultRowHeight="15.6" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="1" max="16384" width="9.33203125" style="1"/>
+    <col min="1" max="1" width="15.5546875" style="1" customWidth="1"/>
+    <col min="2" max="16384" width="9.33203125" style="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:30" ht="16.2" thickBot="1" x14ac:dyDescent="0.35">
@@ -4922,7 +4825,8 @@
   </sheetViews>
   <sheetFormatPr defaultColWidth="9.33203125" defaultRowHeight="15.6" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="1" max="16384" width="9.33203125" style="1"/>
+    <col min="1" max="1" width="16.88671875" style="1" customWidth="1"/>
+    <col min="2" max="16384" width="9.33203125" style="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:30" ht="16.2" thickBot="1" x14ac:dyDescent="0.35">
@@ -5183,7 +5087,8 @@
   </sheetViews>
   <sheetFormatPr defaultColWidth="9.33203125" defaultRowHeight="15.6" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="1" max="16384" width="9.33203125" style="1"/>
+    <col min="1" max="1" width="17.44140625" style="1" customWidth="1"/>
+    <col min="2" max="16384" width="9.33203125" style="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:5" ht="16.2" thickBot="1" x14ac:dyDescent="0.35">
@@ -5331,7 +5236,8 @@
   </sheetViews>
   <sheetFormatPr defaultColWidth="9.33203125" defaultRowHeight="15.6" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="1" max="16384" width="9.33203125" style="1"/>
+    <col min="1" max="1" width="15.33203125" style="1" customWidth="1"/>
+    <col min="2" max="16384" width="9.33203125" style="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:30" ht="16.2" thickBot="1" x14ac:dyDescent="0.35">
@@ -6552,7 +6458,8 @@
   </sheetViews>
   <sheetFormatPr defaultColWidth="9.33203125" defaultRowHeight="15.6" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="1" max="16384" width="9.33203125" style="1"/>
+    <col min="1" max="1" width="15.77734375" style="1" customWidth="1"/>
+    <col min="2" max="16384" width="9.33203125" style="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:5" ht="16.2" thickBot="1" x14ac:dyDescent="0.35">
@@ -6854,7 +6761,8 @@
   </sheetViews>
   <sheetFormatPr defaultColWidth="9.33203125" defaultRowHeight="15.6" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="1" max="16384" width="9.33203125" style="1"/>
+    <col min="1" max="1" width="14.77734375" style="1" customWidth="1"/>
+    <col min="2" max="16384" width="9.33203125" style="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:6" ht="16.2" thickBot="1" x14ac:dyDescent="0.35">
@@ -7203,7 +7111,8 @@
   </sheetViews>
   <sheetFormatPr defaultColWidth="9.33203125" defaultRowHeight="15.6" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="1" max="16384" width="9.33203125" style="1"/>
+    <col min="1" max="1" width="15" style="1" customWidth="1"/>
+    <col min="2" max="16384" width="9.33203125" style="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:3" ht="16.2" thickBot="1" x14ac:dyDescent="0.35">
@@ -7446,7 +7355,8 @@
   </sheetViews>
   <sheetFormatPr defaultColWidth="9.33203125" defaultRowHeight="15.6" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="1" max="16384" width="9.33203125" style="1"/>
+    <col min="1" max="1" width="16" style="1" customWidth="1"/>
+    <col min="2" max="16384" width="9.33203125" style="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:2" ht="16.2" thickBot="1" x14ac:dyDescent="0.35">
@@ -7486,7 +7396,8 @@
   </sheetViews>
   <sheetFormatPr defaultColWidth="9.33203125" defaultRowHeight="15.6" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="1" max="16384" width="9.33203125" style="1"/>
+    <col min="1" max="1" width="13.21875" style="1" customWidth="1"/>
+    <col min="2" max="16384" width="9.33203125" style="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:2" ht="16.2" thickBot="1" x14ac:dyDescent="0.35">
@@ -7526,7 +7437,8 @@
   </sheetViews>
   <sheetFormatPr defaultColWidth="9.33203125" defaultRowHeight="15.6" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="1" max="16384" width="9.33203125" style="1"/>
+    <col min="1" max="1" width="19.77734375" style="1" customWidth="1"/>
+    <col min="2" max="16384" width="9.33203125" style="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:5" ht="16.2" thickBot="1" x14ac:dyDescent="0.35">
@@ -7656,7 +7568,8 @@
   </sheetViews>
   <sheetFormatPr defaultColWidth="9.33203125" defaultRowHeight="15.6" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="1" max="16384" width="9.33203125" style="1"/>
+    <col min="1" max="1" width="15.5546875" style="1" customWidth="1"/>
+    <col min="2" max="16384" width="9.33203125" style="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:5" ht="16.2" thickBot="1" x14ac:dyDescent="0.35">
@@ -7723,7 +7636,8 @@
   </sheetViews>
   <sheetFormatPr defaultColWidth="9.33203125" defaultRowHeight="15.6" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="1" max="16384" width="9.33203125" style="1"/>
+    <col min="1" max="1" width="15.6640625" style="1" customWidth="1"/>
+    <col min="2" max="16384" width="9.33203125" style="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:3" ht="16.2" thickBot="1" x14ac:dyDescent="0.35">
@@ -7772,7 +7686,8 @@
   </sheetViews>
   <sheetFormatPr defaultColWidth="9.33203125" defaultRowHeight="15.6" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="1" max="16384" width="9.33203125" style="1"/>
+    <col min="1" max="1" width="15.44140625" style="1" customWidth="1"/>
+    <col min="2" max="16384" width="9.33203125" style="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:5" ht="16.2" thickBot="1" x14ac:dyDescent="0.35">
@@ -7941,302 +7856,327 @@
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{6FEB10CD-C2F5-4A5B-9D35-9BA20FBC12B6}">
-  <dimension ref="A1:AY12"/>
+  <dimension ref="A1:AZ12"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0"/>
+    <sheetView tabSelected="1" zoomScale="120" zoomScaleNormal="120" workbookViewId="0"/>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9.33203125" defaultRowHeight="15.6" x14ac:dyDescent="0.3"/>
   <cols>
     <col min="1" max="1" width="16.88671875" style="1" customWidth="1"/>
     <col min="2" max="2" width="13.109375" style="1" customWidth="1"/>
     <col min="3" max="3" width="9.33203125" style="1"/>
-    <col min="4" max="4" width="8.44140625" style="1" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="2.21875" style="1" bestFit="1" customWidth="1"/>
-    <col min="6" max="6" width="12.44140625" style="1" bestFit="1" customWidth="1"/>
-    <col min="7" max="7" width="0.77734375" style="1" customWidth="1"/>
-    <col min="8" max="8" width="8.44140625" style="1" bestFit="1" customWidth="1"/>
-    <col min="9" max="9" width="2.21875" style="1" bestFit="1" customWidth="1"/>
-    <col min="10" max="10" width="12.44140625" style="1" bestFit="1" customWidth="1"/>
-    <col min="11" max="47" width="9.33203125" style="1"/>
-    <col min="48" max="48" width="13.88671875" style="1" bestFit="1" customWidth="1"/>
-    <col min="49" max="49" width="9.21875" style="1" bestFit="1" customWidth="1"/>
-    <col min="50" max="50" width="6.21875" style="1" bestFit="1" customWidth="1"/>
-    <col min="51" max="51" width="15.5546875" style="1" bestFit="1" customWidth="1"/>
-    <col min="52" max="16384" width="9.33203125" style="1"/>
+    <col min="4" max="4" width="92.5546875" style="1" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="8.44140625" style="1" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="2.21875" style="1" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="12.44140625" style="1" bestFit="1" customWidth="1"/>
+    <col min="8" max="8" width="0.77734375" style="1" customWidth="1"/>
+    <col min="9" max="9" width="8.44140625" style="1" bestFit="1" customWidth="1"/>
+    <col min="10" max="10" width="2.21875" style="1" bestFit="1" customWidth="1"/>
+    <col min="11" max="11" width="12.44140625" style="1" bestFit="1" customWidth="1"/>
+    <col min="12" max="48" width="9.33203125" style="1"/>
+    <col min="49" max="49" width="13.88671875" style="1" bestFit="1" customWidth="1"/>
+    <col min="50" max="50" width="9.21875" style="1" bestFit="1" customWidth="1"/>
+    <col min="51" max="51" width="6.21875" style="1" bestFit="1" customWidth="1"/>
+    <col min="52" max="52" width="15.5546875" style="1" bestFit="1" customWidth="1"/>
+    <col min="53" max="16384" width="9.33203125" style="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:51" ht="16.2" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="1" spans="1:52" ht="16.2" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A1" s="1" t="s">
-        <v>292</v>
-      </c>
-    </row>
-    <row r="2" spans="1:51" s="9" customFormat="1" x14ac:dyDescent="0.3">
+        <v>260</v>
+      </c>
+    </row>
+    <row r="2" spans="1:52" s="9" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A2" s="7" t="s">
         <v>244</v>
       </c>
       <c r="B2" s="28" t="s">
         <v>228</v>
       </c>
-      <c r="D2" s="98" t="s">
-        <v>313</v>
-      </c>
-      <c r="E2" s="91"/>
-      <c r="F2" s="91"/>
-      <c r="G2" s="92"/>
+      <c r="D2" s="97" t="s">
+        <v>284</v>
+      </c>
+      <c r="E2" s="98" t="s">
+        <v>285</v>
+      </c>
+      <c r="F2" s="90"/>
+      <c r="G2" s="90"/>
       <c r="H2" s="91"/>
-      <c r="I2" s="91"/>
-      <c r="J2" s="93"/>
-    </row>
-    <row r="3" spans="1:51" x14ac:dyDescent="0.3">
+      <c r="I2" s="90"/>
+      <c r="J2" s="90"/>
+      <c r="K2" s="92"/>
+    </row>
+    <row r="3" spans="1:52" x14ac:dyDescent="0.3">
       <c r="A3" s="29" t="s">
+        <v>251</v>
+      </c>
+      <c r="B3" s="52" t="s">
+        <v>281</v>
+      </c>
+      <c r="D3" s="85" t="s">
+        <v>289</v>
+      </c>
+      <c r="E3" s="86" t="s">
+        <v>281</v>
+      </c>
+      <c r="F3" s="87" t="s">
+        <v>271</v>
+      </c>
+      <c r="G3" s="80" t="s">
+        <v>272</v>
+      </c>
+      <c r="H3" s="84"/>
+      <c r="I3" s="80" t="s">
+        <v>282</v>
+      </c>
+      <c r="J3" s="87" t="s">
+        <v>271</v>
+      </c>
+      <c r="K3" s="82" t="s">
         <v>283</v>
       </c>
-      <c r="B3" s="52" t="s">
-        <v>299</v>
-      </c>
-      <c r="D3" s="87" t="s">
-        <v>299</v>
-      </c>
-      <c r="E3" s="88" t="s">
-        <v>305</v>
-      </c>
-      <c r="F3" s="81" t="s">
-        <v>306</v>
-      </c>
-      <c r="G3" s="85"/>
-      <c r="H3" s="81" t="s">
-        <v>300</v>
-      </c>
-      <c r="I3" s="88" t="s">
-        <v>305</v>
-      </c>
-      <c r="J3" s="83" t="s">
-        <v>307</v>
-      </c>
-    </row>
-    <row r="4" spans="1:51" x14ac:dyDescent="0.3">
+    </row>
+    <row r="4" spans="1:52" x14ac:dyDescent="0.3">
       <c r="A4" s="29" t="s">
-        <v>284</v>
+        <v>252</v>
       </c>
       <c r="B4" s="52" t="s">
-        <v>285</v>
-      </c>
-      <c r="D4" s="87" t="s">
-        <v>303</v>
-      </c>
-      <c r="E4" s="88" t="s">
-        <v>305</v>
-      </c>
-      <c r="F4" s="81" t="s">
-        <v>308</v>
-      </c>
-      <c r="G4" s="85"/>
-      <c r="H4" s="81"/>
-      <c r="I4" s="81"/>
-      <c r="J4" s="83"/>
-    </row>
-    <row r="5" spans="1:51" x14ac:dyDescent="0.3">
+        <v>253</v>
+      </c>
+      <c r="D4" s="85" t="s">
+        <v>286</v>
+      </c>
+      <c r="E4" s="86" t="s">
+        <v>269</v>
+      </c>
+      <c r="F4" s="87" t="s">
+        <v>271</v>
+      </c>
+      <c r="G4" s="80" t="s">
+        <v>273</v>
+      </c>
+      <c r="H4" s="84"/>
+      <c r="I4" s="80"/>
+      <c r="J4" s="80"/>
+      <c r="K4" s="82"/>
+    </row>
+    <row r="5" spans="1:52" x14ac:dyDescent="0.3">
       <c r="A5" s="29" t="s">
-        <v>296</v>
+        <v>264</v>
       </c>
       <c r="B5" s="52" t="s">
-        <v>297</v>
-      </c>
-      <c r="D5" s="89"/>
-      <c r="E5" s="82"/>
-      <c r="F5" s="82"/>
-      <c r="G5" s="86"/>
-      <c r="H5" s="82"/>
-      <c r="I5" s="82"/>
-      <c r="J5" s="84"/>
-    </row>
-    <row r="6" spans="1:51" x14ac:dyDescent="0.3">
+        <v>265</v>
+      </c>
+      <c r="D5" s="85" t="s">
+        <v>287</v>
+      </c>
+      <c r="E5" s="88"/>
+      <c r="F5" s="81"/>
+      <c r="G5" s="81"/>
+      <c r="H5" s="85"/>
+      <c r="I5" s="81"/>
+      <c r="J5" s="81"/>
+      <c r="K5" s="83"/>
+    </row>
+    <row r="6" spans="1:52" x14ac:dyDescent="0.3">
       <c r="A6" s="29" t="s">
-        <v>286</v>
+        <v>254</v>
       </c>
       <c r="B6" s="52" t="s">
-        <v>315</v>
-      </c>
-      <c r="D6" s="87" t="s">
-        <v>315</v>
-      </c>
-      <c r="E6" s="88" t="s">
-        <v>305</v>
-      </c>
-      <c r="F6" s="81" t="s">
-        <v>314</v>
-      </c>
-      <c r="G6" s="86"/>
-      <c r="H6" s="82"/>
-      <c r="I6" s="82"/>
-      <c r="J6" s="84"/>
-    </row>
-    <row r="7" spans="1:51" x14ac:dyDescent="0.3">
+        <v>279</v>
+      </c>
+      <c r="D6" s="85" t="s">
+        <v>288</v>
+      </c>
+      <c r="E6" s="86" t="s">
+        <v>279</v>
+      </c>
+      <c r="F6" s="87" t="s">
+        <v>271</v>
+      </c>
+      <c r="G6" s="80" t="s">
+        <v>278</v>
+      </c>
+      <c r="H6" s="85"/>
+      <c r="I6" s="81"/>
+      <c r="J6" s="81"/>
+      <c r="K6" s="83"/>
+    </row>
+    <row r="7" spans="1:52" x14ac:dyDescent="0.3">
       <c r="A7" s="29" t="s">
-        <v>287</v>
+        <v>255</v>
       </c>
       <c r="B7" s="52" t="s">
-        <v>288</v>
-      </c>
-      <c r="D7" s="87" t="s">
-        <v>294</v>
-      </c>
-      <c r="E7" s="88" t="s">
-        <v>305</v>
-      </c>
-      <c r="F7" s="81" t="s">
-        <v>311</v>
-      </c>
-      <c r="G7" s="86"/>
-      <c r="H7" s="82"/>
-      <c r="I7" s="82"/>
-      <c r="J7" s="84"/>
-    </row>
-    <row r="8" spans="1:51" x14ac:dyDescent="0.3">
+        <v>256</v>
+      </c>
+      <c r="D7" s="85" t="s">
+        <v>290</v>
+      </c>
+      <c r="E7" s="86" t="s">
+        <v>262</v>
+      </c>
+      <c r="F7" s="87" t="s">
+        <v>271</v>
+      </c>
+      <c r="G7" s="80" t="s">
+        <v>276</v>
+      </c>
+      <c r="H7" s="85"/>
+      <c r="I7" s="81"/>
+      <c r="J7" s="81"/>
+      <c r="K7" s="83"/>
+    </row>
+    <row r="8" spans="1:52" x14ac:dyDescent="0.3">
       <c r="A8" s="29" t="s">
-        <v>289</v>
+        <v>257</v>
       </c>
       <c r="B8" s="52" t="s">
-        <v>293</v>
-      </c>
-      <c r="D8" s="89"/>
-      <c r="E8" s="82"/>
-      <c r="F8" s="82"/>
-      <c r="G8" s="86"/>
-      <c r="H8" s="82"/>
-      <c r="I8" s="82"/>
-      <c r="J8" s="84"/>
-      <c r="AS8" s="33" t="s">
-        <v>283</v>
-      </c>
+        <v>261</v>
+      </c>
+      <c r="D8" s="85" t="s">
+        <v>291</v>
+      </c>
+      <c r="E8" s="88"/>
+      <c r="F8" s="81"/>
+      <c r="G8" s="81"/>
+      <c r="H8" s="85"/>
+      <c r="I8" s="81"/>
+      <c r="J8" s="81"/>
+      <c r="K8" s="83"/>
       <c r="AT8" s="33" t="s">
-        <v>284</v>
+        <v>251</v>
       </c>
       <c r="AU8" s="33" t="s">
-        <v>296</v>
+        <v>252</v>
       </c>
       <c r="AV8" s="33" t="s">
-        <v>286</v>
+        <v>264</v>
       </c>
       <c r="AW8" s="33" t="s">
-        <v>287</v>
+        <v>254</v>
       </c>
       <c r="AX8" s="33" t="s">
-        <v>289</v>
+        <v>255</v>
       </c>
       <c r="AY8" s="33" t="s">
-        <v>291</v>
-      </c>
-    </row>
-    <row r="9" spans="1:51" ht="16.2" thickBot="1" x14ac:dyDescent="0.35">
+        <v>257</v>
+      </c>
+      <c r="AZ8" s="33" t="s">
+        <v>259</v>
+      </c>
+    </row>
+    <row r="9" spans="1:52" ht="16.2" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A9" s="30" t="s">
-        <v>309</v>
+        <v>274</v>
       </c>
       <c r="B9" s="40" t="s">
-        <v>290</v>
-      </c>
-      <c r="D9" s="94" t="s">
-        <v>304</v>
-      </c>
-      <c r="E9" s="95" t="s">
-        <v>305</v>
-      </c>
-      <c r="F9" s="96" t="s">
-        <v>310</v>
-      </c>
-      <c r="G9" s="90"/>
-      <c r="H9" s="97" t="s">
-        <v>295</v>
-      </c>
-      <c r="I9" s="95" t="s">
-        <v>305</v>
-      </c>
-      <c r="J9" s="96" t="s">
-        <v>312</v>
-      </c>
-      <c r="AS9" s="1" t="s">
-        <v>299</v>
+        <v>258</v>
+      </c>
+      <c r="D9" s="89" t="s">
+        <v>292</v>
+      </c>
+      <c r="E9" s="93" t="s">
+        <v>270</v>
+      </c>
+      <c r="F9" s="94" t="s">
+        <v>271</v>
+      </c>
+      <c r="G9" s="95" t="s">
+        <v>275</v>
+      </c>
+      <c r="H9" s="89"/>
+      <c r="I9" s="96" t="s">
+        <v>263</v>
+      </c>
+      <c r="J9" s="94" t="s">
+        <v>271</v>
+      </c>
+      <c r="K9" s="95" t="s">
+        <v>277</v>
       </c>
       <c r="AT9" s="1" t="s">
-        <v>301</v>
+        <v>281</v>
       </c>
       <c r="AU9" s="1" t="s">
-        <v>297</v>
+        <v>267</v>
       </c>
       <c r="AV9" s="1" t="s">
-        <v>315</v>
+        <v>265</v>
       </c>
       <c r="AW9" s="1" t="s">
-        <v>288</v>
+        <v>279</v>
       </c>
       <c r="AX9" s="1" t="s">
-        <v>293</v>
+        <v>256</v>
       </c>
       <c r="AY9" s="1" t="s">
-        <v>293</v>
-      </c>
-    </row>
-    <row r="10" spans="1:51" x14ac:dyDescent="0.3">
-      <c r="AS10" s="1" t="s">
-        <v>300</v>
-      </c>
+        <v>261</v>
+      </c>
+      <c r="AZ9" s="1" t="s">
+        <v>261</v>
+      </c>
+    </row>
+    <row r="10" spans="1:52" x14ac:dyDescent="0.3">
       <c r="AT10" s="1" t="s">
-        <v>285</v>
+        <v>282</v>
       </c>
       <c r="AU10" s="1" t="s">
-        <v>298</v>
+        <v>253</v>
       </c>
       <c r="AV10" s="1" t="s">
-        <v>316</v>
+        <v>266</v>
       </c>
       <c r="AW10" s="1" t="s">
-        <v>294</v>
+        <v>280</v>
       </c>
       <c r="AX10" s="1" t="s">
-        <v>290</v>
+        <v>262</v>
       </c>
       <c r="AY10" s="1" t="s">
-        <v>290</v>
-      </c>
-    </row>
-    <row r="11" spans="1:51" x14ac:dyDescent="0.3">
-      <c r="AT11" s="1" t="s">
-        <v>302</v>
-      </c>
-      <c r="AY11" s="1" t="s">
-        <v>304</v>
-      </c>
-    </row>
-    <row r="12" spans="1:51" x14ac:dyDescent="0.3">
-      <c r="AT12" s="1" t="s">
-        <v>303</v>
-      </c>
-      <c r="AY12" s="1" t="s">
-        <v>295</v>
+        <v>258</v>
+      </c>
+      <c r="AZ10" s="1" t="s">
+        <v>258</v>
+      </c>
+    </row>
+    <row r="11" spans="1:52" x14ac:dyDescent="0.3">
+      <c r="AU11" s="1" t="s">
+        <v>268</v>
+      </c>
+      <c r="AZ11" s="1" t="s">
+        <v>270</v>
+      </c>
+    </row>
+    <row r="12" spans="1:52" x14ac:dyDescent="0.3">
+      <c r="AU12" s="1" t="s">
+        <v>269</v>
+      </c>
+      <c r="AZ12" s="1" t="s">
+        <v>263</v>
       </c>
     </row>
   </sheetData>
   <dataValidations count="7">
     <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="B3" xr:uid="{0366540F-07AE-4F25-B907-A754D6EED801}">
-      <formula1>$AS$9:$AS$10</formula1>
+      <formula1>$AT$9:$AT$10</formula1>
     </dataValidation>
     <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="B4" xr:uid="{C79D4C95-A2FA-4887-96DC-7C746F015FE0}">
-      <formula1>$AT$9:$AT$12</formula1>
+      <formula1>$AU$9:$AU$12</formula1>
     </dataValidation>
     <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="B6" xr:uid="{31C57A55-793D-4314-90EE-3947816FAD7C}">
-      <formula1>$AV$9:$AV$10</formula1>
+      <formula1>$AW$9:$AW$10</formula1>
     </dataValidation>
     <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="B7" xr:uid="{2875C8E3-1AA6-4283-BA6A-B0ED7E3E7451}">
-      <formula1>$AW$9:$AW$10</formula1>
+      <formula1>$AX$9:$AX$10</formula1>
     </dataValidation>
     <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="B8" xr:uid="{A2352212-D4AC-4060-A6D0-EDF0F167C76E}">
-      <formula1>$AX$9:$AX$10</formula1>
+      <formula1>$AY$9:$AY$10</formula1>
     </dataValidation>
     <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="B9" xr:uid="{6A0898C7-A0E4-4D50-B77F-749952BD9BF8}">
-      <formula1>$AY$9:$AY$12</formula1>
+      <formula1>$AZ$9:$AZ$12</formula1>
     </dataValidation>
     <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="B5" xr:uid="{7798E450-1C40-4081-9434-3CDB06544C0F}">
-      <formula1>$AU$9:$AU$10</formula1>
+      <formula1>$AV$9:$AV$10</formula1>
     </dataValidation>
   </dataValidations>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
@@ -8254,7 +8194,8 @@
   </sheetViews>
   <sheetFormatPr defaultColWidth="9.33203125" defaultRowHeight="15.6" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="1" max="16384" width="9.33203125" style="1"/>
+    <col min="1" max="1" width="19.88671875" style="1" customWidth="1"/>
+    <col min="2" max="16384" width="9.33203125" style="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:5" ht="16.2" thickBot="1" x14ac:dyDescent="0.35">
@@ -8383,7 +8324,8 @@
   </sheetViews>
   <sheetFormatPr defaultColWidth="9.33203125" defaultRowHeight="15.6" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="1" max="16384" width="9.33203125" style="1"/>
+    <col min="1" max="1" width="15.44140625" style="1" customWidth="1"/>
+    <col min="2" max="16384" width="9.33203125" style="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:6" ht="16.2" thickBot="1" x14ac:dyDescent="0.35">
@@ -8727,7 +8669,8 @@
   </sheetViews>
   <sheetFormatPr defaultColWidth="9.33203125" defaultRowHeight="15.6" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="1" max="16384" width="9.33203125" style="1"/>
+    <col min="1" max="1" width="17" style="1" customWidth="1"/>
+    <col min="2" max="16384" width="9.33203125" style="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:6" ht="16.2" thickBot="1" x14ac:dyDescent="0.35">
@@ -8851,7 +8794,8 @@
   </sheetViews>
   <sheetFormatPr defaultColWidth="9.33203125" defaultRowHeight="15.6" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="1" max="16384" width="9.33203125" style="1"/>
+    <col min="1" max="1" width="17.6640625" style="1" customWidth="1"/>
+    <col min="2" max="16384" width="9.33203125" style="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:5" ht="16.2" thickBot="1" x14ac:dyDescent="0.35">
@@ -8928,7 +8872,8 @@
   </sheetViews>
   <sheetFormatPr defaultColWidth="9.33203125" defaultRowHeight="15.6" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="1" max="16384" width="9.33203125" style="1"/>
+    <col min="1" max="1" width="16.33203125" style="1" customWidth="1"/>
+    <col min="2" max="16384" width="9.33203125" style="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:2" ht="16.2" thickBot="1" x14ac:dyDescent="0.35">
@@ -8960,18 +8905,22 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{0D6FA210-6C83-4CC4-AF45-F41CDC53F769}">
   <dimension ref="A1:BA17"/>
   <sheetViews>
-    <sheetView showZeros="0" workbookViewId="0"/>
+    <sheetView showZeros="0" workbookViewId="0">
+      <selection activeCell="A2" sqref="A2"/>
+    </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9.33203125" defaultRowHeight="15.6" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="1" max="1" width="9.33203125" style="1"/>
+    <col min="1" max="1" width="16.5546875" style="1" customWidth="1"/>
     <col min="2" max="2" width="11" style="1" bestFit="1" customWidth="1"/>
-    <col min="3" max="16384" width="9.33203125" style="1"/>
+    <col min="3" max="3" width="9.88671875" style="1" bestFit="1" customWidth="1"/>
+    <col min="4" max="16384" width="9.33203125" style="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:53" ht="16.2" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A1" s="1" t="s">
-        <v>260</v>
+      <c r="A1" s="1" t="str">
+        <f>_xlfn.CONCAT( "Table of Completions Water Demand for Completions Sites over ",VLOOKUP("decision period", Units!$A$2:$B$9, 2, FALSE),"s [",VLOOKUP("volume", Units!$A$2:$B$9, 2, FALSE),"/", VLOOKUP("time", Units!$A$2:$B$9, 2, FALSE),"]")</f>
+        <v>Table of Completions Water Demand for Completions Sites over weeks [bbl/day]</v>
       </c>
     </row>
     <row r="2" spans="1:53" s="9" customFormat="1" ht="16.2" thickBot="1" x14ac:dyDescent="0.35">
@@ -9832,222 +9781,16 @@
 </file>
 
 <file path=xl/worksheets/sheet36.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{FF13C221-12DF-4609-BB39-C92B41E7288D}">
-  <dimension ref="A1:B31"/>
-  <sheetViews>
-    <sheetView workbookViewId="0"/>
-  </sheetViews>
-  <sheetFormatPr defaultColWidth="9.33203125" defaultRowHeight="15.6" x14ac:dyDescent="0.3"/>
-  <cols>
-    <col min="1" max="1" width="11" style="1" customWidth="1"/>
-    <col min="2" max="2" width="10.109375" style="1" bestFit="1" customWidth="1"/>
-    <col min="3" max="16384" width="9.33203125" style="1"/>
-  </cols>
-  <sheetData>
-    <row r="1" spans="1:2" ht="16.2" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A1" s="1" t="s">
-        <v>259</v>
-      </c>
-    </row>
-    <row r="2" spans="1:2" s="9" customFormat="1" x14ac:dyDescent="0.3">
-      <c r="A2" s="7" t="s">
-        <v>226</v>
-      </c>
-      <c r="B2" s="28" t="s">
-        <v>228</v>
-      </c>
-    </row>
-    <row r="3" spans="1:2" x14ac:dyDescent="0.3">
-      <c r="A3" s="29" t="s">
-        <v>137</v>
-      </c>
-      <c r="B3" s="38"/>
-    </row>
-    <row r="4" spans="1:2" x14ac:dyDescent="0.3">
-      <c r="A4" s="29" t="s">
-        <v>80</v>
-      </c>
-      <c r="B4" s="38"/>
-    </row>
-    <row r="5" spans="1:2" x14ac:dyDescent="0.3">
-      <c r="A5" s="29" t="s">
-        <v>81</v>
-      </c>
-      <c r="B5" s="38"/>
-    </row>
-    <row r="6" spans="1:2" x14ac:dyDescent="0.3">
-      <c r="A6" s="29" t="s">
-        <v>82</v>
-      </c>
-      <c r="B6" s="38"/>
-    </row>
-    <row r="7" spans="1:2" x14ac:dyDescent="0.3">
-      <c r="A7" s="29" t="s">
-        <v>83</v>
-      </c>
-      <c r="B7" s="38"/>
-    </row>
-    <row r="8" spans="1:2" x14ac:dyDescent="0.3">
-      <c r="A8" s="29" t="s">
-        <v>84</v>
-      </c>
-      <c r="B8" s="38"/>
-    </row>
-    <row r="9" spans="1:2" x14ac:dyDescent="0.3">
-      <c r="A9" s="29" t="s">
-        <v>85</v>
-      </c>
-      <c r="B9" s="38"/>
-    </row>
-    <row r="10" spans="1:2" x14ac:dyDescent="0.3">
-      <c r="A10" s="29" t="s">
-        <v>86</v>
-      </c>
-      <c r="B10" s="38"/>
-    </row>
-    <row r="11" spans="1:2" x14ac:dyDescent="0.3">
-      <c r="A11" s="29" t="s">
-        <v>138</v>
-      </c>
-      <c r="B11" s="38"/>
-    </row>
-    <row r="12" spans="1:2" x14ac:dyDescent="0.3">
-      <c r="A12" s="29" t="s">
-        <v>139</v>
-      </c>
-      <c r="B12" s="38"/>
-    </row>
-    <row r="13" spans="1:2" x14ac:dyDescent="0.3">
-      <c r="A13" s="29" t="s">
-        <v>140</v>
-      </c>
-      <c r="B13" s="38"/>
-    </row>
-    <row r="14" spans="1:2" x14ac:dyDescent="0.3">
-      <c r="A14" s="29" t="s">
-        <v>141</v>
-      </c>
-      <c r="B14" s="38"/>
-    </row>
-    <row r="15" spans="1:2" x14ac:dyDescent="0.3">
-      <c r="A15" s="29" t="s">
-        <v>142</v>
-      </c>
-      <c r="B15" s="38"/>
-    </row>
-    <row r="16" spans="1:2" x14ac:dyDescent="0.3">
-      <c r="A16" s="29" t="s">
-        <v>143</v>
-      </c>
-      <c r="B16" s="38"/>
-    </row>
-    <row r="17" spans="1:2" x14ac:dyDescent="0.3">
-      <c r="A17" s="29" t="s">
-        <v>144</v>
-      </c>
-      <c r="B17" s="38"/>
-    </row>
-    <row r="18" spans="1:2" x14ac:dyDescent="0.3">
-      <c r="A18" s="29" t="s">
-        <v>145</v>
-      </c>
-      <c r="B18" s="38"/>
-    </row>
-    <row r="19" spans="1:2" x14ac:dyDescent="0.3">
-      <c r="A19" s="29" t="s">
-        <v>146</v>
-      </c>
-      <c r="B19" s="38"/>
-    </row>
-    <row r="20" spans="1:2" x14ac:dyDescent="0.3">
-      <c r="A20" s="29" t="s">
-        <v>147</v>
-      </c>
-      <c r="B20" s="38"/>
-    </row>
-    <row r="21" spans="1:2" x14ac:dyDescent="0.3">
-      <c r="A21" s="29" t="s">
-        <v>148</v>
-      </c>
-      <c r="B21" s="38"/>
-    </row>
-    <row r="22" spans="1:2" x14ac:dyDescent="0.3">
-      <c r="A22" s="29" t="s">
-        <v>149</v>
-      </c>
-      <c r="B22" s="38"/>
-    </row>
-    <row r="23" spans="1:2" x14ac:dyDescent="0.3">
-      <c r="A23" s="29" t="s">
-        <v>150</v>
-      </c>
-      <c r="B23" s="38"/>
-    </row>
-    <row r="24" spans="1:2" x14ac:dyDescent="0.3">
-      <c r="A24" s="29" t="s">
-        <v>151</v>
-      </c>
-      <c r="B24" s="38"/>
-    </row>
-    <row r="25" spans="1:2" x14ac:dyDescent="0.3">
-      <c r="A25" s="29" t="s">
-        <v>152</v>
-      </c>
-      <c r="B25" s="38"/>
-    </row>
-    <row r="26" spans="1:2" x14ac:dyDescent="0.3">
-      <c r="A26" s="29" t="s">
-        <v>153</v>
-      </c>
-      <c r="B26" s="38"/>
-    </row>
-    <row r="27" spans="1:2" x14ac:dyDescent="0.3">
-      <c r="A27" s="29" t="s">
-        <v>154</v>
-      </c>
-      <c r="B27" s="38"/>
-    </row>
-    <row r="28" spans="1:2" x14ac:dyDescent="0.3">
-      <c r="A28" s="29" t="s">
-        <v>155</v>
-      </c>
-      <c r="B28" s="38"/>
-    </row>
-    <row r="29" spans="1:2" x14ac:dyDescent="0.3">
-      <c r="A29" s="29" t="s">
-        <v>156</v>
-      </c>
-      <c r="B29" s="38"/>
-    </row>
-    <row r="30" spans="1:2" x14ac:dyDescent="0.3">
-      <c r="A30" s="29" t="s">
-        <v>157</v>
-      </c>
-      <c r="B30" s="38"/>
-    </row>
-    <row r="31" spans="1:2" ht="16.2" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A31" s="30" t="s">
-        <v>158</v>
-      </c>
-      <c r="B31" s="40"/>
-    </row>
-  </sheetData>
-  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <pageSetup orientation="portrait" r:id="rId1"/>
-</worksheet>
-</file>
-
-<file path=xl/worksheets/sheet37.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{81EF4E1D-6CE0-4F02-8B9E-F2818C0A814C}">
   <dimension ref="A1:BA18"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="C3" sqref="C3"/>
+      <selection activeCell="A2" sqref="A2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9.33203125" defaultRowHeight="15.6" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="1" max="1" width="9.33203125" style="9"/>
+    <col min="1" max="1" width="15.77734375" style="9" customWidth="1"/>
     <col min="2" max="2" width="9.33203125" style="1"/>
     <col min="3" max="3" width="14.33203125" style="1" bestFit="1" customWidth="1"/>
     <col min="4" max="5" width="10.109375" style="1" bestFit="1" customWidth="1"/>
@@ -10055,8 +9798,9 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:53" ht="16.2" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A1" s="31" t="s">
-        <v>261</v>
+      <c r="A1" s="1" t="str">
+        <f>_xlfn.CONCAT( "Table of Production Rate Forecasts by Pads [",VLOOKUP("volume", Units!$A$2:$B$9, 2, FALSE),"/", VLOOKUP("time", Units!$A$2:$B$9, 2, FALSE),"]")</f>
+        <v>Table of Production Rate Forecasts by Pads [bbl/day]</v>
       </c>
     </row>
     <row r="2" spans="1:53" s="9" customFormat="1" x14ac:dyDescent="0.3">
@@ -13416,8 +13160,8 @@
       </c>
     </row>
     <row r="18" spans="1:53" x14ac:dyDescent="0.3">
-      <c r="B18" s="64"/>
-      <c r="C18" s="65"/>
+      <c r="B18" s="63"/>
+      <c r="C18" s="64"/>
       <c r="D18" s="2"/>
       <c r="E18" s="2"/>
       <c r="F18" s="2"/>
@@ -13429,17 +13173,17 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet38.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet37.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{68666333-AE69-4574-92B2-6BE3A00DF612}">
   <dimension ref="A1:BA14"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="I13" sqref="I13"/>
+      <selection activeCell="A2" sqref="A2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9.33203125" defaultRowHeight="15.6" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="1" max="1" width="9.33203125" style="9"/>
+    <col min="1" max="1" width="17.109375" style="9" customWidth="1"/>
     <col min="2" max="13" width="9.33203125" style="1"/>
     <col min="14" max="15" width="11.33203125" style="1" bestFit="1" customWidth="1"/>
     <col min="16" max="23" width="10.109375" style="1" bestFit="1" customWidth="1"/>
@@ -13447,8 +13191,9 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:53" ht="16.2" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A1" s="31" t="s">
-        <v>262</v>
+      <c r="A1" s="1" t="str">
+        <f>_xlfn.CONCAT( "Table of Flowback Rate Forecasts by Pads [",VLOOKUP("volume", Units!$A$2:$B$9, 2, FALSE),"/", VLOOKUP("time", Units!$A$2:$B$9, 2, FALSE),"]")</f>
+        <v>Table of Flowback Rate Forecasts by Pads [bbl/day]</v>
       </c>
     </row>
     <row r="2" spans="1:53" s="9" customFormat="1" x14ac:dyDescent="0.3">
@@ -13793,11 +13538,11 @@
       <c r="A4" s="29" t="s">
         <v>122</v>
       </c>
-      <c r="B4" s="66"/>
-      <c r="C4" s="66"/>
-      <c r="D4" s="66"/>
-      <c r="E4" s="66"/>
-      <c r="F4" s="66"/>
+      <c r="B4" s="65"/>
+      <c r="C4" s="65"/>
+      <c r="D4" s="65"/>
+      <c r="E4" s="65"/>
+      <c r="F4" s="65"/>
       <c r="G4" s="45"/>
       <c r="H4" s="45"/>
       <c r="I4" s="45"/>
@@ -13898,11 +13643,11 @@
       <c r="A5" s="29" t="s">
         <v>123</v>
       </c>
-      <c r="B5" s="66"/>
-      <c r="C5" s="66"/>
-      <c r="D5" s="66"/>
-      <c r="E5" s="66"/>
-      <c r="F5" s="66"/>
+      <c r="B5" s="65"/>
+      <c r="C5" s="65"/>
+      <c r="D5" s="65"/>
+      <c r="E5" s="65"/>
+      <c r="F5" s="65"/>
       <c r="G5" s="45"/>
       <c r="H5" s="45"/>
       <c r="I5" s="45"/>
@@ -14149,12 +13894,221 @@
 </worksheet>
 </file>
 
+<file path=xl/worksheets/sheet38.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{FF13C221-12DF-4609-BB39-C92B41E7288D}">
+  <dimension ref="A1:B31"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="A2" sqref="A2"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultColWidth="9.33203125" defaultRowHeight="15.6" x14ac:dyDescent="0.3"/>
+  <cols>
+    <col min="1" max="1" width="11" style="1" customWidth="1"/>
+    <col min="2" max="2" width="10.109375" style="1" bestFit="1" customWidth="1"/>
+    <col min="3" max="16384" width="9.33203125" style="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:2" ht="16.2" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="A1" s="1" t="str">
+        <f>_xlfn.CONCAT( "Table of Node Capacity Capacity [",VLOOKUP("volume", Units!$A$2:$B$9, 2, FALSE),"/", VLOOKUP("time", Units!$A$2:$B$9, 2, FALSE),"]", " *absence of node or empty cell signifies no max capacity")</f>
+        <v>Table of Node Capacity Capacity [bbl/day] *absence of node or empty cell signifies no max capacity</v>
+      </c>
+    </row>
+    <row r="2" spans="1:2" s="9" customFormat="1" x14ac:dyDescent="0.3">
+      <c r="A2" s="7" t="s">
+        <v>226</v>
+      </c>
+      <c r="B2" s="28" t="s">
+        <v>228</v>
+      </c>
+    </row>
+    <row r="3" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A3" s="29" t="s">
+        <v>137</v>
+      </c>
+      <c r="B3" s="38"/>
+    </row>
+    <row r="4" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A4" s="29" t="s">
+        <v>80</v>
+      </c>
+      <c r="B4" s="38"/>
+    </row>
+    <row r="5" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A5" s="29" t="s">
+        <v>81</v>
+      </c>
+      <c r="B5" s="38"/>
+    </row>
+    <row r="6" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A6" s="29" t="s">
+        <v>82</v>
+      </c>
+      <c r="B6" s="38"/>
+    </row>
+    <row r="7" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A7" s="29" t="s">
+        <v>83</v>
+      </c>
+      <c r="B7" s="38"/>
+    </row>
+    <row r="8" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A8" s="29" t="s">
+        <v>84</v>
+      </c>
+      <c r="B8" s="38"/>
+    </row>
+    <row r="9" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A9" s="29" t="s">
+        <v>85</v>
+      </c>
+      <c r="B9" s="38"/>
+    </row>
+    <row r="10" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A10" s="29" t="s">
+        <v>86</v>
+      </c>
+      <c r="B10" s="38"/>
+    </row>
+    <row r="11" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A11" s="29" t="s">
+        <v>138</v>
+      </c>
+      <c r="B11" s="38"/>
+    </row>
+    <row r="12" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A12" s="29" t="s">
+        <v>139</v>
+      </c>
+      <c r="B12" s="38"/>
+    </row>
+    <row r="13" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A13" s="29" t="s">
+        <v>140</v>
+      </c>
+      <c r="B13" s="38"/>
+    </row>
+    <row r="14" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A14" s="29" t="s">
+        <v>141</v>
+      </c>
+      <c r="B14" s="38"/>
+    </row>
+    <row r="15" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A15" s="29" t="s">
+        <v>142</v>
+      </c>
+      <c r="B15" s="38"/>
+    </row>
+    <row r="16" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A16" s="29" t="s">
+        <v>143</v>
+      </c>
+      <c r="B16" s="38"/>
+    </row>
+    <row r="17" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A17" s="29" t="s">
+        <v>144</v>
+      </c>
+      <c r="B17" s="38"/>
+    </row>
+    <row r="18" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A18" s="29" t="s">
+        <v>145</v>
+      </c>
+      <c r="B18" s="38"/>
+    </row>
+    <row r="19" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A19" s="29" t="s">
+        <v>146</v>
+      </c>
+      <c r="B19" s="38"/>
+    </row>
+    <row r="20" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A20" s="29" t="s">
+        <v>147</v>
+      </c>
+      <c r="B20" s="38"/>
+    </row>
+    <row r="21" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A21" s="29" t="s">
+        <v>148</v>
+      </c>
+      <c r="B21" s="38"/>
+    </row>
+    <row r="22" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A22" s="29" t="s">
+        <v>149</v>
+      </c>
+      <c r="B22" s="38"/>
+    </row>
+    <row r="23" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A23" s="29" t="s">
+        <v>150</v>
+      </c>
+      <c r="B23" s="38"/>
+    </row>
+    <row r="24" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A24" s="29" t="s">
+        <v>151</v>
+      </c>
+      <c r="B24" s="38"/>
+    </row>
+    <row r="25" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A25" s="29" t="s">
+        <v>152</v>
+      </c>
+      <c r="B25" s="38"/>
+    </row>
+    <row r="26" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A26" s="29" t="s">
+        <v>153</v>
+      </c>
+      <c r="B26" s="38"/>
+    </row>
+    <row r="27" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A27" s="29" t="s">
+        <v>154</v>
+      </c>
+      <c r="B27" s="38"/>
+    </row>
+    <row r="28" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A28" s="29" t="s">
+        <v>155</v>
+      </c>
+      <c r="B28" s="38"/>
+    </row>
+    <row r="29" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A29" s="29" t="s">
+        <v>156</v>
+      </c>
+      <c r="B29" s="38"/>
+    </row>
+    <row r="30" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A30" s="29" t="s">
+        <v>157</v>
+      </c>
+      <c r="B30" s="38"/>
+    </row>
+    <row r="31" spans="1:2" ht="16.2" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="A31" s="30" t="s">
+        <v>158</v>
+      </c>
+      <c r="B31" s="40"/>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup orientation="portrait" r:id="rId1"/>
+</worksheet>
+</file>
+
 <file path=xl/worksheets/sheet39.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{9AE628BF-A05C-42C8-8EC7-63FF3B624ADC}">
   <dimension ref="A1:U26"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="B3" sqref="B3:U26"/>
+    <sheetView showZeros="0" workbookViewId="0">
+      <selection activeCell="A2" sqref="A2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9.33203125" defaultRowHeight="15.6" x14ac:dyDescent="0.3"/>
@@ -14163,8 +14117,9 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:21" ht="16.2" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A1" s="2" t="s">
-        <v>263</v>
+      <c r="A1" s="1" t="str">
+        <f>_xlfn.CONCAT( "Table of Initial Pipeline Capacity between Sites  [",VLOOKUP("volume", Units!$A$2:$B$9, 2, FALSE),"/", VLOOKUP("time", Units!$A$2:$B$9, 2, FALSE),"]")</f>
+        <v>Table of Initial Pipeline Capacity between Sites  [bbl/day]</v>
       </c>
       <c r="B1" s="2"/>
       <c r="C1" s="2"/>
@@ -15959,18 +15914,18 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{50D65BC4-7454-4A45-AA93-771B11A13108}">
   <dimension ref="A1:B7"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="C3" sqref="C3"/>
-    </sheetView>
+    <sheetView workbookViewId="0"/>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9.33203125" defaultRowHeight="15.6" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="1" max="16384" width="9.33203125" style="1"/>
+    <col min="1" max="1" width="12.109375" style="1" customWidth="1"/>
+    <col min="2" max="16384" width="9.33203125" style="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:2" ht="16.2" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A1" s="1" t="s">
-        <v>264</v>
+      <c r="A1" s="1" t="str">
+        <f>_xlfn.CONCAT( "Table of Initial Disposal Capacity  [",VLOOKUP("volume", Units!$A$2:$B$9, 2, FALSE),"/", VLOOKUP("time", Units!$A$2:$B$9, 2, FALSE),"]")</f>
+        <v>Table of Initial Disposal Capacity  [bbl/day]</v>
       </c>
     </row>
     <row r="2" spans="1:2" s="9" customFormat="1" x14ac:dyDescent="0.3">
@@ -16017,7 +15972,7 @@
       <c r="A7" s="30" t="s">
         <v>127</v>
       </c>
-      <c r="B7" s="63">
+      <c r="B7" s="62">
         <v>0</v>
       </c>
     </row>
@@ -16035,12 +15990,14 @@
   </sheetViews>
   <sheetFormatPr defaultColWidth="9.33203125" defaultRowHeight="15.6" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="1" max="16384" width="9.33203125" style="1"/>
+    <col min="1" max="1" width="12.33203125" style="1" customWidth="1"/>
+    <col min="2" max="16384" width="9.33203125" style="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:2" ht="16.2" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A1" s="1" t="s">
-        <v>271</v>
+      <c r="A1" s="1" t="str">
+        <f>_xlfn.CONCAT( "Table of Initial Storage Capacity [",VLOOKUP("volume", Units!$A$2:$B$9, 2, FALSE),"]")</f>
+        <v>Table of Initial Storage Capacity [bbl]</v>
       </c>
     </row>
     <row r="2" spans="1:2" s="9" customFormat="1" x14ac:dyDescent="0.3">
@@ -16069,18 +16026,18 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{09A13F53-E3AE-452E-A1A1-316A2C800322}">
   <dimension ref="A1:B4"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="G7" sqref="G7"/>
-    </sheetView>
+    <sheetView workbookViewId="0"/>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9.33203125" defaultRowHeight="15.6" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="1" max="16384" width="9.33203125" style="1"/>
+    <col min="1" max="1" width="14.88671875" style="1" customWidth="1"/>
+    <col min="2" max="16384" width="9.33203125" style="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:2" ht="16.2" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A1" s="1" t="s">
-        <v>265</v>
+      <c r="A1" s="1" t="str">
+        <f>_xlfn.CONCAT( "Table of Initial Treatment Capacity [",VLOOKUP("volume", Units!$A$2:$B$9, 2, FALSE),"/", VLOOKUP("time", Units!$A$2:$B$9, 2, FALSE),"]")</f>
+        <v>Table of Initial Treatment Capacity [bbl/day]</v>
       </c>
     </row>
     <row r="2" spans="1:2" s="9" customFormat="1" x14ac:dyDescent="0.3">
@@ -16103,7 +16060,7 @@
       <c r="A4" s="30" t="s">
         <v>135</v>
       </c>
-      <c r="B4" s="63">
+      <c r="B4" s="62">
         <v>7142.8571428571431</v>
       </c>
     </row>
@@ -16117,18 +16074,18 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{F4A2DBF7-A8C0-4CE1-BE66-F8E077B6F0F1}">
   <dimension ref="A1:BA21"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="G24" sqref="G24"/>
-    </sheetView>
+    <sheetView workbookViewId="0"/>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9.33203125" defaultRowHeight="15.6" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="1" max="16384" width="9.33203125" style="1"/>
+    <col min="1" max="1" width="19.109375" style="1" customWidth="1"/>
+    <col min="2" max="16384" width="9.33203125" style="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:53" ht="16.2" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A1" s="1" t="s">
-        <v>266</v>
+      <c r="A1" s="1" t="str">
+        <f>_xlfn.CONCAT( "Table of Freshwater Sourcing Availability [",VLOOKUP("volume", Units!$A$2:$B$9, 2, FALSE),"/", VLOOKUP("time", Units!$A$2:$B$9, 2, FALSE),"]")</f>
+        <v>Table of Freshwater Sourcing Availability [bbl/day]</v>
       </c>
     </row>
     <row r="2" spans="1:53" s="9" customFormat="1" x14ac:dyDescent="0.3">
@@ -17638,19 +17595,20 @@
   <dimension ref="A1:B6"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="A2" sqref="A2"/>
+      <selection activeCell="H18" sqref="H18"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9.33203125" defaultRowHeight="15.6" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="1" max="1" width="9.33203125" style="1"/>
+    <col min="1" max="1" width="16.88671875" style="1" customWidth="1"/>
     <col min="2" max="2" width="10.109375" style="1" bestFit="1" customWidth="1"/>
     <col min="3" max="16384" width="9.33203125" style="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:2" ht="16.2" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A1" s="1" t="s">
-        <v>272</v>
+      <c r="A1" s="1" t="str">
+        <f>_xlfn.CONCAT( "Table of Completions Pad Storage Capacity [",VLOOKUP("volume", Units!$A$2:$B$9, 2, FALSE),"]")</f>
+        <v>Table of Completions Pad Storage Capacity [bbl]</v>
       </c>
     </row>
     <row r="2" spans="1:2" s="9" customFormat="1" x14ac:dyDescent="0.3">
@@ -17703,18 +17661,18 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{F216C6A0-7BAD-498F-AAE7-F43EE79415DD}">
   <dimension ref="A1:B3"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="M39" sqref="M39"/>
-    </sheetView>
+    <sheetView workbookViewId="0"/>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9.33203125" defaultRowHeight="15.6" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="1" max="16384" width="9.33203125" style="1"/>
+    <col min="1" max="1" width="17.5546875" style="1" customWidth="1"/>
+    <col min="2" max="16384" width="9.33203125" style="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:2" ht="16.2" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A1" s="1" t="s">
-        <v>267</v>
+      <c r="A1" s="1" t="str">
+        <f>_xlfn.CONCAT( "Table of Pad Offloading Capacity  [",VLOOKUP("volume", Units!$A$2:$B$9, 2, FALSE),"/", VLOOKUP("time", Units!$A$2:$B$9, 2, FALSE),"]")</f>
+        <v>Table of Pad Offloading Capacity  [bbl/day]</v>
       </c>
     </row>
     <row r="2" spans="1:2" s="9" customFormat="1" x14ac:dyDescent="0.3">
@@ -17744,7 +17702,7 @@
   <dimension ref="A1:F20"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="A3" sqref="A3:F5"/>
+      <selection activeCell="A2" sqref="A2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9.33203125" defaultRowHeight="15.6" x14ac:dyDescent="0.3"/>
@@ -17961,12 +17919,14 @@
   </sheetViews>
   <sheetFormatPr defaultColWidth="9.33203125" defaultRowHeight="15.6" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="1" max="16384" width="9.33203125" style="1"/>
+    <col min="1" max="1" width="11.88671875" style="1" customWidth="1"/>
+    <col min="2" max="16384" width="9.33203125" style="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:2" ht="16.2" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A1" s="1" t="s">
-        <v>253</v>
+      <c r="A1" s="1" t="str">
+        <f>_xlfn.CONCAT( "Table of Disposal Operational Cost [",VLOOKUP("currency", Units!$A$2:$B$9, 2, FALSE),"/", VLOOKUP("volume", Units!$A$2:$B$9, 2, FALSE),"]")</f>
+        <v>Table of Disposal Operational Cost [USD/bbl]</v>
       </c>
     </row>
     <row r="2" spans="1:2" s="9" customFormat="1" x14ac:dyDescent="0.3">
@@ -18028,18 +17988,18 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{E7050C77-5C7B-4C97-8F2B-C60EA6AF1AED}">
   <dimension ref="A1:B4"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="B5" sqref="B5"/>
-    </sheetView>
+    <sheetView workbookViewId="0"/>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9.33203125" defaultRowHeight="15.6" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="1" max="16384" width="9.33203125" style="1"/>
+    <col min="1" max="1" width="15.5546875" style="1" customWidth="1"/>
+    <col min="2" max="16384" width="9.33203125" style="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:2" ht="16.2" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A1" s="1" t="s">
-        <v>254</v>
+      <c r="A1" s="1" t="str">
+        <f>_xlfn.CONCAT( "Table of Treatment Operational Cost [",VLOOKUP("currency", Units!$A$2:$B$9, 2, FALSE),"/", VLOOKUP("volume", Units!$A$2:$B$9, 2, FALSE),"]")</f>
+        <v>Table of Treatment Operational Cost [USD/bbl]</v>
       </c>
     </row>
     <row r="2" spans="1:2" s="9" customFormat="1" x14ac:dyDescent="0.3">
@@ -18082,12 +18042,14 @@
   </sheetViews>
   <sheetFormatPr defaultColWidth="9.33203125" defaultRowHeight="15.6" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="1" max="16384" width="9.33203125" style="1"/>
+    <col min="1" max="1" width="17.21875" style="1" customWidth="1"/>
+    <col min="2" max="16384" width="9.33203125" style="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:2" ht="16.2" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A1" s="1" t="s">
-        <v>255</v>
+      <c r="A1" s="1" t="str">
+        <f>_xlfn.CONCAT( "Table of Reuse Operational Cost [",VLOOKUP("currency", Units!$A$2:$B$9, 2, FALSE),"/", VLOOKUP("volume", Units!$A$2:$B$9, 2, FALSE),"]")</f>
+        <v>Table of Reuse Operational Cost [USD/bbl]</v>
       </c>
     </row>
     <row r="2" spans="1:2" s="9" customFormat="1" x14ac:dyDescent="0.3">
@@ -18323,7 +18285,7 @@
   <dimension ref="A1:G10"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="G7" sqref="G7"/>
+      <selection activeCell="A2" sqref="A2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9.33203125" defaultRowHeight="15.6" x14ac:dyDescent="0.3"/>
@@ -18334,8 +18296,9 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:7" ht="16.2" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A1" s="1" t="s">
-        <v>256</v>
+      <c r="A1" s="1" t="str">
+        <f>_xlfn.CONCAT( "Table of Pipeline Operational Cost between Sites [",VLOOKUP("currency", Units!$A$2:$B$9, 2, FALSE),"/", VLOOKUP("volume", Units!$A$2:$B$9, 2, FALSE),"]")</f>
+        <v>Table of Pipeline Operational Cost between Sites [USD/bbl]</v>
       </c>
     </row>
     <row r="2" spans="1:7" x14ac:dyDescent="0.3">
@@ -18468,18 +18431,18 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{61B9AF2E-9304-4DC1-ABFA-7D5DAA6BA0BC}">
   <dimension ref="A1:B10"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="A2" sqref="A2"/>
-    </sheetView>
+    <sheetView workbookViewId="0"/>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9.33203125" defaultRowHeight="15.6" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="1" max="16384" width="9.33203125" style="1"/>
+    <col min="1" max="1" width="18" style="1" customWidth="1"/>
+    <col min="2" max="16384" width="9.33203125" style="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:2" ht="16.2" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A1" s="1" t="s">
-        <v>257</v>
+      <c r="A1" s="1" t="str">
+        <f>_xlfn.CONCAT( "Table of Freshwater Souring Cost [",VLOOKUP("currency", Units!$A$2:$B$9, 2, FALSE),"/", VLOOKUP("volume", Units!$A$2:$B$9, 2, FALSE),"]")</f>
+        <v>Table of Freshwater Souring Cost [USD/bbl]</v>
       </c>
     </row>
     <row r="2" spans="1:2" s="9" customFormat="1" x14ac:dyDescent="0.3">
@@ -18564,9 +18527,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{35585569-7889-4883-A327-3B12D4AB6358}">
   <dimension ref="A1:B23"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="E23" sqref="E23"/>
-    </sheetView>
+    <sheetView workbookViewId="0"/>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9.33203125" defaultRowHeight="15.6" x14ac:dyDescent="0.3"/>
   <cols>
@@ -18574,8 +18535,9 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:2" ht="16.2" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A1" s="1" t="s">
-        <v>252</v>
+      <c r="A1" s="1" t="str">
+        <f>_xlfn.CONCAT( "Table of Trucking Hourly Cost [",VLOOKUP("currency", Units!$A$2:$B$9, 2, FALSE),"/", "hour","]")</f>
+        <v>Table of Trucking Hourly Cost [USD/hour]</v>
       </c>
     </row>
     <row r="2" spans="1:2" s="9" customFormat="1" x14ac:dyDescent="0.3">
@@ -18765,16 +18727,20 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{805632D3-BD42-4D5C-8C0F-68DF124ED3E8}">
   <dimension ref="A1:B8"/>
   <sheetViews>
-    <sheetView workbookViewId="0"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="A2" sqref="A2"/>
+    </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9.33203125" defaultRowHeight="15.6" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="1" max="16384" width="9.33203125" style="1"/>
+    <col min="1" max="1" width="18" style="1" customWidth="1"/>
+    <col min="2" max="16384" width="9.33203125" style="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:2" ht="16.2" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A1" s="1" t="s">
-        <v>274</v>
+      <c r="A1" s="1" t="str">
+        <f>_xlfn.CONCAT( "Table of Pipeline Diameters [",VLOOKUP("diameter", Units!$A$2:$B$9, 2, FALSE),"]")</f>
+        <v>Table of Pipeline Diameters [inch]</v>
       </c>
     </row>
     <row r="2" spans="1:2" x14ac:dyDescent="0.3">
@@ -18843,18 +18809,18 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{982C988E-F277-4EB8-BD08-045871CAA4ED}">
   <dimension ref="A1:B6"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="E7" sqref="E7"/>
-    </sheetView>
+    <sheetView workbookViewId="0"/>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9.33203125" defaultRowHeight="15.6" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="1" max="16384" width="9.33203125" style="1"/>
+    <col min="1" max="1" width="19" style="1" customWidth="1"/>
+    <col min="2" max="16384" width="9.33203125" style="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:2" ht="16.2" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A1" s="1" t="s">
-        <v>268</v>
+      <c r="A1" s="1" t="str">
+        <f>_xlfn.CONCAT( "Table of Disposal Capacity Expansion Increments  [",VLOOKUP("volume", Units!$A$2:$B$9, 2, FALSE),"/", VLOOKUP("time", Units!$A$2:$B$9, 2, FALSE),"]")</f>
+        <v>Table of Disposal Capacity Expansion Increments  [bbl/day]</v>
       </c>
     </row>
     <row r="2" spans="1:2" x14ac:dyDescent="0.3">
@@ -18893,7 +18859,7 @@
       <c r="A6" s="30" t="s">
         <v>185</v>
       </c>
-      <c r="B6" s="63">
+      <c r="B6" s="62">
         <v>50000</v>
       </c>
     </row>
@@ -18907,18 +18873,18 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{52F26805-7F3D-4935-8D0C-80B2E9E9F409}">
   <dimension ref="A1:B6"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="A2" sqref="A2"/>
-    </sheetView>
+    <sheetView workbookViewId="0"/>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9.33203125" defaultRowHeight="15.6" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="1" max="16384" width="9.33203125" style="1"/>
+    <col min="1" max="1" width="18.21875" style="1" customWidth="1"/>
+    <col min="2" max="16384" width="9.33203125" style="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:2" ht="16.2" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A1" s="1" t="s">
-        <v>273</v>
+      <c r="A1" s="1" t="str">
+        <f>_xlfn.CONCAT( "Table of Storage Capacity Expansion Increments [",VLOOKUP("volume", Units!$A$2:$B$9, 2, FALSE),"]")</f>
+        <v>Table of Storage Capacity Expansion Increments [bbl]</v>
       </c>
     </row>
     <row r="2" spans="1:2" x14ac:dyDescent="0.3">
@@ -18977,12 +18943,14 @@
   </sheetViews>
   <sheetFormatPr defaultColWidth="9.33203125" defaultRowHeight="15.6" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="1" max="16384" width="9.33203125" style="1"/>
+    <col min="1" max="1" width="21.5546875" style="1" customWidth="1"/>
+    <col min="2" max="16384" width="9.33203125" style="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:2" ht="16.2" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A1" s="62" t="s">
-        <v>269</v>
+      <c r="A1" s="1" t="str">
+        <f>_xlfn.CONCAT( "Table of Treatment Capacity Expansion Increments  [",VLOOKUP("volume", Units!$A$2:$B$9, 2, FALSE),"/", VLOOKUP("time", Units!$A$2:$B$9, 2, FALSE),"]")</f>
+        <v>Table of Treatment Capacity Expansion Increments  [bbl/day]</v>
       </c>
     </row>
     <row r="2" spans="1:2" x14ac:dyDescent="0.3">
@@ -19021,7 +18989,7 @@
       <c r="A6" s="30" t="s">
         <v>225</v>
       </c>
-      <c r="B6" s="63">
+      <c r="B6" s="62">
         <v>35714.285714285717</v>
       </c>
     </row>
@@ -19036,12 +19004,13 @@
   <dimension ref="A1:B4"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="C8" sqref="C8"/>
+      <selection activeCell="A2" sqref="A2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9.33203125" defaultRowHeight="15.6" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="1" max="16384" width="9.33203125" style="1"/>
+    <col min="1" max="1" width="16.6640625" style="1" customWidth="1"/>
+    <col min="2" max="16384" width="9.33203125" style="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:2" ht="16.2" thickBot="1" x14ac:dyDescent="0.35">
@@ -19089,12 +19058,14 @@
   </sheetViews>
   <sheetFormatPr defaultColWidth="9.33203125" defaultRowHeight="15.6" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="1" max="16384" width="9.33203125" style="1"/>
+    <col min="1" max="1" width="12.6640625" style="1" customWidth="1"/>
+    <col min="2" max="16384" width="9.33203125" style="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:5" ht="16.2" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A1" s="1" t="s">
-        <v>275</v>
+      <c r="A1" s="1" t="str">
+        <f>_xlfn.CONCAT( "Table of Disposal Capacity Expansion Cost [",VLOOKUP("currency", Units!$A$2:$B$9, 2, FALSE),"/(", VLOOKUP("volume", Units!$A$2:$B$9, 2, FALSE),"/", VLOOKUP("time", Units!$A$2:$B$9, 2, FALSE),")]")</f>
+        <v>Table of Disposal Capacity Expansion Cost [USD/(bbl/day)]</v>
       </c>
     </row>
     <row r="2" spans="1:5" s="9" customFormat="1" x14ac:dyDescent="0.3">
@@ -19247,17 +19218,19 @@
   <dimension ref="A1:E14"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="D9" sqref="D9"/>
+      <selection activeCell="A2" sqref="A2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9.33203125" defaultRowHeight="15.6" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="1" max="16384" width="9.33203125" style="1"/>
+    <col min="1" max="1" width="13.21875" style="1" customWidth="1"/>
+    <col min="2" max="16384" width="9.33203125" style="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:5" ht="16.2" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A1" s="1" t="s">
-        <v>258</v>
+      <c r="A1" s="1" t="str">
+        <f>_xlfn.CONCAT( "Table of Storage Capacity Expansion Cost [",VLOOKUP("currency", Units!$A$2:$B$9, 2, FALSE),"/", VLOOKUP("volume", Units!$A$2:$B$9, 2, FALSE),"]")</f>
+        <v>Table of Storage Capacity Expansion Cost [USD/bbl]</v>
       </c>
     </row>
     <row r="2" spans="1:5" s="9" customFormat="1" x14ac:dyDescent="0.3">
@@ -19533,12 +19506,14 @@
   </sheetViews>
   <sheetFormatPr defaultColWidth="9.33203125" defaultRowHeight="15.6" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="1" max="16384" width="9.33203125" style="1"/>
+    <col min="1" max="1" width="16.21875" style="1" customWidth="1"/>
+    <col min="2" max="16384" width="9.33203125" style="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:5" ht="16.2" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A1" s="1" t="s">
-        <v>276</v>
+      <c r="A1" s="1" t="str">
+        <f>_xlfn.CONCAT( "Table of Treatment Capacity Expansion Cost [",VLOOKUP("currency", Units!$A$2:$B$9, 2, FALSE),"/(", VLOOKUP("volume", Units!$A$2:$B$9, 2, FALSE),"/", VLOOKUP("time", Units!$A$2:$B$9, 2, FALSE),")]")</f>
+        <v>Table of Treatment Capacity Expansion Cost [USD/(bbl/day)]</v>
       </c>
     </row>
     <row r="2" spans="1:5" s="9" customFormat="1" x14ac:dyDescent="0.3">
@@ -19649,8 +19624,9 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:2" ht="16.2" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A1" s="31" t="s">
-        <v>277</v>
+      <c r="A1" s="1" t="str">
+        <f>_xlfn.CONCAT( "Pipeline Expansion Cost [",VLOOKUP("currency", Units!$A$2:$B$9, 2, FALSE),"/(", VLOOKUP("diameter", Units!$A$2:$B$9, 2, FALSE),"-", VLOOKUP("distance", Units!$A$2:$B$9, 2, FALSE),")]")</f>
+        <v>Pipeline Expansion Cost [USD/(inch-mile)]</v>
       </c>
     </row>
     <row r="2" spans="1:2" ht="15.6" x14ac:dyDescent="0.3">
@@ -19683,11 +19659,13 @@
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <sheetData>
     <row r="1" spans="1:42" ht="16.2" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A1" s="1" t="s">
-        <v>278</v>
+      <c r="A1" s="1" t="str">
+        <f>_xlfn.CONCAT( "Table of Pipeline Expansion Distances [",VLOOKUP("distance", Units!$A$2:$B$9, 2, FALSE),"]")</f>
+        <v>Table of Pipeline Expansion Distances [mile]</v>
       </c>
       <c r="B1" s="1"/>
       <c r="C1" s="1"/>
+      <c r="H1" s="1"/>
     </row>
     <row r="2" spans="1:42" ht="15.6" x14ac:dyDescent="0.3">
       <c r="A2" s="7" t="s">
@@ -21813,31 +21791,31 @@
       <c r="Y18" s="45" t="s">
         <v>248</v>
       </c>
-      <c r="Z18" s="66" t="s">
-        <v>248</v>
-      </c>
-      <c r="AA18" s="66" t="s">
-        <v>248</v>
-      </c>
-      <c r="AB18" s="66" t="s">
-        <v>248</v>
-      </c>
-      <c r="AC18" s="66" t="s">
+      <c r="Z18" s="65" t="s">
+        <v>248</v>
+      </c>
+      <c r="AA18" s="65" t="s">
+        <v>248</v>
+      </c>
+      <c r="AB18" s="65" t="s">
+        <v>248</v>
+      </c>
+      <c r="AC18" s="65" t="s">
         <v>248</v>
       </c>
       <c r="AD18" s="35" t="s">
         <v>248</v>
       </c>
-      <c r="AE18" s="66" t="s">
-        <v>248</v>
-      </c>
-      <c r="AF18" s="66" t="s">
-        <v>248</v>
-      </c>
-      <c r="AG18" s="66" t="s">
-        <v>248</v>
-      </c>
-      <c r="AH18" s="66" t="s">
+      <c r="AE18" s="65" t="s">
+        <v>248</v>
+      </c>
+      <c r="AF18" s="65" t="s">
+        <v>248</v>
+      </c>
+      <c r="AG18" s="65" t="s">
+        <v>248</v>
+      </c>
+      <c r="AH18" s="65" t="s">
         <v>248</v>
       </c>
       <c r="AI18" s="35" t="s">
@@ -21852,13 +21830,13 @@
       <c r="AL18" s="35" t="s">
         <v>248</v>
       </c>
-      <c r="AM18" s="66" t="s">
-        <v>248</v>
-      </c>
-      <c r="AN18" s="66" t="s">
-        <v>248</v>
-      </c>
-      <c r="AO18" s="66" t="s">
+      <c r="AM18" s="65" t="s">
+        <v>248</v>
+      </c>
+      <c r="AN18" s="65" t="s">
+        <v>248</v>
+      </c>
+      <c r="AO18" s="65" t="s">
         <v>248</v>
       </c>
       <c r="AP18" s="35" t="s">
@@ -21941,31 +21919,31 @@
       <c r="Y19" s="45" t="s">
         <v>248</v>
       </c>
-      <c r="Z19" s="66" t="s">
-        <v>248</v>
-      </c>
-      <c r="AA19" s="66" t="s">
-        <v>248</v>
-      </c>
-      <c r="AB19" s="66" t="s">
-        <v>248</v>
-      </c>
-      <c r="AC19" s="66" t="s">
+      <c r="Z19" s="65" t="s">
+        <v>248</v>
+      </c>
+      <c r="AA19" s="65" t="s">
+        <v>248</v>
+      </c>
+      <c r="AB19" s="65" t="s">
+        <v>248</v>
+      </c>
+      <c r="AC19" s="65" t="s">
         <v>248</v>
       </c>
       <c r="AD19" s="35" t="s">
         <v>248</v>
       </c>
-      <c r="AE19" s="66" t="s">
-        <v>248</v>
-      </c>
-      <c r="AF19" s="66" t="s">
-        <v>248</v>
-      </c>
-      <c r="AG19" s="66" t="s">
-        <v>248</v>
-      </c>
-      <c r="AH19" s="66" t="s">
+      <c r="AE19" s="65" t="s">
+        <v>248</v>
+      </c>
+      <c r="AF19" s="65" t="s">
+        <v>248</v>
+      </c>
+      <c r="AG19" s="65" t="s">
+        <v>248</v>
+      </c>
+      <c r="AH19" s="65" t="s">
         <v>248</v>
       </c>
       <c r="AI19" s="35" t="s">
@@ -21980,13 +21958,13 @@
       <c r="AL19" s="35" t="s">
         <v>248</v>
       </c>
-      <c r="AM19" s="66" t="s">
-        <v>248</v>
-      </c>
-      <c r="AN19" s="66" t="s">
-        <v>248</v>
-      </c>
-      <c r="AO19" s="66" t="s">
+      <c r="AM19" s="65" t="s">
+        <v>248</v>
+      </c>
+      <c r="AN19" s="65" t="s">
+        <v>248</v>
+      </c>
+      <c r="AO19" s="65" t="s">
         <v>248</v>
       </c>
       <c r="AP19" s="35" t="s">
@@ -22069,31 +22047,31 @@
       <c r="Y20" s="45" t="s">
         <v>248</v>
       </c>
-      <c r="Z20" s="66" t="s">
-        <v>248</v>
-      </c>
-      <c r="AA20" s="66" t="s">
-        <v>248</v>
-      </c>
-      <c r="AB20" s="66" t="s">
-        <v>248</v>
-      </c>
-      <c r="AC20" s="66" t="s">
+      <c r="Z20" s="65" t="s">
+        <v>248</v>
+      </c>
+      <c r="AA20" s="65" t="s">
+        <v>248</v>
+      </c>
+      <c r="AB20" s="65" t="s">
+        <v>248</v>
+      </c>
+      <c r="AC20" s="65" t="s">
         <v>248</v>
       </c>
       <c r="AD20" s="35" t="s">
         <v>248</v>
       </c>
-      <c r="AE20" s="66" t="s">
-        <v>248</v>
-      </c>
-      <c r="AF20" s="66" t="s">
-        <v>248</v>
-      </c>
-      <c r="AG20" s="66" t="s">
-        <v>248</v>
-      </c>
-      <c r="AH20" s="66" t="s">
+      <c r="AE20" s="65" t="s">
+        <v>248</v>
+      </c>
+      <c r="AF20" s="65" t="s">
+        <v>248</v>
+      </c>
+      <c r="AG20" s="65" t="s">
+        <v>248</v>
+      </c>
+      <c r="AH20" s="65" t="s">
         <v>248</v>
       </c>
       <c r="AI20" s="35" t="s">
@@ -22108,13 +22086,13 @@
       <c r="AL20" s="35" t="s">
         <v>248</v>
       </c>
-      <c r="AM20" s="66" t="s">
-        <v>248</v>
-      </c>
-      <c r="AN20" s="66" t="s">
-        <v>248</v>
-      </c>
-      <c r="AO20" s="66" t="s">
+      <c r="AM20" s="65" t="s">
+        <v>248</v>
+      </c>
+      <c r="AN20" s="65" t="s">
+        <v>248</v>
+      </c>
+      <c r="AO20" s="65" t="s">
         <v>248</v>
       </c>
       <c r="AP20" s="35" t="s">
@@ -22253,10 +22231,10 @@
       <c r="A22" s="29" t="s">
         <v>137</v>
       </c>
-      <c r="B22" s="74" t="s">
-        <v>248</v>
-      </c>
-      <c r="C22" s="74">
+      <c r="B22" s="73" t="s">
+        <v>248</v>
+      </c>
+      <c r="C22" s="73">
         <v>40.752409775985356</v>
       </c>
       <c r="D22" s="45" t="s">
@@ -22340,7 +22318,7 @@
       <c r="AD22" s="32" t="s">
         <v>248</v>
       </c>
-      <c r="AE22" s="74">
+      <c r="AE22" s="73">
         <v>41.716999999999999</v>
       </c>
       <c r="AF22" s="45" t="s">
@@ -22381,10 +22359,10 @@
       <c r="A23" s="29" t="s">
         <v>80</v>
       </c>
-      <c r="B23" s="74">
+      <c r="B23" s="73">
         <v>40.752409775985356</v>
       </c>
-      <c r="C23" s="74" t="s">
+      <c r="C23" s="73" t="s">
         <v>248</v>
       </c>
       <c r="D23" s="45">
@@ -22768,7 +22746,7 @@
       <c r="B26" s="45" t="s">
         <v>248</v>
       </c>
-      <c r="C26" s="74">
+      <c r="C26" s="73">
         <v>18.141999999999999</v>
       </c>
       <c r="D26" s="45" t="s">
@@ -27378,17 +27356,19 @@
   <dimension ref="A1:B8"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="K5" sqref="K5"/>
+      <selection activeCell="A2" sqref="A2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9.21875" defaultRowHeight="15.6" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="1" max="16384" width="9.21875" style="1"/>
+    <col min="1" max="1" width="19.109375" style="1" customWidth="1"/>
+    <col min="2" max="16384" width="9.21875" style="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:2" ht="16.2" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A1" s="1" t="s">
-        <v>270</v>
+      <c r="A1" s="1" t="str">
+        <f>_xlfn.CONCAT( "Table of Pipeline Capacity Expansion Increments [",VLOOKUP("volume", Units!$A$2:$B$9, 2, FALSE),"/", VLOOKUP("time", Units!$A$2:$B$9, 2, FALSE),"]")</f>
+        <v>Table of Pipeline Capacity Expansion Increments [bbl/day]</v>
       </c>
     </row>
     <row r="2" spans="1:2" x14ac:dyDescent="0.3">
@@ -27458,14 +27438,15 @@
   <dimension ref="A1:H6"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="K27" sqref="K27"/>
+      <selection activeCell="A2" sqref="A2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <sheetData>
     <row r="1" spans="1:8" ht="16.2" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A1" s="1" t="s">
-        <v>279</v>
+      <c r="A1" s="1" t="str">
+        <f>_xlfn.CONCAT( "Table of Pipeline Capacity Expansion Costs [",VLOOKUP("currency", Units!$A$2:$B$9, 2, FALSE),"/(", VLOOKUP("volume", Units!$A$2:$B$9, 2, FALSE),"/", VLOOKUP("time", Units!$A$2:$B$9, 2, FALSE),")]")</f>
+        <v>Table of Pipeline Capacity Expansion Costs [USD/(bbl/day)]</v>
       </c>
       <c r="B1" s="1"/>
       <c r="C1" s="1"/>
@@ -27501,25 +27482,25 @@
       <c r="A3" s="47" t="s">
         <v>139</v>
       </c>
-      <c r="B3" s="67" t="s">
+      <c r="B3" s="66" t="s">
         <v>141</v>
       </c>
-      <c r="C3" s="68">
+      <c r="C3" s="67">
         <v>30</v>
       </c>
-      <c r="D3" s="68">
+      <c r="D3" s="67">
         <v>30</v>
       </c>
-      <c r="E3" s="68">
+      <c r="E3" s="67">
         <v>30</v>
       </c>
-      <c r="F3" s="68">
+      <c r="F3" s="67">
         <v>30</v>
       </c>
-      <c r="G3" s="68">
+      <c r="G3" s="67">
         <v>30</v>
       </c>
-      <c r="H3" s="69">
+      <c r="H3" s="68">
         <v>30</v>
       </c>
     </row>
@@ -27527,25 +27508,25 @@
       <c r="A4" s="47" t="s">
         <v>141</v>
       </c>
-      <c r="B4" s="67" t="s">
+      <c r="B4" s="66" t="s">
         <v>139</v>
       </c>
-      <c r="C4" s="68">
+      <c r="C4" s="67">
         <v>30</v>
       </c>
-      <c r="D4" s="68">
+      <c r="D4" s="67">
         <v>30</v>
       </c>
-      <c r="E4" s="68">
+      <c r="E4" s="67">
         <v>30</v>
       </c>
-      <c r="F4" s="68">
+      <c r="F4" s="67">
         <v>30</v>
       </c>
-      <c r="G4" s="68">
+      <c r="G4" s="67">
         <v>30</v>
       </c>
-      <c r="H4" s="69">
+      <c r="H4" s="68">
         <v>30</v>
       </c>
     </row>
@@ -27553,51 +27534,51 @@
       <c r="A5" s="47" t="s">
         <v>138</v>
       </c>
-      <c r="B5" s="67" t="s">
+      <c r="B5" s="66" t="s">
         <v>140</v>
       </c>
-      <c r="C5" s="68">
+      <c r="C5" s="67">
         <v>30</v>
       </c>
-      <c r="D5" s="68">
+      <c r="D5" s="67">
         <v>30</v>
       </c>
-      <c r="E5" s="68">
+      <c r="E5" s="67">
         <v>30</v>
       </c>
-      <c r="F5" s="68">
+      <c r="F5" s="67">
         <v>30</v>
       </c>
-      <c r="G5" s="68">
+      <c r="G5" s="67">
         <v>30</v>
       </c>
-      <c r="H5" s="69">
+      <c r="H5" s="68">
         <v>30</v>
       </c>
     </row>
     <row r="6" spans="1:8" ht="16.2" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A6" s="70" t="s">
+      <c r="A6" s="69" t="s">
         <v>140</v>
       </c>
-      <c r="B6" s="71" t="s">
+      <c r="B6" s="70" t="s">
         <v>138</v>
       </c>
-      <c r="C6" s="72">
+      <c r="C6" s="71">
         <v>30</v>
       </c>
-      <c r="D6" s="72">
+      <c r="D6" s="71">
         <v>30</v>
       </c>
-      <c r="E6" s="72">
+      <c r="E6" s="71">
         <v>30</v>
       </c>
-      <c r="F6" s="72">
+      <c r="F6" s="71">
         <v>30</v>
       </c>
-      <c r="G6" s="72">
+      <c r="G6" s="71">
         <v>30</v>
       </c>
-      <c r="H6" s="73">
+      <c r="H6" s="72">
         <v>30</v>
       </c>
     </row>
@@ -27612,7 +27593,7 @@
   <dimension ref="A1:B4"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="D10" sqref="D10"/>
+      <selection activeCell="A2" sqref="A2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -27658,7 +27639,9 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{ED2F8796-71C2-44EA-9373-5A0165D7B559}">
   <dimension ref="A1:B4"/>
   <sheetViews>
-    <sheetView workbookViewId="0"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="A2" sqref="A2"/>
+    </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
@@ -27703,7 +27686,9 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{134045F2-617D-4B6C-9AE3-C6E73CF3B321}">
   <dimension ref="A1:B21"/>
   <sheetViews>
-    <sheetView workbookViewId="0"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="A2" sqref="A2"/>
+    </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
@@ -27716,24 +27701,25 @@
     <col min="8" max="8" width="11" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:2" ht="15" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A1" t="s">
-        <v>280</v>
+    <row r="1" spans="1:2" ht="16.2" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="A1" s="1" t="str">
+        <f>_xlfn.CONCAT( "Table of Water Quality of Produced Water and Flowback Water [",VLOOKUP("concentration", Units!$A$2:$B$9, 2, FALSE),"]")</f>
+        <v>Table of Water Quality of Produced Water and Flowback Water [mg/liter]</v>
       </c>
     </row>
     <row r="2" spans="1:2" ht="15.6" x14ac:dyDescent="0.3">
       <c r="A2" s="7" t="s">
         <v>250</v>
       </c>
-      <c r="B2" s="75" t="s">
+      <c r="B2" s="74" t="s">
         <v>249</v>
       </c>
     </row>
     <row r="3" spans="1:2" ht="15.6" x14ac:dyDescent="0.3">
-      <c r="A3" s="76" t="s">
+      <c r="A3" s="75" t="s">
         <v>117</v>
       </c>
-      <c r="B3" s="77">
+      <c r="B3" s="76">
         <v>142277</v>
       </c>
     </row>
@@ -27741,7 +27727,7 @@
       <c r="A4" s="29" t="s">
         <v>3</v>
       </c>
-      <c r="B4" s="78">
+      <c r="B4" s="77">
         <v>140998</v>
       </c>
     </row>
@@ -27749,7 +27735,7 @@
       <c r="A5" s="29" t="s">
         <v>4</v>
       </c>
-      <c r="B5" s="78">
+      <c r="B5" s="77">
         <v>172490.2</v>
       </c>
     </row>
@@ -27757,7 +27743,7 @@
       <c r="A6" s="29" t="s">
         <v>109</v>
       </c>
-      <c r="B6" s="78">
+      <c r="B6" s="77">
         <v>257547</v>
       </c>
     </row>
@@ -27765,7 +27751,7 @@
       <c r="A7" s="29" t="s">
         <v>110</v>
       </c>
-      <c r="B7" s="78">
+      <c r="B7" s="77">
         <v>241833.8</v>
       </c>
     </row>
@@ -27773,7 +27759,7 @@
       <c r="A8" s="29" t="s">
         <v>111</v>
       </c>
-      <c r="B8" s="78">
+      <c r="B8" s="77">
         <v>188503.7</v>
       </c>
     </row>
@@ -27781,7 +27767,7 @@
       <c r="A9" s="29" t="s">
         <v>112</v>
       </c>
-      <c r="B9" s="78">
+      <c r="B9" s="77">
         <v>146716</v>
       </c>
     </row>
@@ -27789,7 +27775,7 @@
       <c r="A10" s="29" t="s">
         <v>113</v>
       </c>
-      <c r="B10" s="78">
+      <c r="B10" s="77">
         <v>216563</v>
       </c>
     </row>
@@ -27797,7 +27783,7 @@
       <c r="A11" s="29" t="s">
         <v>114</v>
       </c>
-      <c r="B11" s="78">
+      <c r="B11" s="77">
         <v>150626</v>
       </c>
     </row>
@@ -27805,7 +27791,7 @@
       <c r="A12" s="29" t="s">
         <v>115</v>
       </c>
-      <c r="B12" s="78">
+      <c r="B12" s="77">
         <v>247061</v>
       </c>
     </row>
@@ -27813,7 +27799,7 @@
       <c r="A13" s="29" t="s">
         <v>116</v>
       </c>
-      <c r="B13" s="78">
+      <c r="B13" s="77">
         <v>180968</v>
       </c>
     </row>
@@ -27821,7 +27807,7 @@
       <c r="A14" s="29" t="s">
         <v>118</v>
       </c>
-      <c r="B14" s="78">
+      <c r="B14" s="77">
         <v>195584</v>
       </c>
     </row>
@@ -27829,7 +27815,7 @@
       <c r="A15" s="29" t="s">
         <v>119</v>
       </c>
-      <c r="B15" s="78">
+      <c r="B15" s="77">
         <v>148655</v>
       </c>
     </row>
@@ -27837,7 +27823,7 @@
       <c r="A16" s="29" t="s">
         <v>120</v>
       </c>
-      <c r="B16" s="78">
+      <c r="B16" s="77">
         <v>185369</v>
       </c>
     </row>
@@ -27845,7 +27831,7 @@
       <c r="A17" s="29" t="s">
         <v>121</v>
       </c>
-      <c r="B17" s="78">
+      <c r="B17" s="77">
         <v>222724</v>
       </c>
     </row>
@@ -27853,7 +27839,7 @@
       <c r="A18" s="29" t="s">
         <v>5</v>
       </c>
-      <c r="B18" s="78">
+      <c r="B18" s="77">
         <v>165376</v>
       </c>
     </row>
@@ -27861,7 +27847,7 @@
       <c r="A19" s="29" t="s">
         <v>122</v>
       </c>
-      <c r="B19" s="78">
+      <c r="B19" s="77">
         <v>240977</v>
       </c>
     </row>
@@ -27869,7 +27855,7 @@
       <c r="A20" s="29" t="s">
         <v>123</v>
       </c>
-      <c r="B20" s="78">
+      <c r="B20" s="77">
         <v>192794</v>
       </c>
     </row>
@@ -27877,7 +27863,7 @@
       <c r="A21" s="30" t="s">
         <v>124</v>
       </c>
-      <c r="B21" s="79">
+      <c r="B21" s="78">
         <v>216769</v>
       </c>
     </row>
@@ -27891,23 +27877,26 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{6FE4BAFD-2A94-4164-976F-B9E5B42E5AAB}">
   <dimension ref="A1:B3"/>
   <sheetViews>
-    <sheetView workbookViewId="0"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="A2" sqref="A2"/>
+    </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
     <col min="2" max="2" width="12.6640625" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:2" ht="15" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A1" t="s">
-        <v>281</v>
+    <row r="1" spans="1:2" ht="16.2" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="A1" s="1" t="str">
+        <f>_xlfn.CONCAT( "Table of Initial Water Quality at Storage [",VLOOKUP("concentration", Units!$A$2:$B$9, 2, FALSE),"]")</f>
+        <v>Table of Initial Water Quality at Storage [mg/liter]</v>
       </c>
     </row>
     <row r="2" spans="1:2" ht="15.6" x14ac:dyDescent="0.3">
       <c r="A2" s="7" t="s">
-        <v>251</v>
-      </c>
-      <c r="B2" s="75" t="s">
+        <v>250</v>
+      </c>
+      <c r="B2" s="74" t="s">
         <v>249</v>
       </c>
     </row>
@@ -27915,7 +27904,7 @@
       <c r="A3" s="53" t="s">
         <v>78</v>
       </c>
-      <c r="B3" s="80">
+      <c r="B3" s="79">
         <v>150000</v>
       </c>
     </row>
@@ -27930,24 +27919,26 @@
   <dimension ref="A1:B6"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="I38" sqref="I38"/>
+      <selection activeCell="A2" sqref="A2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
+    <col min="1" max="1" width="17.6640625" customWidth="1"/>
     <col min="2" max="2" width="12.5546875" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:2" ht="15" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A1" t="s">
-        <v>282</v>
+    <row r="1" spans="1:2" ht="16.2" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="A1" s="1" t="str">
+        <f>_xlfn.CONCAT( "Table of Initial Water Quality at Completions Pad Storage [",VLOOKUP("concentration", Units!$A$2:$B$9, 2, FALSE),"]")</f>
+        <v>Table of Initial Water Quality at Completions Pad Storage [mg/liter]</v>
       </c>
     </row>
     <row r="2" spans="1:2" ht="15.6" x14ac:dyDescent="0.3">
       <c r="A2" s="7" t="s">
         <v>229</v>
       </c>
-      <c r="B2" s="75" t="s">
+      <c r="B2" s="74" t="s">
         <v>249</v>
       </c>
     </row>
@@ -27955,7 +27946,7 @@
       <c r="A3" s="29" t="s">
         <v>5</v>
       </c>
-      <c r="B3" s="78">
+      <c r="B3" s="77">
         <v>150000</v>
       </c>
     </row>
@@ -27963,7 +27954,7 @@
       <c r="A4" s="29" t="s">
         <v>122</v>
       </c>
-      <c r="B4" s="78">
+      <c r="B4" s="77">
         <v>150000</v>
       </c>
     </row>
@@ -27971,7 +27962,7 @@
       <c r="A5" s="29" t="s">
         <v>123</v>
       </c>
-      <c r="B5" s="78">
+      <c r="B5" s="77">
         <v>150000</v>
       </c>
     </row>
@@ -27979,7 +27970,7 @@
       <c r="A6" s="30" t="s">
         <v>124</v>
       </c>
-      <c r="B6" s="79">
+      <c r="B6" s="78">
         <v>150000</v>
       </c>
     </row>

</xml_diff>

<commit_message>
update input file for distance based pipeline costs
</commit_message>
<xml_diff>
--- a/pareto/case_studies/input_data_generic_strategic_case_study_LAYFLAT_FULL.xlsx
+++ b/pareto/case_studies/input_data_generic_strategic_case_study_LAYFLAT_FULL.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="25128"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="25330"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\melodys\Documents\1. Projects\PARETO - Department of Energy\Code Updates\GIT Tracked Folder\project-pareto\pareto\case_studies\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{07327253-9B73-474C-AA9A-D5C81C57AF57}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{C219849D-6ED1-45CB-B43F-7A47759C2908}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="16680" yWindow="-16320" windowWidth="29040" windowHeight="15840" tabRatio="834" firstSheet="2" activeTab="2" xr2:uid="{FB8C51AB-905F-4544-9E4B-1F4384FA855C}"/>
+    <workbookView xWindow="-21720" yWindow="-3555" windowWidth="21840" windowHeight="13140" tabRatio="834" firstSheet="27" activeTab="35" xr2:uid="{FB8C51AB-905F-4544-9E4B-1F4384FA855C}"/>
   </bookViews>
   <sheets>
     <sheet name="Overview" sheetId="33" r:id="rId1"/>
@@ -108,11 +108,11 @@
 <file path=xl/comments1.xml><?xml version="1.0" encoding="utf-8"?>
 <comments xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="xr">
   <authors>
-    <author>tc={351D21B0-A2E0-4661-9BC9-3E29F23CD077}</author>
-    <author>tc={954D1F11-FD45-4D3D-A8AF-0FD2369021B3}</author>
+    <author>tc={F48106AB-FCCB-457F-ACFA-F44AC7743ED7}</author>
+    <author>tc={17549EBD-A9AD-4A09-B0F1-99A5A1C7F0B1}</author>
   </authors>
   <commentList>
-    <comment ref="AJ18" authorId="0" shapeId="0" xr:uid="{351D21B0-A2E0-4661-9BC9-3E29F23CD077}">
+    <comment ref="AJ18" authorId="0" shapeId="0" xr:uid="{F48106AB-FCCB-457F-ACFA-F44AC7743ED7}">
       <text>
         <t>[Threaded comment]
 Your version of Excel allows you to read this threaded comment; however, any edits to it will get removed if the file is opened in a newer version of Excel. Learn more: https://go.microsoft.com/fwlink/?linkid=870924
@@ -120,7 +120,7 @@
     Distances between completion pads and treatment facilities (layflat lines) are calculated as a straight distance times 1.3 (tortuosity factor)</t>
       </text>
     </comment>
-    <comment ref="AM52" authorId="1" shapeId="0" xr:uid="{954D1F11-FD45-4D3D-A8AF-0FD2369021B3}">
+    <comment ref="AM52" authorId="1" shapeId="0" xr:uid="{17549EBD-A9AD-4A09-B0F1-99A5A1C7F0B1}">
       <text>
         <t>[Threaded comment]
 Your version of Excel allows you to read this threaded comment; however, any edits to it will get removed if the file is opened in a newer version of Excel. Learn more: https://go.microsoft.com/fwlink/?linkid=870924
@@ -1023,7 +1023,7 @@
     <numFmt numFmtId="164" formatCode="#,##0.0"/>
     <numFmt numFmtId="165" formatCode="0.0"/>
   </numFmts>
-  <fonts count="9" x14ac:knownFonts="1">
+  <fonts count="10" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -1088,6 +1088,12 @@
       <name val="Calibri"/>
       <family val="2"/>
       <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="9"/>
+      <color indexed="81"/>
+      <name val="Tahoma"/>
+      <charset val="1"/>
     </font>
   </fonts>
   <fills count="5">
@@ -2250,10 +2256,10 @@
 
 <file path=xl/threadedComments/threadedComment1.xml><?xml version="1.0" encoding="utf-8"?>
 <ThreadedComments xmlns="http://schemas.microsoft.com/office/spreadsheetml/2018/threadedcomments" xmlns:x="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
-  <threadedComment ref="AJ18" dT="2021-10-28T19:21:23.79" personId="{7E20C1B5-7AC5-453E-B7BB-A7A530AF52E0}" id="{351D21B0-A2E0-4661-9BC9-3E29F23CD077}">
+  <threadedComment ref="AJ18" dT="2021-10-28T19:21:23.79" personId="{7E20C1B5-7AC5-453E-B7BB-A7A530AF52E0}" id="{F48106AB-FCCB-457F-ACFA-F44AC7743ED7}">
     <text>Distances between completion pads and treatment facilities (layflat lines) are calculated as a straight distance times 1.3 (tortuosity factor)</text>
   </threadedComment>
-  <threadedComment ref="AM52" dT="2021-10-28T19:18:35.38" personId="{7E20C1B5-7AC5-453E-B7BB-A7A530AF52E0}" id="{954D1F11-FD45-4D3D-A8AF-0FD2369021B3}">
+  <threadedComment ref="AM52" dT="2021-10-28T19:18:35.38" personId="{7E20C1B5-7AC5-453E-B7BB-A7A530AF52E0}" id="{17549EBD-A9AD-4A09-B0F1-99A5A1C7F0B1}">
     <text>Distances between fresh water sources and completion pads are assumed, not measured from the diagram</text>
   </threadedComment>
 </ThreadedComments>
@@ -7858,7 +7864,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{6FEB10CD-C2F5-4A5B-9D35-9BA20FBC12B6}">
   <dimension ref="A1:AZ12"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="120" zoomScaleNormal="120" workbookViewId="0"/>
+    <sheetView zoomScale="120" zoomScaleNormal="120" workbookViewId="0"/>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9.33203125" defaultRowHeight="15.6" x14ac:dyDescent="0.3"/>
   <cols>
@@ -8903,6 +8909,9 @@
 
 <file path=xl/worksheets/sheet35.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{0D6FA210-6C83-4CC4-AF45-F41CDC53F769}">
+  <sheetPr>
+    <tabColor theme="9"/>
+  </sheetPr>
   <dimension ref="A1:BA17"/>
   <sheetViews>
     <sheetView showZeros="0" workbookViewId="0">
@@ -9782,9 +9791,12 @@
 
 <file path=xl/worksheets/sheet36.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{81EF4E1D-6CE0-4F02-8B9E-F2818C0A814C}">
+  <sheetPr>
+    <tabColor theme="9"/>
+  </sheetPr>
   <dimension ref="A1:BA18"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
+    <sheetView tabSelected="1" workbookViewId="0">
       <selection activeCell="A2" sqref="A2"/>
     </sheetView>
   </sheetViews>
@@ -19614,7 +19626,7 @@
   <dimension ref="A1:B3"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="A2" sqref="A2"/>
+      <selection activeCell="B3" sqref="B3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -19642,7 +19654,7 @@
         <v>243</v>
       </c>
       <c r="B3" s="40">
-        <v>120000</v>
+        <v>300000</v>
       </c>
     </row>
   </sheetData>
@@ -19800,7 +19812,7 @@
         <v>117</v>
       </c>
       <c r="B3" s="45">
-        <v>14.26</v>
+        <v>1.4259999999999999</v>
       </c>
       <c r="C3" s="45" t="s">
         <v>248</v>
@@ -19940,7 +19952,7 @@
         <v>248</v>
       </c>
       <c r="F4" s="45">
-        <v>16.847000000000001</v>
+        <v>1.6847000000000001</v>
       </c>
       <c r="G4" s="45" t="s">
         <v>248</v>
@@ -20071,7 +20083,7 @@
         <v>248</v>
       </c>
       <c r="G5" s="45">
-        <v>12.562999999999999</v>
+        <v>1.2563</v>
       </c>
       <c r="H5" s="45" t="s">
         <v>248</v>
@@ -20214,7 +20226,7 @@
         <v>248</v>
       </c>
       <c r="L6" s="45">
-        <v>25.074000000000002</v>
+        <v>2.5074000000000001</v>
       </c>
       <c r="M6" s="45" t="s">
         <v>248</v>
@@ -20339,13 +20351,13 @@
         <v>248</v>
       </c>
       <c r="K7" s="45">
-        <v>59.184867367820758</v>
+        <v>5.9184867367820804</v>
       </c>
       <c r="L7" s="45" t="s">
         <v>248</v>
       </c>
       <c r="M7" s="45">
-        <v>14.871</v>
+        <v>1.4871000000000001</v>
       </c>
       <c r="N7" s="45" t="s">
         <v>248</v>
@@ -20485,7 +20497,7 @@
         <v>248</v>
       </c>
       <c r="Q8" s="45">
-        <v>24.758000000000003</v>
+        <v>2.4758</v>
       </c>
       <c r="R8" s="45" t="s">
         <v>248</v>
@@ -20610,7 +20622,7 @@
         <v>248</v>
       </c>
       <c r="P9" s="45">
-        <v>30.722259990726229</v>
+        <v>3.0722259990726202</v>
       </c>
       <c r="Q9" s="45" t="s">
         <v>248</v>
@@ -20884,7 +20896,7 @@
         <v>248</v>
       </c>
       <c r="V11" s="45">
-        <v>24.247</v>
+        <v>2.4247000000000001</v>
       </c>
       <c r="W11" s="45" t="s">
         <v>248</v>
@@ -21006,7 +21018,7 @@
         <v>248</v>
       </c>
       <c r="T12" s="45">
-        <v>24.036999999999999</v>
+        <v>2.4037000000000002</v>
       </c>
       <c r="U12" s="45" t="s">
         <v>248</v>
@@ -21152,7 +21164,7 @@
         <v>248</v>
       </c>
       <c r="Z13" s="45">
-        <v>38.297000000000004</v>
+        <v>3.8296999999999999</v>
       </c>
       <c r="AA13" s="45" t="s">
         <v>248</v>
@@ -21542,7 +21554,7 @@
         <v>248</v>
       </c>
       <c r="AB16" s="45">
-        <v>12.425000000000001</v>
+        <v>1.2424999999999999</v>
       </c>
       <c r="AC16" s="45" t="s">
         <v>248</v>
@@ -21661,7 +21673,7 @@
         <v>248</v>
       </c>
       <c r="Y17" s="11">
-        <v>24.249000000000002</v>
+        <v>2.4249000000000001</v>
       </c>
       <c r="Z17" s="11" t="s">
         <v>248</v>
@@ -21726,7 +21738,7 @@
         <v>248</v>
       </c>
       <c r="D18" s="45">
-        <v>11.209999999999999</v>
+        <v>1.121</v>
       </c>
       <c r="E18" s="45" t="s">
         <v>248</v>
@@ -21822,7 +21834,7 @@
         <v>248</v>
       </c>
       <c r="AJ18" s="45">
-        <v>35.07985</v>
+        <v>3.5079850000000001</v>
       </c>
       <c r="AK18" s="32" t="s">
         <v>248</v>
@@ -21875,7 +21887,7 @@
         <v>248</v>
       </c>
       <c r="K19" s="45">
-        <v>21.292999999999999</v>
+        <v>2.1293000000000002</v>
       </c>
       <c r="L19" s="45" t="s">
         <v>248</v>
@@ -21950,7 +21962,7 @@
         <v>248</v>
       </c>
       <c r="AJ19" s="45">
-        <v>30.886050000000001</v>
+        <v>3.0886049999999998</v>
       </c>
       <c r="AK19" s="32" t="s">
         <v>248</v>
@@ -22024,7 +22036,7 @@
         <v>248</v>
       </c>
       <c r="R20" s="45">
-        <v>20.696999999999999</v>
+        <v>2.0697000000000001</v>
       </c>
       <c r="S20" s="45" t="s">
         <v>248</v>
@@ -22081,7 +22093,7 @@
         <v>248</v>
       </c>
       <c r="AK20" s="32">
-        <v>46.94885</v>
+        <v>4.6948850000000002</v>
       </c>
       <c r="AL20" s="35" t="s">
         <v>248</v>
@@ -22170,7 +22182,7 @@
         <v>248</v>
       </c>
       <c r="X21" s="11">
-        <v>22.094999999999999</v>
+        <v>2.2094999999999998</v>
       </c>
       <c r="Y21" s="11" t="s">
         <v>248</v>
@@ -22209,7 +22221,7 @@
         <v>248</v>
       </c>
       <c r="AK21" s="12">
-        <v>46.479550000000003</v>
+        <v>4.6479549999999996</v>
       </c>
       <c r="AL21" s="36" t="s">
         <v>248</v>
@@ -22235,7 +22247,7 @@
         <v>248</v>
       </c>
       <c r="C22" s="73">
-        <v>40.752409775985356</v>
+        <v>4.0752409775985399</v>
       </c>
       <c r="D22" s="45" t="s">
         <v>248</v>
@@ -22319,7 +22331,7 @@
         <v>248</v>
       </c>
       <c r="AE22" s="73">
-        <v>41.716999999999999</v>
+        <v>4.1717000000000004</v>
       </c>
       <c r="AF22" s="45" t="s">
         <v>248</v>
@@ -22360,7 +22372,7 @@
         <v>80</v>
       </c>
       <c r="B23" s="73">
-        <v>40.752409775985356</v>
+        <v>4.0752409775985399</v>
       </c>
       <c r="C23" s="73" t="s">
         <v>248</v>
@@ -22372,7 +22384,7 @@
         <v>248</v>
       </c>
       <c r="F23" s="45">
-        <v>18.141999999999999</v>
+        <v>1.8142</v>
       </c>
       <c r="G23" s="45" t="s">
         <v>248</v>
@@ -22599,7 +22611,7 @@
         <v>248</v>
       </c>
       <c r="AM24" s="45">
-        <v>11.209999999999999</v>
+        <v>1.121</v>
       </c>
       <c r="AN24" s="45" t="s">
         <v>248</v>
@@ -22631,7 +22643,7 @@
         <v>248</v>
       </c>
       <c r="G25" s="45">
-        <v>12.532999999999999</v>
+        <v>1.2533000000000001</v>
       </c>
       <c r="H25" s="45" t="s">
         <v>248</v>
@@ -22706,7 +22718,7 @@
         <v>248</v>
       </c>
       <c r="AF25" s="45">
-        <v>13.163</v>
+        <v>1.3163</v>
       </c>
       <c r="AG25" s="45" t="s">
         <v>248</v>
@@ -22747,7 +22759,7 @@
         <v>248</v>
       </c>
       <c r="C26" s="73">
-        <v>18.141999999999999</v>
+        <v>1.8142</v>
       </c>
       <c r="D26" s="45" t="s">
         <v>248</v>
@@ -22765,7 +22777,7 @@
         <v>248</v>
       </c>
       <c r="I26" s="45">
-        <v>14.431000000000001</v>
+        <v>1.4431</v>
       </c>
       <c r="J26" s="45" t="s">
         <v>248</v>
@@ -22881,7 +22893,7 @@
         <v>248</v>
       </c>
       <c r="E27" s="45">
-        <v>12.532999999999999</v>
+        <v>1.2533000000000001</v>
       </c>
       <c r="F27" s="45" t="s">
         <v>248</v>
@@ -22890,7 +22902,7 @@
         <v>248</v>
       </c>
       <c r="H27" s="45">
-        <v>11.53</v>
+        <v>1.153</v>
       </c>
       <c r="I27" s="45" t="s">
         <v>248</v>
@@ -23015,7 +23027,7 @@
         <v>248</v>
       </c>
       <c r="G28" s="45">
-        <v>11.53</v>
+        <v>1.153</v>
       </c>
       <c r="H28" s="45" t="s">
         <v>248</v>
@@ -23024,7 +23036,7 @@
         <v>6.0780000000000003</v>
       </c>
       <c r="J28" s="45">
-        <v>24.449000000000002</v>
+        <v>2.4449000000000001</v>
       </c>
       <c r="K28" s="45" t="s">
         <v>248</v>
@@ -23140,7 +23152,7 @@
         <v>248</v>
       </c>
       <c r="F29" s="45">
-        <v>14.431000000000001</v>
+        <v>1.4431</v>
       </c>
       <c r="G29" s="45" t="s">
         <v>248</v>
@@ -23230,7 +23242,7 @@
         <v>248</v>
       </c>
       <c r="AJ29" s="45">
-        <v>17.599</v>
+        <v>1.7599</v>
       </c>
       <c r="AK29" s="32" t="s">
         <v>248</v>
@@ -23274,7 +23286,7 @@
         <v>248</v>
       </c>
       <c r="H30" s="45">
-        <v>24.449000000000002</v>
+        <v>2.4449000000000001</v>
       </c>
       <c r="I30" s="45" t="s">
         <v>248</v>
@@ -23286,7 +23298,7 @@
         <v>9.9379999999999988</v>
       </c>
       <c r="L30" s="45">
-        <v>38.850999999999999</v>
+        <v>3.8851</v>
       </c>
       <c r="M30" s="45" t="s">
         <v>248</v>
@@ -23417,7 +23429,7 @@
         <v>248</v>
       </c>
       <c r="M31" s="45">
-        <v>74.055867367820753</v>
+        <v>7.4055867367820802</v>
       </c>
       <c r="N31" s="45" t="s">
         <v>248</v>
@@ -23498,7 +23510,7 @@
         <v>248</v>
       </c>
       <c r="AN31" s="45">
-        <v>21.292999999999999</v>
+        <v>2.1293000000000002</v>
       </c>
       <c r="AO31" s="45" t="s">
         <v>248</v>
@@ -23536,7 +23548,7 @@
         <v>248</v>
       </c>
       <c r="J32" s="45">
-        <v>38.850999999999999</v>
+        <v>3.8851</v>
       </c>
       <c r="K32" s="45" t="s">
         <v>248</v>
@@ -23548,7 +23560,7 @@
         <v>248</v>
       </c>
       <c r="N32" s="45">
-        <v>26.43</v>
+        <v>2.6429999999999998</v>
       </c>
       <c r="O32" s="45" t="s">
         <v>248</v>
@@ -23667,7 +23679,7 @@
         <v>248</v>
       </c>
       <c r="K33" s="45">
-        <v>74.055867367820753</v>
+        <v>7.4055867367820802</v>
       </c>
       <c r="L33" s="45" t="s">
         <v>248</v>
@@ -23679,7 +23691,7 @@
         <v>248</v>
       </c>
       <c r="O33" s="45">
-        <v>48.848606101876086</v>
+        <v>4.8848606101876104</v>
       </c>
       <c r="P33" s="45" t="s">
         <v>248</v>
@@ -23748,7 +23760,7 @@
         <v>248</v>
       </c>
       <c r="AL33" s="32">
-        <v>10.85</v>
+        <v>1.085</v>
       </c>
       <c r="AM33" s="45" t="s">
         <v>248</v>
@@ -23798,7 +23810,7 @@
         <v>248</v>
       </c>
       <c r="L34" s="45">
-        <v>26.43</v>
+        <v>2.6429999999999998</v>
       </c>
       <c r="M34" s="45" t="s">
         <v>248</v>
@@ -23807,7 +23819,7 @@
         <v>248</v>
       </c>
       <c r="O34" s="45">
-        <v>31.087656701677112</v>
+        <v>3.1087656701677102</v>
       </c>
       <c r="P34" s="45" t="s">
         <v>248</v>
@@ -23861,7 +23873,7 @@
         <v>248</v>
       </c>
       <c r="AG34" s="45">
-        <v>30.183999999999997</v>
+        <v>3.0184000000000002</v>
       </c>
       <c r="AH34" s="45" t="s">
         <v>248</v>
@@ -23929,10 +23941,10 @@
         <v>248</v>
       </c>
       <c r="M35" s="45">
-        <v>48.848606101876086</v>
+        <v>4.8848606101876104</v>
       </c>
       <c r="N35" s="45">
-        <v>31.087656701677112</v>
+        <v>3.1087656701677102</v>
       </c>
       <c r="O35" s="45" t="s">
         <v>248</v>
@@ -23980,7 +23992,7 @@
         <v>248</v>
       </c>
       <c r="AD35" s="32">
-        <v>13.959</v>
+        <v>1.3958999999999999</v>
       </c>
       <c r="AE35" s="45" t="s">
         <v>248</v>
@@ -24069,7 +24081,7 @@
         <v>248</v>
       </c>
       <c r="Q36" s="45">
-        <v>13.553999999999998</v>
+        <v>1.3553999999999999</v>
       </c>
       <c r="R36" s="45" t="s">
         <v>248</v>
@@ -24194,13 +24206,13 @@
         <v>248</v>
       </c>
       <c r="P37" s="45">
-        <v>13.553999999999998</v>
+        <v>1.3553999999999999</v>
       </c>
       <c r="Q37" s="45" t="s">
         <v>248</v>
       </c>
       <c r="R37" s="45">
-        <v>32.003367068383</v>
+        <v>3.2003367068383</v>
       </c>
       <c r="S37" s="45" t="s">
         <v>248</v>
@@ -24325,7 +24337,7 @@
         <v>248</v>
       </c>
       <c r="Q38" s="45">
-        <v>32.003367068383</v>
+        <v>3.2003367068383</v>
       </c>
       <c r="R38" s="45" t="s">
         <v>248</v>
@@ -24376,7 +24388,7 @@
         <v>248</v>
       </c>
       <c r="AH38" s="45">
-        <v>64.859913942891041</v>
+        <v>6.4859913942891003</v>
       </c>
       <c r="AI38" s="32" t="s">
         <v>248</v>
@@ -24397,7 +24409,7 @@
         <v>248</v>
       </c>
       <c r="AO38" s="45">
-        <v>20.696999999999999</v>
+        <v>2.0697000000000001</v>
       </c>
       <c r="AP38" s="32" t="s">
         <v>248</v>
@@ -24504,7 +24516,7 @@
         <v>248</v>
       </c>
       <c r="AH39" s="45">
-        <v>34.19</v>
+        <v>3.419</v>
       </c>
       <c r="AI39" s="32" t="s">
         <v>248</v>
@@ -24599,7 +24611,7 @@
         <v>248</v>
       </c>
       <c r="W40" s="45">
-        <v>54.977999999999994</v>
+        <v>5.4977999999999998</v>
       </c>
       <c r="X40" s="45" t="s">
         <v>248</v>
@@ -24769,7 +24781,7 @@
         <v>248</v>
       </c>
       <c r="AK41" s="32">
-        <v>22.666999999999998</v>
+        <v>2.2667000000000002</v>
       </c>
       <c r="AL41" s="32" t="s">
         <v>248</v>
@@ -24974,7 +24986,7 @@
         <v>248</v>
       </c>
       <c r="T43" s="45">
-        <v>54.977999999999994</v>
+        <v>5.4977999999999998</v>
       </c>
       <c r="U43" s="45" t="s">
         <v>248</v>
@@ -24986,7 +24998,7 @@
         <v>248</v>
       </c>
       <c r="X43" s="45">
-        <v>28.763999999999999</v>
+        <v>2.8763999999999998</v>
       </c>
       <c r="Y43" s="45" t="s">
         <v>248</v>
@@ -25013,7 +25025,7 @@
         <v>248</v>
       </c>
       <c r="AG43" s="45">
-        <v>38.808</v>
+        <v>3.8807999999999998</v>
       </c>
       <c r="AH43" s="45" t="s">
         <v>248</v>
@@ -25111,13 +25123,13 @@
         <v>248</v>
       </c>
       <c r="W44" s="45">
-        <v>28.763999999999999</v>
+        <v>2.8763999999999998</v>
       </c>
       <c r="X44" s="45" t="s">
         <v>248</v>
       </c>
       <c r="Y44" s="45">
-        <v>28.606999999999999</v>
+        <v>2.8607</v>
       </c>
       <c r="Z44" s="45" t="s">
         <v>248</v>
@@ -25168,7 +25180,7 @@
         <v>248</v>
       </c>
       <c r="AP44" s="32">
-        <v>22.094999999999999</v>
+        <v>2.2094999999999998</v>
       </c>
     </row>
     <row r="45" spans="1:42" ht="15.6" x14ac:dyDescent="0.3">
@@ -25242,13 +25254,13 @@
         <v>248</v>
       </c>
       <c r="X45" s="45">
-        <v>28.606999999999999</v>
+        <v>2.8607</v>
       </c>
       <c r="Y45" s="45" t="s">
         <v>248</v>
       </c>
       <c r="Z45" s="45">
-        <v>12.731</v>
+        <v>1.2730999999999999</v>
       </c>
       <c r="AA45" s="45" t="s">
         <v>248</v>
@@ -25373,13 +25385,13 @@
         <v>248</v>
       </c>
       <c r="Y46" s="45">
-        <v>12.731</v>
+        <v>1.2730999999999999</v>
       </c>
       <c r="Z46" s="45" t="s">
         <v>248</v>
       </c>
       <c r="AA46" s="45">
-        <v>15.840999999999999</v>
+        <v>1.5841000000000001</v>
       </c>
       <c r="AB46" s="45" t="s">
         <v>248</v>
@@ -25504,16 +25516,16 @@
         <v>248</v>
       </c>
       <c r="Z47" s="45">
-        <v>15.840999999999999</v>
+        <v>1.5841000000000001</v>
       </c>
       <c r="AA47" s="45" t="s">
         <v>248</v>
       </c>
       <c r="AB47" s="45">
-        <v>16.506</v>
+        <v>1.6506000000000001</v>
       </c>
       <c r="AC47" s="45">
-        <v>17.848000000000003</v>
+        <v>1.7847999999999999</v>
       </c>
       <c r="AD47" s="32" t="s">
         <v>248</v>
@@ -25635,7 +25647,7 @@
         <v>248</v>
       </c>
       <c r="AA48" s="45">
-        <v>16.506</v>
+        <v>1.6506000000000001</v>
       </c>
       <c r="AB48" s="45" t="s">
         <v>248</v>
@@ -25763,7 +25775,7 @@
         <v>248</v>
       </c>
       <c r="AA49" s="45">
-        <v>17.848000000000003</v>
+        <v>1.7847999999999999</v>
       </c>
       <c r="AB49" s="45" t="s">
         <v>248</v>
@@ -25787,7 +25799,7 @@
         <v>248</v>
       </c>
       <c r="AI49" s="32">
-        <v>22.458000000000002</v>
+        <v>2.2458</v>
       </c>
       <c r="AJ49" s="45" t="s">
         <v>248</v>
@@ -25855,7 +25867,7 @@
         <v>248</v>
       </c>
       <c r="O50" s="11">
-        <v>13.959</v>
+        <v>1.3958999999999999</v>
       </c>
       <c r="P50" s="11">
         <v>7.1440000000000001</v>
@@ -25977,7 +25989,7 @@
         <v>248</v>
       </c>
       <c r="M51" s="11">
-        <v>10.85</v>
+        <v>1.085</v>
       </c>
       <c r="N51" s="11" t="s">
         <v>248</v>
@@ -26183,7 +26195,7 @@
         <v>248</v>
       </c>
       <c r="AM52" s="45">
-        <v>26</v>
+        <v>2.6</v>
       </c>
       <c r="AN52" s="45" t="s">
         <v>248</v>
@@ -26311,7 +26323,7 @@
         <v>248</v>
       </c>
       <c r="AM53" s="45">
-        <v>27</v>
+        <v>2.7</v>
       </c>
       <c r="AN53" s="45" t="s">
         <v>248</v>
@@ -26442,7 +26454,7 @@
         <v>248</v>
       </c>
       <c r="AN54" s="45">
-        <v>26</v>
+        <v>2.6</v>
       </c>
       <c r="AO54" s="45" t="s">
         <v>248</v>
@@ -26570,7 +26582,7 @@
         <v>248</v>
       </c>
       <c r="AN55" s="45">
-        <v>27</v>
+        <v>2.7</v>
       </c>
       <c r="AO55" s="45" t="s">
         <v>248</v>
@@ -26701,7 +26713,7 @@
         <v>248</v>
       </c>
       <c r="AO56" s="45">
-        <v>30</v>
+        <v>3</v>
       </c>
       <c r="AP56" s="32" t="s">
         <v>248</v>
@@ -26829,7 +26841,7 @@
         <v>248</v>
       </c>
       <c r="AO57" s="45">
-        <v>28</v>
+        <v>2.8</v>
       </c>
       <c r="AP57" s="32" t="s">
         <v>248</v>
@@ -26960,7 +26972,7 @@
         <v>248</v>
       </c>
       <c r="AP58" s="32">
-        <v>22</v>
+        <v>2.2000000000000002</v>
       </c>
     </row>
     <row r="59" spans="1:42" ht="16.2" thickBot="1" x14ac:dyDescent="0.35">
@@ -27088,7 +27100,7 @@
         <v>248</v>
       </c>
       <c r="AP59" s="12">
-        <v>21</v>
+        <v>2.1</v>
       </c>
     </row>
     <row r="60" spans="1:42" ht="15.6" x14ac:dyDescent="0.3">
@@ -27117,7 +27129,7 @@
         <v>248</v>
       </c>
       <c r="I60" s="45">
-        <v>17.599</v>
+        <v>1.7599</v>
       </c>
       <c r="J60" s="45" t="s">
         <v>248</v>
@@ -27207,10 +27219,10 @@
         <v>248</v>
       </c>
       <c r="AM60" s="45">
-        <v>35.07985</v>
+        <v>3.5079850000000001</v>
       </c>
       <c r="AN60" s="45">
-        <v>30.886050000000001</v>
+        <v>3.0886049999999998</v>
       </c>
       <c r="AO60" s="45" t="s">
         <v>248</v>
@@ -27279,7 +27291,7 @@
         <v>248</v>
       </c>
       <c r="U61" s="11">
-        <v>22.666999999999998</v>
+        <v>2.2667000000000002</v>
       </c>
       <c r="V61" s="11" t="s">
         <v>248</v>
@@ -27339,10 +27351,10 @@
         <v>248</v>
       </c>
       <c r="AO61" s="11">
-        <v>46.94885</v>
+        <v>4.6948850000000002</v>
       </c>
       <c r="AP61" s="12">
-        <v>46.479550000000003</v>
+        <v>4.6479549999999996</v>
       </c>
     </row>
   </sheetData>

</xml_diff>